<commit_message>
started including calculated cells into the xslx file - MOVPE CNR
</commit_message>
<xml_diff>
--- a/movpe_CNR/Parma_datafile_nomad.xlsx
+++ b/movpe_CNR/Parma_datafile_nomad.xlsx
@@ -14,10 +14,11 @@
     <sheet name="SetUp" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Pregrowth" sheetId="5" state="visible" r:id="rId6"/>
     <sheet name="Growthrun" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Sample-cut" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="HRXRD" sheetId="8" state="visible" r:id="rId9"/>
-    <sheet name="AFMReflectanceSEM" sheetId="9" state="visible" r:id="rId10"/>
-    <sheet name="Contacts" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Growthrun_mod" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="Sample-cut" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="HRXRD" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="AFMReflectanceSEM" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="Contacts" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="748" uniqueCount="254">
   <si>
     <t xml:space="preserve"># COMMENTS:</t>
   </si>
@@ -1373,7 +1374,7 @@
   </sheetPr>
   <dimension ref="A1:R1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -1838,11 +1839,545 @@
   </sheetPr>
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="17.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="25.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="17.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="27" width="25.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="27" width="25.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="59" t="s">
+        <v>200</v>
+      </c>
+      <c r="B1" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+    </row>
+    <row r="2" s="3" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="61" t="s">
+        <v>227</v>
+      </c>
+      <c r="B2" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="61" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="60" t="s">
+        <v>1</v>
+      </c>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
+      <c r="K2" s="11"/>
+      <c r="L2" s="4"/>
+      <c r="M2" s="4"/>
+      <c r="P2" s="4"/>
+      <c r="Q2" s="4"/>
+    </row>
+    <row r="3" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
+      <c r="G3" s="20"/>
+      <c r="H3" s="20"/>
+      <c r="I3" s="20"/>
+      <c r="J3" s="20"/>
+      <c r="K3" s="20"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="6"/>
+      <c r="Q3" s="6"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
+      <c r="AB3" s="7"/>
+    </row>
+    <row r="4" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="9"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="9"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="9"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="9"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="9"/>
+      <c r="AB4" s="9"/>
+    </row>
+    <row r="5" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="43" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="43" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="44"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="10"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="11"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="12"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="12"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="12"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="12"/>
+      <c r="AA5" s="12"/>
+      <c r="AB5" s="12"/>
+    </row>
+    <row r="6" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="9"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="9"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="9"/>
+    </row>
+    <row r="7" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44" t="s">
+        <v>228</v>
+      </c>
+      <c r="G7" s="44"/>
+      <c r="H7" s="44" t="s">
+        <v>228</v>
+      </c>
+      <c r="I7" s="44"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15"/>
+      <c r="V7" s="15"/>
+      <c r="W7" s="15"/>
+      <c r="X7" s="15"/>
+      <c r="Y7" s="15"/>
+      <c r="Z7" s="15"/>
+      <c r="AA7" s="15"/>
+      <c r="AB7" s="15"/>
+    </row>
+    <row r="8" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="P8" s="16"/>
+      <c r="Q8" s="16"/>
+      <c r="R8" s="17"/>
+      <c r="S8" s="17"/>
+      <c r="T8" s="17"/>
+      <c r="U8" s="17"/>
+      <c r="V8" s="17"/>
+      <c r="W8" s="17"/>
+      <c r="X8" s="17"/>
+      <c r="Y8" s="17"/>
+      <c r="Z8" s="17"/>
+      <c r="AA8" s="17"/>
+      <c r="AB8" s="17"/>
+    </row>
+    <row r="9" s="17" customFormat="true" ht="15.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="62" t="s">
+        <v>229</v>
+      </c>
+      <c r="B9" s="62" t="s">
+        <v>216</v>
+      </c>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="62" t="s">
+        <v>230</v>
+      </c>
+      <c r="F9" s="62" t="s">
+        <v>231</v>
+      </c>
+      <c r="G9" s="62" t="s">
+        <v>232</v>
+      </c>
+      <c r="H9" s="62" t="s">
+        <v>233</v>
+      </c>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="15"/>
+      <c r="O9" s="15"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
+      <c r="U9" s="15"/>
+      <c r="V9" s="15"/>
+      <c r="W9" s="15"/>
+      <c r="X9" s="15"/>
+      <c r="Y9" s="15"/>
+      <c r="Z9" s="15"/>
+      <c r="AA9" s="15"/>
+      <c r="AB9" s="15"/>
+    </row>
+    <row r="10" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" s="20"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
+      <c r="G10" s="20"/>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20"/>
+      <c r="K10" s="20"/>
+      <c r="L10" s="20"/>
+      <c r="M10" s="20"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="20"/>
+      <c r="Q10" s="20"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="21"/>
+      <c r="U10" s="21"/>
+      <c r="V10" s="21"/>
+      <c r="W10" s="21"/>
+      <c r="X10" s="21"/>
+      <c r="Y10" s="21"/>
+      <c r="Z10" s="21"/>
+      <c r="AA10" s="21"/>
+      <c r="AB10" s="21"/>
+    </row>
+    <row r="11" s="21" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="63" t="s">
+        <v>221</v>
+      </c>
+      <c r="B11" s="63" t="s">
+        <v>234</v>
+      </c>
+      <c r="C11" s="63" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="63" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="63" t="s">
+        <v>235</v>
+      </c>
+      <c r="F11" s="63" t="s">
+        <v>236</v>
+      </c>
+      <c r="G11" s="63" t="s">
+        <v>237</v>
+      </c>
+      <c r="H11" s="63" t="s">
+        <v>238</v>
+      </c>
+      <c r="I11" s="61"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="61"/>
+      <c r="L11" s="0"/>
+      <c r="M11" s="0"/>
+      <c r="N11" s="0"/>
+      <c r="O11" s="0"/>
+      <c r="P11" s="0"/>
+      <c r="Q11" s="0"/>
+      <c r="R11" s="0"/>
+      <c r="S11" s="0"/>
+      <c r="T11" s="0"/>
+      <c r="U11" s="0"/>
+      <c r="V11" s="0"/>
+      <c r="W11" s="0"/>
+      <c r="X11" s="0"/>
+      <c r="Y11" s="0"/>
+      <c r="Z11" s="0"/>
+      <c r="AA11" s="0"/>
+      <c r="AB11" s="0"/>
+    </row>
+    <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="26" t="s">
+        <v>239</v>
+      </c>
+      <c r="B12" s="64"/>
+      <c r="C12" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="D12" s="65" t="s">
+        <v>241</v>
+      </c>
+      <c r="E12" s="66"/>
+      <c r="F12" s="26" t="n">
+        <v>3</v>
+      </c>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="61"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="61"/>
+    </row>
+    <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="26" t="s">
+        <v>242</v>
+      </c>
+      <c r="B13" s="64"/>
+      <c r="C13" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="D13" s="65" t="s">
+        <v>243</v>
+      </c>
+      <c r="E13" s="66"/>
+      <c r="F13" s="26" t="n">
+        <v>3</v>
+      </c>
+      <c r="G13" s="66"/>
+      <c r="H13" s="66"/>
+      <c r="I13" s="61"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="61"/>
+    </row>
+    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="26" t="s">
+        <v>244</v>
+      </c>
+      <c r="B14" s="64"/>
+      <c r="C14" s="65" t="s">
+        <v>240</v>
+      </c>
+      <c r="D14" s="65" t="s">
+        <v>245</v>
+      </c>
+      <c r="E14" s="66"/>
+      <c r="F14" s="26" t="n">
+        <v>3</v>
+      </c>
+      <c r="G14" s="66"/>
+      <c r="H14" s="66"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D15" s="27"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="27"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
+      <c r="F16" s="27"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="60"/>
+      <c r="K16" s="60"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="60"/>
+      <c r="K17" s="60"/>
+    </row>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AB1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D62" activeCellId="0" sqref="D62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="12.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="24.15"/>
@@ -2188,13 +2723,13 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="32.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="12.17"/>
@@ -2677,7 +3212,7 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
@@ -3048,11 +3583,11 @@
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K28" activeCellId="0" sqref="K28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="36" width="16.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="27" width="15.53"/>
@@ -3901,11 +4436,11 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8671875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="15.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="20.22"/>
@@ -4299,11 +4834,11 @@
   </sheetPr>
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S22" activeCellId="0" sqref="S22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="12.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="7.49"/>
@@ -4838,8 +5373,9 @@
       <c r="J10" s="54" t="n">
         <v>1</v>
       </c>
-      <c r="K10" s="54" t="n">
-        <v>4.86E-005</v>
+      <c r="K10" s="54" t="e">
+        <f aca="false">(F7*H7)/((Q7+R7+L7+H7+S7)*(I7/1000)*(F7+G7))*10^(8.07-1703/(J7+273.15))/760*1.01325</f>
+        <v>#VALUE!</v>
       </c>
       <c r="L10" s="53" t="n">
         <v>50</v>
@@ -4866,10 +5402,12 @@
         <v>3</v>
       </c>
       <c r="T10" s="53" t="n">
-        <v>4</v>
+        <f aca="false"> SetUp!F12*E10</f>
+        <v>6</v>
       </c>
       <c r="U10" s="53" t="n">
-        <v>2</v>
+        <f aca="false">T10/(Q10+R10+S10+L10+H10)</f>
+        <v>0.00290838584585555</v>
       </c>
       <c r="V10" s="53" t="n">
         <v>200</v>
@@ -4952,7 +5490,8 @@
         <v>4</v>
       </c>
       <c r="U11" s="53" t="n">
-        <v>2</v>
+        <f aca="false">T11/(Q11+R11+S11+L11+H11)</f>
+        <v>0.00193892389723703</v>
       </c>
       <c r="V11" s="53" t="n">
         <v>200</v>
@@ -5035,7 +5574,8 @@
         <v>4</v>
       </c>
       <c r="U12" s="53" t="n">
-        <v>2</v>
+        <f aca="false">T12/(Q12+R12+S12+L12+H12)</f>
+        <v>0.00193892389723703</v>
       </c>
       <c r="V12" s="53" t="n">
         <v>200</v>
@@ -5118,7 +5658,8 @@
         <v>4</v>
       </c>
       <c r="U13" s="53" t="n">
-        <v>2</v>
+        <f aca="false">T13/(Q13+R13+S13+L13+H13)</f>
+        <v>0.00193892389723703</v>
       </c>
       <c r="V13" s="53" t="n">
         <v>200</v>
@@ -5496,13 +6037,969 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
+  <dimension ref="A1:AD17"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="T19" activeCellId="0" sqref="T19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" s="7" customFormat="true" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+    </row>
+    <row r="2" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+    </row>
+    <row r="3" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="H3" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="44" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="K3" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="N3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="P3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="R3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="S3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="T3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="U3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="V3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="W3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="X3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="Y3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="Z3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
+    </row>
+    <row r="4" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+      <c r="L4" s="8"/>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="8"/>
+      <c r="R4" s="8"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="8"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
+      <c r="X4" s="8"/>
+      <c r="Y4" s="8"/>
+      <c r="Z4" s="8"/>
+      <c r="AA4" s="8"/>
+      <c r="AB4" s="8"/>
+    </row>
+    <row r="5" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="43" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="44" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="E5" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" s="43" t="s">
+        <v>132</v>
+      </c>
+      <c r="G5" s="43" t="s">
+        <v>131</v>
+      </c>
+      <c r="H5" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="I5" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="K5" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="L5" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="M5" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="N5" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="O5" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="P5" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="Q5" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="R5" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="T5" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="U5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="V5" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="W5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="X5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Y5" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Z5" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="10"/>
+    </row>
+    <row r="6" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="16"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
+      <c r="L6" s="16"/>
+      <c r="M6" s="16"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
+      <c r="R6" s="16"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="16"/>
+      <c r="U6" s="16"/>
+      <c r="V6" s="16"/>
+      <c r="W6" s="16"/>
+      <c r="X6" s="16"/>
+      <c r="Y6" s="16"/>
+      <c r="Z6" s="16"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="16"/>
+    </row>
+    <row r="7" s="18" customFormat="true" ht="34.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10"/>
+      <c r="K7" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="L7" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="Q7" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="R7" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>163</v>
+      </c>
+      <c r="T7" s="10" t="s">
+        <v>164</v>
+      </c>
+      <c r="U7" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="V7" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="W7" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="X7" s="10" t="s">
+        <v>168</v>
+      </c>
+      <c r="Y7" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="Z7" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
+    </row>
+    <row r="8" s="21" customFormat="true" ht="23.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="20"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+      <c r="L8" s="20"/>
+      <c r="M8" s="20"/>
+      <c r="N8" s="20"/>
+      <c r="O8" s="20"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="20"/>
+      <c r="R8" s="20"/>
+      <c r="S8" s="20"/>
+      <c r="T8" s="20"/>
+      <c r="U8" s="20"/>
+      <c r="V8" s="20"/>
+      <c r="W8" s="20"/>
+      <c r="X8" s="20"/>
+      <c r="Y8" s="20"/>
+      <c r="Z8" s="20"/>
+      <c r="AA8" s="20"/>
+      <c r="AB8" s="20"/>
+    </row>
+    <row r="9" customFormat="false" ht="34.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B9" s="52" t="s">
+        <v>171</v>
+      </c>
+      <c r="C9" s="52" t="s">
+        <v>172</v>
+      </c>
+      <c r="D9" s="52" t="s">
+        <v>173</v>
+      </c>
+      <c r="E9" s="52" t="s">
+        <v>120</v>
+      </c>
+      <c r="F9" s="52" t="s">
+        <v>174</v>
+      </c>
+      <c r="G9" s="52" t="s">
+        <v>175</v>
+      </c>
+      <c r="H9" s="52" t="s">
+        <v>176</v>
+      </c>
+      <c r="I9" s="52" t="s">
+        <v>177</v>
+      </c>
+      <c r="J9" s="52" t="s">
+        <v>178</v>
+      </c>
+      <c r="K9" s="52" t="s">
+        <v>179</v>
+      </c>
+      <c r="L9" s="52" t="s">
+        <v>180</v>
+      </c>
+      <c r="M9" s="52" t="s">
+        <v>181</v>
+      </c>
+      <c r="N9" s="52" t="s">
+        <v>182</v>
+      </c>
+      <c r="O9" s="52" t="s">
+        <v>183</v>
+      </c>
+      <c r="P9" s="52" t="s">
+        <v>184</v>
+      </c>
+      <c r="Q9" s="52" t="s">
+        <v>185</v>
+      </c>
+      <c r="R9" s="52" t="s">
+        <v>186</v>
+      </c>
+      <c r="S9" s="52" t="s">
+        <v>187</v>
+      </c>
+      <c r="T9" s="52" t="s">
+        <v>188</v>
+      </c>
+      <c r="U9" s="52" t="s">
+        <v>165</v>
+      </c>
+      <c r="V9" s="52" t="s">
+        <v>189</v>
+      </c>
+      <c r="W9" s="52" t="s">
+        <v>190</v>
+      </c>
+      <c r="X9" s="52" t="s">
+        <v>191</v>
+      </c>
+      <c r="Y9" s="52" t="s">
+        <v>192</v>
+      </c>
+      <c r="Z9" s="52" t="s">
+        <v>193</v>
+      </c>
+      <c r="AA9" s="53"/>
+      <c r="AB9" s="53"/>
+      <c r="AD9" s="27"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="53" t="s">
+        <v>194</v>
+      </c>
+      <c r="B10" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="53" t="n">
+        <v>100</v>
+      </c>
+      <c r="D10" s="53" t="n">
+        <v>610</v>
+      </c>
+      <c r="E10" s="53" t="n">
+        <v>60</v>
+      </c>
+      <c r="F10" s="53" t="n">
+        <f aca="false">SUM(D10:E10)</f>
+        <v>670</v>
+      </c>
+      <c r="G10" s="53" t="n">
+        <v>35</v>
+      </c>
+      <c r="H10" s="53" t="n">
+        <v>10</v>
+      </c>
+      <c r="I10" s="53" t="n">
+        <v>1200</v>
+      </c>
+      <c r="J10" s="54" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="54" t="n">
+        <v>4.86E-005</v>
+      </c>
+      <c r="L10" s="53" t="n">
+        <v>50</v>
+      </c>
+      <c r="M10" s="53" t="n">
+        <v>3</v>
+      </c>
+      <c r="N10" s="53" t="n">
+        <v>3</v>
+      </c>
+      <c r="O10" s="54" t="n">
+        <v>30</v>
+      </c>
+      <c r="P10" s="54" t="n">
+        <v>0.0169</v>
+      </c>
+      <c r="Q10" s="53" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R10" s="53" t="n">
+        <v>1000</v>
+      </c>
+      <c r="S10" s="53" t="n">
+        <v>3</v>
+      </c>
+      <c r="T10" s="53" t="n">
+        <f aca="false"> SetUp!F12*E10</f>
+        <v>6</v>
+      </c>
+      <c r="U10" s="53" t="n">
+        <v>2</v>
+      </c>
+      <c r="V10" s="53" t="n">
+        <v>200</v>
+      </c>
+      <c r="W10" s="53" t="s">
+        <v>195</v>
+      </c>
+      <c r="X10" s="53" t="s">
+        <v>195</v>
+      </c>
+      <c r="Y10" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z10" s="53" t="n">
+        <v>234</v>
+      </c>
+      <c r="AA10" s="53"/>
+      <c r="AB10" s="53"/>
+      <c r="AD10" s="27"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="53" t="s">
+        <v>197</v>
+      </c>
+      <c r="B11" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="53" t="n">
+        <v>100</v>
+      </c>
+      <c r="D11" s="53" t="n">
+        <v>610</v>
+      </c>
+      <c r="E11" s="53" t="n">
+        <v>60</v>
+      </c>
+      <c r="F11" s="53" t="n">
+        <f aca="false">SUM(D11:E11)</f>
+        <v>670</v>
+      </c>
+      <c r="G11" s="53" t="n">
+        <v>35</v>
+      </c>
+      <c r="H11" s="53" t="n">
+        <v>10</v>
+      </c>
+      <c r="I11" s="53" t="n">
+        <v>1200</v>
+      </c>
+      <c r="J11" s="54" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="54" t="n">
+        <v>4.86E-005</v>
+      </c>
+      <c r="L11" s="53" t="n">
+        <v>50</v>
+      </c>
+      <c r="M11" s="53" t="n">
+        <v>3</v>
+      </c>
+      <c r="N11" s="53" t="n">
+        <v>3</v>
+      </c>
+      <c r="O11" s="54" t="n">
+        <v>30</v>
+      </c>
+      <c r="P11" s="54" t="n">
+        <v>0.0169</v>
+      </c>
+      <c r="Q11" s="53" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R11" s="53" t="n">
+        <v>1000</v>
+      </c>
+      <c r="S11" s="53" t="n">
+        <v>3</v>
+      </c>
+      <c r="T11" s="53" t="n">
+        <v>4</v>
+      </c>
+      <c r="U11" s="53" t="n">
+        <v>2</v>
+      </c>
+      <c r="V11" s="53" t="n">
+        <v>200</v>
+      </c>
+      <c r="W11" s="53" t="s">
+        <v>195</v>
+      </c>
+      <c r="X11" s="53" t="s">
+        <v>195</v>
+      </c>
+      <c r="Y11" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z11" s="53" t="n">
+        <v>234</v>
+      </c>
+      <c r="AA11" s="53"/>
+      <c r="AB11" s="53"/>
+      <c r="AD11" s="27"/>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="53" t="s">
+        <v>198</v>
+      </c>
+      <c r="B12" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="53" t="n">
+        <v>100</v>
+      </c>
+      <c r="D12" s="53" t="n">
+        <v>610</v>
+      </c>
+      <c r="E12" s="53" t="n">
+        <v>60</v>
+      </c>
+      <c r="F12" s="53" t="n">
+        <f aca="false">SUM(D12:E12)</f>
+        <v>670</v>
+      </c>
+      <c r="G12" s="53" t="n">
+        <v>35</v>
+      </c>
+      <c r="H12" s="53" t="n">
+        <v>10</v>
+      </c>
+      <c r="I12" s="53" t="n">
+        <v>1200</v>
+      </c>
+      <c r="J12" s="54" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="54" t="n">
+        <v>4.86E-005</v>
+      </c>
+      <c r="L12" s="53" t="n">
+        <v>50</v>
+      </c>
+      <c r="M12" s="53" t="n">
+        <v>3</v>
+      </c>
+      <c r="N12" s="53" t="n">
+        <v>3</v>
+      </c>
+      <c r="O12" s="54" t="n">
+        <v>30</v>
+      </c>
+      <c r="P12" s="54" t="n">
+        <v>0.0169</v>
+      </c>
+      <c r="Q12" s="53" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R12" s="53" t="n">
+        <v>1000</v>
+      </c>
+      <c r="S12" s="53" t="n">
+        <v>3</v>
+      </c>
+      <c r="T12" s="53" t="n">
+        <v>4</v>
+      </c>
+      <c r="U12" s="53" t="n">
+        <v>2</v>
+      </c>
+      <c r="V12" s="53" t="n">
+        <v>200</v>
+      </c>
+      <c r="W12" s="53" t="s">
+        <v>195</v>
+      </c>
+      <c r="X12" s="53" t="s">
+        <v>195</v>
+      </c>
+      <c r="Y12" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z12" s="53" t="n">
+        <v>234</v>
+      </c>
+      <c r="AA12" s="53"/>
+      <c r="AB12" s="53"/>
+      <c r="AD12" s="27"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="53" t="s">
+        <v>199</v>
+      </c>
+      <c r="B13" s="53" t="n">
+        <v>1</v>
+      </c>
+      <c r="C13" s="53" t="n">
+        <v>100</v>
+      </c>
+      <c r="D13" s="53" t="n">
+        <v>610</v>
+      </c>
+      <c r="E13" s="53" t="n">
+        <v>60</v>
+      </c>
+      <c r="F13" s="53" t="n">
+        <f aca="false">SUM(D13:E13)</f>
+        <v>670</v>
+      </c>
+      <c r="G13" s="53" t="n">
+        <v>35</v>
+      </c>
+      <c r="H13" s="53" t="n">
+        <v>10</v>
+      </c>
+      <c r="I13" s="53" t="n">
+        <v>1200</v>
+      </c>
+      <c r="J13" s="54" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" s="54" t="n">
+        <v>4.86E-005</v>
+      </c>
+      <c r="L13" s="53" t="n">
+        <v>50</v>
+      </c>
+      <c r="M13" s="53" t="n">
+        <v>3</v>
+      </c>
+      <c r="N13" s="53" t="n">
+        <v>3</v>
+      </c>
+      <c r="O13" s="54" t="n">
+        <v>30</v>
+      </c>
+      <c r="P13" s="54" t="n">
+        <v>0.0169</v>
+      </c>
+      <c r="Q13" s="53" t="n">
+        <v>1000</v>
+      </c>
+      <c r="R13" s="53" t="n">
+        <v>1000</v>
+      </c>
+      <c r="S13" s="53" t="n">
+        <v>3</v>
+      </c>
+      <c r="T13" s="53" t="n">
+        <v>4</v>
+      </c>
+      <c r="U13" s="53" t="n">
+        <v>2</v>
+      </c>
+      <c r="V13" s="53" t="n">
+        <v>200</v>
+      </c>
+      <c r="W13" s="53" t="s">
+        <v>195</v>
+      </c>
+      <c r="X13" s="53" t="s">
+        <v>195</v>
+      </c>
+      <c r="Y13" s="53" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z13" s="53" t="n">
+        <v>234</v>
+      </c>
+      <c r="AA13" s="53"/>
+      <c r="AB13" s="53"/>
+      <c r="AD13" s="27"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="53"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="53"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="53"/>
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="53"/>
+      <c r="L14" s="53"/>
+      <c r="M14" s="53"/>
+      <c r="N14" s="53"/>
+      <c r="O14" s="53"/>
+      <c r="P14" s="53"/>
+      <c r="Q14" s="53"/>
+      <c r="R14" s="53"/>
+      <c r="S14" s="53"/>
+      <c r="T14" s="53"/>
+      <c r="U14" s="53"/>
+      <c r="V14" s="53"/>
+      <c r="W14" s="53"/>
+      <c r="X14" s="53"/>
+      <c r="Y14" s="53"/>
+      <c r="Z14" s="53"/>
+      <c r="AA14" s="53"/>
+      <c r="AB14" s="53"/>
+      <c r="AD14" s="27"/>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="53"/>
+      <c r="B15" s="53"/>
+      <c r="C15" s="53"/>
+      <c r="D15" s="53"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="53"/>
+      <c r="I15" s="53"/>
+      <c r="J15" s="53"/>
+      <c r="K15" s="53"/>
+      <c r="L15" s="53"/>
+      <c r="M15" s="53"/>
+      <c r="N15" s="53"/>
+      <c r="O15" s="53"/>
+      <c r="P15" s="53"/>
+      <c r="Q15" s="53"/>
+      <c r="R15" s="53"/>
+      <c r="S15" s="53"/>
+      <c r="T15" s="53"/>
+      <c r="U15" s="53"/>
+      <c r="V15" s="53"/>
+      <c r="W15" s="53"/>
+      <c r="X15" s="53"/>
+      <c r="Y15" s="53"/>
+      <c r="Z15" s="53"/>
+      <c r="AA15" s="53"/>
+      <c r="AB15" s="53"/>
+      <c r="AD15" s="27"/>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="53"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="53"/>
+      <c r="E16" s="53"/>
+      <c r="F16" s="53"/>
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="53"/>
+      <c r="K16" s="53"/>
+      <c r="L16" s="53"/>
+      <c r="M16" s="53"/>
+      <c r="N16" s="53"/>
+      <c r="O16" s="53"/>
+      <c r="P16" s="53"/>
+      <c r="Q16" s="53"/>
+      <c r="R16" s="53"/>
+      <c r="S16" s="53"/>
+      <c r="T16" s="53"/>
+      <c r="U16" s="53"/>
+      <c r="V16" s="53"/>
+      <c r="W16" s="53"/>
+      <c r="X16" s="53"/>
+      <c r="Y16" s="53"/>
+      <c r="Z16" s="53"/>
+      <c r="AA16" s="53"/>
+      <c r="AB16" s="53"/>
+      <c r="AD16" s="27"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="53"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="53"/>
+      <c r="E17" s="53"/>
+      <c r="F17" s="53"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
+      <c r="K17" s="53"/>
+      <c r="L17" s="53"/>
+      <c r="M17" s="53"/>
+      <c r="N17" s="53"/>
+      <c r="O17" s="53"/>
+      <c r="P17" s="53"/>
+      <c r="Q17" s="53"/>
+      <c r="R17" s="53"/>
+      <c r="S17" s="53"/>
+      <c r="T17" s="53"/>
+      <c r="U17" s="53"/>
+      <c r="V17" s="53"/>
+      <c r="W17" s="53"/>
+      <c r="X17" s="53"/>
+      <c r="Y17" s="53"/>
+      <c r="Z17" s="53"/>
+      <c r="AA17" s="53"/>
+      <c r="AB17" s="53"/>
+      <c r="AD17" s="27"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="17.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="23.77"/>
@@ -5838,18 +7335,18 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="51.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="30.83"/>
@@ -6355,538 +7852,4 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:AB1048576"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="27" width="17.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="27" width="25.21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="27" width="17.52"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="17.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="19.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="27" width="25.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="27" width="25.83"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="59" t="s">
-        <v>200</v>
-      </c>
-      <c r="B1" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-    </row>
-    <row r="2" s="3" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="61" t="s">
-        <v>227</v>
-      </c>
-      <c r="B2" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="4"/>
-    </row>
-    <row r="3" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="20"/>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="7"/>
-      <c r="O3" s="7"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="7"/>
-      <c r="T3" s="7"/>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="7"/>
-      <c r="Z3" s="7"/>
-      <c r="AA3" s="7"/>
-      <c r="AB3" s="7"/>
-    </row>
-    <row r="4" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8"/>
-      <c r="K4" s="8"/>
-      <c r="L4" s="8"/>
-      <c r="M4" s="8"/>
-      <c r="N4" s="9"/>
-      <c r="O4" s="9"/>
-      <c r="P4" s="8"/>
-      <c r="Q4" s="8"/>
-      <c r="R4" s="9"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="9"/>
-      <c r="U4" s="9"/>
-      <c r="V4" s="9"/>
-      <c r="W4" s="9"/>
-      <c r="X4" s="9"/>
-      <c r="Y4" s="9"/>
-      <c r="Z4" s="9"/>
-      <c r="AA4" s="9"/>
-      <c r="AB4" s="9"/>
-    </row>
-    <row r="5" s="9" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="44" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="44" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="F5" s="43" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="43" t="s">
-        <v>9</v>
-      </c>
-      <c r="H5" s="44" t="s">
-        <v>10</v>
-      </c>
-      <c r="I5" s="44"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="11"/>
-      <c r="M5" s="11"/>
-      <c r="N5" s="12"/>
-      <c r="O5" s="12"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="12"/>
-      <c r="T5" s="12"/>
-      <c r="U5" s="12"/>
-      <c r="V5" s="12"/>
-      <c r="W5" s="12"/>
-      <c r="X5" s="12"/>
-      <c r="Y5" s="12"/>
-      <c r="Z5" s="12"/>
-      <c r="AA5" s="12"/>
-      <c r="AB5" s="12"/>
-    </row>
-    <row r="6" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-      <c r="L6" s="8"/>
-      <c r="M6" s="8"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="8"/>
-      <c r="Q6" s="8"/>
-      <c r="R6" s="9"/>
-      <c r="S6" s="9"/>
-      <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Y6" s="9"/>
-      <c r="Z6" s="9"/>
-      <c r="AA6" s="9"/>
-      <c r="AB6" s="9"/>
-    </row>
-    <row r="7" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="44" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44" t="s">
-        <v>228</v>
-      </c>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44" t="s">
-        <v>228</v>
-      </c>
-      <c r="I7" s="44"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="15"/>
-      <c r="S7" s="15"/>
-      <c r="T7" s="15"/>
-      <c r="U7" s="15"/>
-      <c r="V7" s="15"/>
-      <c r="W7" s="15"/>
-      <c r="X7" s="15"/>
-      <c r="Y7" s="15"/>
-      <c r="Z7" s="15"/>
-      <c r="AA7" s="15"/>
-      <c r="AB7" s="15"/>
-    </row>
-    <row r="8" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="8"/>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8"/>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8"/>
-      <c r="K8" s="8"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
-      <c r="P8" s="16"/>
-      <c r="Q8" s="16"/>
-      <c r="R8" s="17"/>
-      <c r="S8" s="17"/>
-      <c r="T8" s="17"/>
-      <c r="U8" s="17"/>
-      <c r="V8" s="17"/>
-      <c r="W8" s="17"/>
-      <c r="X8" s="17"/>
-      <c r="Y8" s="17"/>
-      <c r="Z8" s="17"/>
-      <c r="AA8" s="17"/>
-      <c r="AB8" s="17"/>
-    </row>
-    <row r="9" s="17" customFormat="true" ht="15.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="62" t="s">
-        <v>229</v>
-      </c>
-      <c r="B9" s="62" t="s">
-        <v>216</v>
-      </c>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62" t="s">
-        <v>230</v>
-      </c>
-      <c r="F9" s="62" t="s">
-        <v>231</v>
-      </c>
-      <c r="G9" s="62" t="s">
-        <v>232</v>
-      </c>
-      <c r="H9" s="62" t="s">
-        <v>233</v>
-      </c>
-      <c r="I9" s="10"/>
-      <c r="J9" s="10"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="10"/>
-      <c r="Q9" s="10"/>
-      <c r="R9" s="15"/>
-      <c r="S9" s="15"/>
-      <c r="T9" s="15"/>
-      <c r="U9" s="15"/>
-      <c r="V9" s="15"/>
-      <c r="W9" s="15"/>
-      <c r="X9" s="15"/>
-      <c r="Y9" s="15"/>
-      <c r="Z9" s="15"/>
-      <c r="AA9" s="15"/>
-      <c r="AB9" s="15"/>
-    </row>
-    <row r="10" s="18" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20"/>
-      <c r="K10" s="20"/>
-      <c r="L10" s="20"/>
-      <c r="M10" s="20"/>
-      <c r="N10" s="21"/>
-      <c r="O10" s="21"/>
-      <c r="P10" s="20"/>
-      <c r="Q10" s="20"/>
-      <c r="R10" s="21"/>
-      <c r="S10" s="21"/>
-      <c r="T10" s="21"/>
-      <c r="U10" s="21"/>
-      <c r="V10" s="21"/>
-      <c r="W10" s="21"/>
-      <c r="X10" s="21"/>
-      <c r="Y10" s="21"/>
-      <c r="Z10" s="21"/>
-      <c r="AA10" s="21"/>
-      <c r="AB10" s="21"/>
-    </row>
-    <row r="11" s="21" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="63" t="s">
-        <v>221</v>
-      </c>
-      <c r="B11" s="63" t="s">
-        <v>234</v>
-      </c>
-      <c r="C11" s="63" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" s="63" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="63" t="s">
-        <v>235</v>
-      </c>
-      <c r="F11" s="63" t="s">
-        <v>236</v>
-      </c>
-      <c r="G11" s="63" t="s">
-        <v>237</v>
-      </c>
-      <c r="H11" s="63" t="s">
-        <v>238</v>
-      </c>
-      <c r="I11" s="61"/>
-      <c r="J11" s="61"/>
-      <c r="K11" s="61"/>
-      <c r="L11" s="0"/>
-      <c r="M11" s="0"/>
-      <c r="N11" s="0"/>
-      <c r="O11" s="0"/>
-      <c r="P11" s="0"/>
-      <c r="Q11" s="0"/>
-      <c r="R11" s="0"/>
-      <c r="S11" s="0"/>
-      <c r="T11" s="0"/>
-      <c r="U11" s="0"/>
-      <c r="V11" s="0"/>
-      <c r="W11" s="0"/>
-      <c r="X11" s="0"/>
-      <c r="Y11" s="0"/>
-      <c r="Z11" s="0"/>
-      <c r="AA11" s="0"/>
-      <c r="AB11" s="0"/>
-    </row>
-    <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="26" t="s">
-        <v>239</v>
-      </c>
-      <c r="B12" s="64"/>
-      <c r="C12" s="65" t="s">
-        <v>240</v>
-      </c>
-      <c r="D12" s="65" t="s">
-        <v>241</v>
-      </c>
-      <c r="E12" s="66"/>
-      <c r="F12" s="26" t="n">
-        <v>3</v>
-      </c>
-      <c r="G12" s="66"/>
-      <c r="H12" s="66"/>
-      <c r="I12" s="61"/>
-      <c r="J12" s="61"/>
-      <c r="K12" s="61"/>
-    </row>
-    <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="26" t="s">
-        <v>242</v>
-      </c>
-      <c r="B13" s="64"/>
-      <c r="C13" s="65" t="s">
-        <v>240</v>
-      </c>
-      <c r="D13" s="65" t="s">
-        <v>243</v>
-      </c>
-      <c r="E13" s="66"/>
-      <c r="F13" s="26" t="n">
-        <v>3</v>
-      </c>
-      <c r="G13" s="66"/>
-      <c r="H13" s="66"/>
-      <c r="I13" s="61"/>
-      <c r="J13" s="61"/>
-      <c r="K13" s="61"/>
-    </row>
-    <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="26" t="s">
-        <v>244</v>
-      </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="65" t="s">
-        <v>240</v>
-      </c>
-      <c r="D14" s="65" t="s">
-        <v>245</v>
-      </c>
-      <c r="E14" s="66"/>
-      <c r="F14" s="26" t="n">
-        <v>3</v>
-      </c>
-      <c r="G14" s="66"/>
-      <c r="H14" s="66"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="60"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="60"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
-      <c r="F16" s="27"/>
-      <c r="I16" s="60"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="60"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="I17" s="60"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="60"/>
-    </row>
-    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed bug in tasks MOVPE CNR
</commit_message>
<xml_diff>
--- a/movpe_CNR/Parma_datafile_nomad.xlsx
+++ b/movpe_CNR/Parma_datafile_nomad.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -806,16 +806,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+  <numFmts count="6">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="166" formatCode="@"/>
     <numFmt numFmtId="167" formatCode="0.00E+00"/>
     <numFmt numFmtId="168" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="169" formatCode="BOOLEAN"/>
-    <numFmt numFmtId="170" formatCode="#,##0"/>
+    <numFmt numFmtId="169" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -927,12 +926,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="0"/>
@@ -989,7 +982,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1034,6 +1027,21 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="hair">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="hair">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="hair">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="20">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1060,7 +1068,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="117">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1281,6 +1289,22 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1289,6 +1313,22 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="15" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1297,6 +1337,22 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1321,10 +1377,22 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="15" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="15" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1337,6 +1405,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="4" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1365,6 +1437,18 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1377,22 +1461,14 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1429,7 +1505,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1437,7 +1513,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="170" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="169" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1449,7 +1525,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1534,14 +1610,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AMJ45"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1555,13 +1631,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="17.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="11.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="22.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="11.5"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="31.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="33.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="39.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="18.66"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="16" style="1" width="27.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1909,7 +1985,8 @@
         <v>39</v>
       </c>
       <c r="J12" s="12" t="n">
-        <v>3</v>
+        <f aca="false">Growthrun!S11/Growthrun!K11</f>
+        <v>348.082285817989</v>
       </c>
       <c r="K12" s="12" t="n">
         <v>10</v>
@@ -2058,17 +2135,17 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D62" activeCellId="0" sqref="D62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="12.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="24.15"/>
@@ -2235,7 +2312,7 @@
         <v>251</v>
       </c>
       <c r="G7" s="43"/>
-      <c r="H7" s="90"/>
+      <c r="H7" s="107"/>
       <c r="I7" s="10"/>
       <c r="J7" s="10"/>
       <c r="K7" s="10"/>
@@ -2277,7 +2354,7 @@
       <c r="Q8" s="20"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="95" t="s">
+      <c r="A9" s="112" t="s">
         <v>252</v>
       </c>
       <c r="B9" s="18" t="s">
@@ -2289,92 +2366,92 @@
       <c r="D9" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="95" t="s">
+      <c r="E9" s="112" t="s">
         <v>250</v>
       </c>
-      <c r="F9" s="95" t="s">
+      <c r="F9" s="112" t="s">
         <v>254</v>
       </c>
-      <c r="G9" s="95"/>
-      <c r="H9" s="88"/>
-      <c r="I9" s="88"/>
-      <c r="J9" s="88"/>
+      <c r="G9" s="112"/>
+      <c r="H9" s="105"/>
+      <c r="I9" s="105"/>
+      <c r="J9" s="105"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="96"/>
-      <c r="B10" s="97"/>
-      <c r="C10" s="98" t="s">
+      <c r="A10" s="113"/>
+      <c r="B10" s="114"/>
+      <c r="C10" s="115" t="s">
         <v>255</v>
       </c>
-      <c r="D10" s="98" t="s">
+      <c r="D10" s="115" t="s">
         <v>256</v>
       </c>
-      <c r="E10" s="88"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="88"/>
-      <c r="H10" s="88"/>
-      <c r="I10" s="88"/>
-      <c r="J10" s="88"/>
+      <c r="E10" s="105"/>
+      <c r="F10" s="105"/>
+      <c r="G10" s="105"/>
+      <c r="H10" s="105"/>
+      <c r="I10" s="105"/>
+      <c r="J10" s="105"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="88"/>
-      <c r="B11" s="99"/>
-      <c r="C11" s="99"/>
-      <c r="D11" s="99"/>
-      <c r="E11" s="88"/>
-      <c r="F11" s="88"/>
-      <c r="G11" s="88"/>
-      <c r="H11" s="88"/>
-      <c r="I11" s="88"/>
-      <c r="J11" s="88"/>
+      <c r="A11" s="105"/>
+      <c r="B11" s="116"/>
+      <c r="C11" s="116"/>
+      <c r="D11" s="116"/>
+      <c r="E11" s="105"/>
+      <c r="F11" s="105"/>
+      <c r="G11" s="105"/>
+      <c r="H11" s="105"/>
+      <c r="I11" s="105"/>
+      <c r="J11" s="105"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="88"/>
-      <c r="B12" s="99"/>
-      <c r="C12" s="99"/>
-      <c r="D12" s="99"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="88"/>
-      <c r="I12" s="88"/>
-      <c r="J12" s="88"/>
+      <c r="A12" s="105"/>
+      <c r="B12" s="116"/>
+      <c r="C12" s="116"/>
+      <c r="D12" s="116"/>
+      <c r="E12" s="105"/>
+      <c r="F12" s="105"/>
+      <c r="G12" s="105"/>
+      <c r="H12" s="105"/>
+      <c r="I12" s="105"/>
+      <c r="J12" s="105"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="88"/>
-      <c r="B13" s="99"/>
-      <c r="C13" s="99"/>
-      <c r="D13" s="99"/>
-      <c r="E13" s="88"/>
-      <c r="F13" s="88"/>
-      <c r="G13" s="88"/>
-      <c r="H13" s="88"/>
-      <c r="I13" s="88"/>
-      <c r="J13" s="88"/>
+      <c r="A13" s="105"/>
+      <c r="B13" s="116"/>
+      <c r="C13" s="116"/>
+      <c r="D13" s="116"/>
+      <c r="E13" s="105"/>
+      <c r="F13" s="105"/>
+      <c r="G13" s="105"/>
+      <c r="H13" s="105"/>
+      <c r="I13" s="105"/>
+      <c r="J13" s="105"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="88"/>
-      <c r="B14" s="99"/>
-      <c r="C14" s="99"/>
-      <c r="D14" s="99"/>
-      <c r="E14" s="88"/>
-      <c r="F14" s="88"/>
-      <c r="G14" s="88"/>
-      <c r="H14" s="88"/>
-      <c r="I14" s="88"/>
-      <c r="J14" s="88"/>
+      <c r="A14" s="105"/>
+      <c r="B14" s="116"/>
+      <c r="C14" s="116"/>
+      <c r="D14" s="116"/>
+      <c r="E14" s="105"/>
+      <c r="F14" s="105"/>
+      <c r="G14" s="105"/>
+      <c r="H14" s="105"/>
+      <c r="I14" s="105"/>
+      <c r="J14" s="105"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="88"/>
-      <c r="B15" s="99"/>
-      <c r="C15" s="99"/>
-      <c r="D15" s="99"/>
-      <c r="E15" s="88"/>
-      <c r="F15" s="88"/>
-      <c r="G15" s="88"/>
-      <c r="H15" s="88"/>
-      <c r="I15" s="88"/>
-      <c r="J15" s="88"/>
+      <c r="A15" s="105"/>
+      <c r="B15" s="116"/>
+      <c r="C15" s="116"/>
+      <c r="D15" s="116"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="105"/>
+      <c r="G15" s="105"/>
+      <c r="H15" s="105"/>
+      <c r="I15" s="105"/>
+      <c r="J15" s="105"/>
     </row>
     <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -2408,19 +2485,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.94140625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="32.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="12.17"/>
@@ -2897,13 +2974,13 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C2" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C2" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
     </sheetView>
   </sheetViews>
@@ -3272,17 +3349,17 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AMJ1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H11" activeCellId="0" sqref="H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="35" width="16.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="26" width="15.53"/>
@@ -4125,17 +4202,17 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E36" activeCellId="0" sqref="E36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.88671875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="15.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="20.22"/>
@@ -4523,22 +4600,22 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AK25"/>
+  <dimension ref="A1:AV47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="U1" activeCellId="0" sqref="U1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F20" activeCellId="0" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="51" width="11.53"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="51" width="4.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="52" width="7.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="51" width="11.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="51" width="11.46"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="51" width="7.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="51" width="7.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="51" width="8.25"/>
@@ -4564,13 +4641,13 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="51" width="10"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="51" width="18.34"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="51" width="17.33"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="30" min="30" style="53" width="11.93"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="30" min="30" style="53" width="11.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="51" width="14.16"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="32" style="53" width="11.93"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="38" style="53" width="11.93"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="34" min="32" style="53" width="11.92"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="38" style="53" width="11.92"/>
   </cols>
   <sheetData>
-    <row r="1" s="55" customFormat="true" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="59" customFormat="true" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
@@ -4603,1239 +4680,2198 @@
       <c r="X1" s="54"/>
       <c r="Y1" s="54"/>
       <c r="Z1" s="54"/>
-      <c r="AA1" s="54"/>
-      <c r="AB1" s="54"/>
-      <c r="AC1" s="54"/>
-      <c r="AF1" s="53"/>
-      <c r="AG1" s="53"/>
-      <c r="AH1" s="53"/>
-      <c r="AI1" s="0"/>
-      <c r="AJ1" s="0"/>
-      <c r="AK1" s="0"/>
-    </row>
-    <row r="2" s="57" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="56" t="s">
+      <c r="AA1" s="55"/>
+      <c r="AB1" s="55"/>
+      <c r="AC1" s="55"/>
+      <c r="AD1" s="56"/>
+      <c r="AE1" s="56"/>
+      <c r="AF1" s="57"/>
+      <c r="AG1" s="57"/>
+      <c r="AH1" s="57"/>
+      <c r="AI1" s="58"/>
+      <c r="AJ1" s="58"/>
+      <c r="AK1" s="58"/>
+      <c r="AL1" s="56"/>
+      <c r="AM1" s="56"/>
+      <c r="AN1" s="56"/>
+      <c r="AO1" s="56"/>
+      <c r="AP1" s="56"/>
+      <c r="AQ1" s="56"/>
+      <c r="AR1" s="56"/>
+      <c r="AS1" s="56"/>
+      <c r="AT1" s="56"/>
+      <c r="AU1" s="56"/>
+      <c r="AV1" s="56"/>
+    </row>
+    <row r="2" s="65" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="56"/>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="56"/>
-      <c r="G2" s="56"/>
-      <c r="H2" s="56"/>
-      <c r="I2" s="56"/>
-      <c r="J2" s="56"/>
-      <c r="K2" s="56"/>
-      <c r="L2" s="56"/>
-      <c r="M2" s="56"/>
-      <c r="N2" s="56"/>
-      <c r="O2" s="56"/>
-      <c r="P2" s="56"/>
-      <c r="Q2" s="56"/>
-      <c r="R2" s="56"/>
-      <c r="S2" s="56"/>
-      <c r="T2" s="56"/>
-      <c r="U2" s="56"/>
-      <c r="V2" s="56"/>
-      <c r="W2" s="56"/>
-      <c r="X2" s="56"/>
-      <c r="Y2" s="56"/>
-      <c r="Z2" s="56"/>
-      <c r="AA2" s="56"/>
-      <c r="AB2" s="56"/>
-      <c r="AC2" s="56"/>
-      <c r="AF2" s="53"/>
-      <c r="AG2" s="53"/>
-      <c r="AH2" s="53"/>
-      <c r="AI2" s="0"/>
-      <c r="AJ2" s="0"/>
-      <c r="AK2" s="0"/>
-    </row>
-    <row r="3" s="59" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="58" t="s">
+      <c r="B2" s="60"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="60"/>
+      <c r="N2" s="60"/>
+      <c r="O2" s="60"/>
+      <c r="P2" s="60"/>
+      <c r="Q2" s="60"/>
+      <c r="R2" s="60"/>
+      <c r="S2" s="60"/>
+      <c r="T2" s="60"/>
+      <c r="U2" s="60"/>
+      <c r="V2" s="60"/>
+      <c r="W2" s="60"/>
+      <c r="X2" s="60"/>
+      <c r="Y2" s="60"/>
+      <c r="Z2" s="60"/>
+      <c r="AA2" s="61"/>
+      <c r="AB2" s="61"/>
+      <c r="AC2" s="61"/>
+      <c r="AD2" s="62"/>
+      <c r="AE2" s="62"/>
+      <c r="AF2" s="63"/>
+      <c r="AG2" s="63"/>
+      <c r="AH2" s="63"/>
+      <c r="AI2" s="64"/>
+      <c r="AJ2" s="64"/>
+      <c r="AK2" s="64"/>
+      <c r="AL2" s="62"/>
+      <c r="AM2" s="62"/>
+      <c r="AN2" s="62"/>
+      <c r="AO2" s="62"/>
+      <c r="AP2" s="62"/>
+      <c r="AQ2" s="62"/>
+      <c r="AR2" s="62"/>
+      <c r="AS2" s="62"/>
+      <c r="AT2" s="62"/>
+      <c r="AU2" s="62"/>
+      <c r="AV2" s="62"/>
+    </row>
+    <row r="3" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="58"/>
-      <c r="E3" s="58"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="58"/>
-      <c r="I3" s="58"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="58"/>
-      <c r="L3" s="58"/>
-      <c r="M3" s="58"/>
-      <c r="N3" s="58"/>
-      <c r="O3" s="58"/>
-      <c r="P3" s="58"/>
-      <c r="Q3" s="58"/>
-      <c r="R3" s="58"/>
-      <c r="S3" s="58"/>
-      <c r="T3" s="58"/>
-      <c r="U3" s="58"/>
-      <c r="V3" s="58"/>
-      <c r="W3" s="58"/>
-      <c r="X3" s="58"/>
-      <c r="Y3" s="58"/>
-      <c r="Z3" s="58"/>
-      <c r="AA3" s="58"/>
-      <c r="AB3" s="58"/>
-      <c r="AC3" s="58"/>
-      <c r="AF3" s="53"/>
-      <c r="AG3" s="53"/>
-      <c r="AH3" s="53"/>
-      <c r="AI3" s="0"/>
-      <c r="AJ3" s="0"/>
-      <c r="AK3" s="0"/>
-    </row>
-    <row r="4" s="64" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="61" t="s">
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
+      <c r="M3" s="66"/>
+      <c r="N3" s="66"/>
+      <c r="O3" s="66"/>
+      <c r="P3" s="66"/>
+      <c r="Q3" s="66"/>
+      <c r="R3" s="66"/>
+      <c r="S3" s="66"/>
+      <c r="T3" s="66"/>
+      <c r="U3" s="66"/>
+      <c r="V3" s="66"/>
+      <c r="W3" s="66"/>
+      <c r="X3" s="66"/>
+      <c r="Y3" s="66"/>
+      <c r="Z3" s="66"/>
+      <c r="AA3" s="67"/>
+      <c r="AB3" s="67"/>
+      <c r="AC3" s="67"/>
+      <c r="AD3" s="68"/>
+      <c r="AE3" s="68"/>
+      <c r="AF3" s="69"/>
+      <c r="AG3" s="69"/>
+      <c r="AH3" s="69"/>
+      <c r="AI3" s="70"/>
+      <c r="AJ3" s="70"/>
+      <c r="AK3" s="70"/>
+      <c r="AL3" s="68"/>
+      <c r="AM3" s="68"/>
+      <c r="AN3" s="68"/>
+      <c r="AO3" s="68"/>
+      <c r="AP3" s="68"/>
+      <c r="AQ3" s="68"/>
+      <c r="AR3" s="68"/>
+      <c r="AS3" s="68"/>
+      <c r="AT3" s="68"/>
+      <c r="AU3" s="68"/>
+      <c r="AV3" s="68"/>
+    </row>
+    <row r="4" s="76" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="73" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="61" t="s">
+      <c r="D4" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="61" t="s">
+      <c r="E4" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="F4" s="61" t="s">
+      <c r="F4" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="61" t="s">
+      <c r="G4" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="61" t="s">
+      <c r="H4" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="61" t="s">
+      <c r="I4" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="J4" s="62" t="s">
+      <c r="J4" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="K4" s="62" t="s">
+      <c r="K4" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="63" t="s">
+      <c r="L4" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="63" t="s">
+      <c r="M4" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="63" t="s">
+      <c r="N4" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="63" t="s">
+      <c r="O4" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="P4" s="63" t="s">
+      <c r="P4" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="Q4" s="61" t="s">
+      <c r="Q4" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="R4" s="63" t="s">
+      <c r="R4" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="S4" s="63" t="s">
+      <c r="S4" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="T4" s="63" t="s">
+      <c r="T4" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="U4" s="63" t="s">
+      <c r="U4" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="V4" s="63" t="s">
+      <c r="V4" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="W4" s="63" t="s">
+      <c r="W4" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="X4" s="63" t="s">
+      <c r="X4" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="Y4" s="63" t="s">
+      <c r="Y4" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="Z4" s="63" t="s">
+      <c r="Z4" s="75" t="s">
         <v>9</v>
       </c>
-      <c r="AA4" s="63" t="s">
+      <c r="AA4" s="55" t="s">
         <v>10</v>
       </c>
-      <c r="AB4" s="63"/>
-      <c r="AC4" s="63"/>
-      <c r="AF4" s="53"/>
-      <c r="AG4" s="53"/>
-      <c r="AH4" s="53"/>
-      <c r="AI4" s="0"/>
-      <c r="AJ4" s="0"/>
-      <c r="AK4" s="0"/>
-    </row>
-    <row r="5" s="65" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="58" t="s">
+      <c r="AB4" s="55"/>
+      <c r="AC4" s="55"/>
+      <c r="AD4" s="56"/>
+      <c r="AE4" s="56"/>
+      <c r="AF4" s="57"/>
+      <c r="AG4" s="57"/>
+      <c r="AH4" s="57"/>
+      <c r="AI4" s="58"/>
+      <c r="AJ4" s="58"/>
+      <c r="AK4" s="58"/>
+      <c r="AL4" s="56"/>
+      <c r="AM4" s="56"/>
+      <c r="AN4" s="56"/>
+      <c r="AO4" s="56"/>
+      <c r="AP4" s="56"/>
+      <c r="AQ4" s="56"/>
+      <c r="AR4" s="56"/>
+      <c r="AS4" s="56"/>
+      <c r="AT4" s="56"/>
+      <c r="AU4" s="56"/>
+      <c r="AV4" s="56"/>
+    </row>
+    <row r="5" s="78" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="58"/>
-      <c r="C5" s="58"/>
-      <c r="D5" s="58"/>
-      <c r="E5" s="58"/>
-      <c r="F5" s="58"/>
-      <c r="G5" s="58"/>
-      <c r="H5" s="58"/>
-      <c r="I5" s="58"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="58"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="58"/>
-      <c r="N5" s="58"/>
-      <c r="O5" s="58"/>
-      <c r="P5" s="58"/>
-      <c r="Q5" s="58"/>
-      <c r="R5" s="58"/>
-      <c r="S5" s="58"/>
-      <c r="T5" s="58"/>
-      <c r="U5" s="58"/>
-      <c r="V5" s="58"/>
-      <c r="W5" s="58"/>
-      <c r="X5" s="58"/>
-      <c r="Y5" s="58"/>
-      <c r="Z5" s="58"/>
-      <c r="AA5" s="58"/>
-      <c r="AB5" s="58"/>
-      <c r="AC5" s="58"/>
-      <c r="AF5" s="53"/>
-      <c r="AG5" s="53"/>
-      <c r="AH5" s="53"/>
-      <c r="AI5" s="0"/>
-      <c r="AJ5" s="0"/>
-      <c r="AK5" s="0"/>
-    </row>
-    <row r="6" s="66" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="60" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="61" t="s">
+      <c r="B5" s="66"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="66"/>
+      <c r="J5" s="66"/>
+      <c r="K5" s="66"/>
+      <c r="L5" s="66"/>
+      <c r="M5" s="66"/>
+      <c r="N5" s="66"/>
+      <c r="O5" s="66"/>
+      <c r="P5" s="66"/>
+      <c r="Q5" s="66"/>
+      <c r="R5" s="66"/>
+      <c r="S5" s="66"/>
+      <c r="T5" s="66"/>
+      <c r="U5" s="66"/>
+      <c r="V5" s="66"/>
+      <c r="W5" s="66"/>
+      <c r="X5" s="66"/>
+      <c r="Y5" s="66"/>
+      <c r="Z5" s="66"/>
+      <c r="AA5" s="67"/>
+      <c r="AB5" s="67"/>
+      <c r="AC5" s="67"/>
+      <c r="AD5" s="77"/>
+      <c r="AE5" s="77"/>
+      <c r="AF5" s="69"/>
+      <c r="AG5" s="69"/>
+      <c r="AH5" s="69"/>
+      <c r="AI5" s="70"/>
+      <c r="AJ5" s="70"/>
+      <c r="AK5" s="70"/>
+      <c r="AL5" s="77"/>
+      <c r="AM5" s="77"/>
+      <c r="AN5" s="77"/>
+      <c r="AO5" s="77"/>
+      <c r="AP5" s="77"/>
+      <c r="AQ5" s="77"/>
+      <c r="AR5" s="77"/>
+      <c r="AS5" s="77"/>
+      <c r="AT5" s="77"/>
+      <c r="AU5" s="77"/>
+      <c r="AV5" s="77"/>
+    </row>
+    <row r="6" s="81" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="73" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="61" t="s">
+      <c r="C6" s="73" t="s">
         <v>131</v>
       </c>
-      <c r="D6" s="61" t="s">
+      <c r="D6" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="E6" s="60" t="s">
+      <c r="E6" s="72" t="s">
         <v>133</v>
       </c>
-      <c r="F6" s="60" t="s">
+      <c r="F6" s="72" t="s">
         <v>133</v>
       </c>
-      <c r="G6" s="60" t="s">
+      <c r="G6" s="72" t="s">
         <v>132</v>
       </c>
-      <c r="H6" s="61" t="s">
+      <c r="H6" s="73" t="s">
         <v>132</v>
       </c>
-      <c r="I6" s="61" t="s">
+      <c r="I6" s="73" t="s">
         <v>159</v>
       </c>
-      <c r="J6" s="62" t="s">
+      <c r="J6" s="74" t="s">
         <v>110</v>
       </c>
-      <c r="K6" s="62" t="s">
+      <c r="K6" s="74" t="s">
         <v>159</v>
       </c>
-      <c r="L6" s="62" t="s">
+      <c r="L6" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="M6" s="62" t="s">
+      <c r="M6" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="62" t="s">
+      <c r="N6" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="O6" s="62" t="s">
+      <c r="O6" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="P6" s="62" t="s">
+      <c r="P6" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="Q6" s="61" t="s">
+      <c r="Q6" s="73" t="s">
         <v>159</v>
       </c>
-      <c r="R6" s="62" t="s">
+      <c r="R6" s="74" t="s">
         <v>110</v>
       </c>
-      <c r="S6" s="62" t="s">
+      <c r="S6" s="74" t="s">
         <v>159</v>
       </c>
-      <c r="T6" s="62" t="s">
+      <c r="T6" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="U6" s="62" t="s">
+      <c r="U6" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="V6" s="62" t="s">
+      <c r="V6" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="W6" s="62" t="s">
+      <c r="W6" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="X6" s="62" t="s">
+      <c r="X6" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="Y6" s="62" t="s">
+      <c r="Y6" s="74" t="s">
         <v>132</v>
       </c>
-      <c r="Z6" s="62" t="s">
+      <c r="Z6" s="74" t="s">
         <v>13</v>
       </c>
-      <c r="AA6" s="62" t="s">
+      <c r="AA6" s="79" t="s">
         <v>134</v>
       </c>
-      <c r="AB6" s="62"/>
-      <c r="AC6" s="62"/>
-      <c r="AF6" s="53"/>
-      <c r="AG6" s="53"/>
-      <c r="AH6" s="53"/>
-      <c r="AI6" s="0"/>
-      <c r="AJ6" s="0"/>
-      <c r="AK6" s="0"/>
-    </row>
-    <row r="7" s="68" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="67" t="s">
+      <c r="AB6" s="79"/>
+      <c r="AC6" s="79"/>
+      <c r="AD6" s="80"/>
+      <c r="AE6" s="80"/>
+      <c r="AF6" s="57"/>
+      <c r="AG6" s="57"/>
+      <c r="AH6" s="57"/>
+      <c r="AI6" s="58"/>
+      <c r="AJ6" s="58"/>
+      <c r="AK6" s="58"/>
+      <c r="AL6" s="80"/>
+      <c r="AM6" s="80"/>
+      <c r="AN6" s="80"/>
+      <c r="AO6" s="80"/>
+      <c r="AP6" s="80"/>
+      <c r="AQ6" s="80"/>
+      <c r="AR6" s="80"/>
+      <c r="AS6" s="80"/>
+      <c r="AT6" s="80"/>
+      <c r="AU6" s="80"/>
+      <c r="AV6" s="80"/>
+    </row>
+    <row r="7" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="67"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="67"/>
-      <c r="E7" s="67"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="H7" s="67"/>
-      <c r="I7" s="67"/>
-      <c r="J7" s="67"/>
-      <c r="K7" s="67"/>
-      <c r="L7" s="67"/>
-      <c r="M7" s="67"/>
-      <c r="N7" s="67"/>
-      <c r="O7" s="67"/>
-      <c r="P7" s="67"/>
-      <c r="Q7" s="67"/>
-      <c r="R7" s="67"/>
-      <c r="S7" s="67"/>
-      <c r="T7" s="67"/>
-      <c r="U7" s="67"/>
-      <c r="V7" s="67"/>
-      <c r="W7" s="67"/>
-      <c r="X7" s="67"/>
-      <c r="Y7" s="67"/>
-      <c r="Z7" s="67"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="82"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="82"/>
+      <c r="O7" s="82"/>
+      <c r="P7" s="82"/>
+      <c r="Q7" s="82"/>
+      <c r="R7" s="82"/>
+      <c r="S7" s="82"/>
+      <c r="T7" s="82"/>
+      <c r="U7" s="82"/>
+      <c r="V7" s="82"/>
+      <c r="W7" s="82"/>
+      <c r="X7" s="82"/>
+      <c r="Y7" s="82"/>
+      <c r="Z7" s="82"/>
       <c r="AA7" s="67"/>
       <c r="AB7" s="67"/>
       <c r="AC7" s="67"/>
-      <c r="AF7" s="53"/>
-      <c r="AG7" s="53"/>
-      <c r="AH7" s="53"/>
-      <c r="AI7" s="0"/>
-      <c r="AJ7" s="0"/>
-      <c r="AK7" s="0"/>
-    </row>
-    <row r="8" s="69" customFormat="true" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="62" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="62"/>
-      <c r="C8" s="62" t="s">
+      <c r="AD7" s="68"/>
+      <c r="AE7" s="68"/>
+      <c r="AF7" s="69"/>
+      <c r="AG7" s="69"/>
+      <c r="AH7" s="69"/>
+      <c r="AI7" s="70"/>
+      <c r="AJ7" s="70"/>
+      <c r="AK7" s="70"/>
+      <c r="AL7" s="68"/>
+      <c r="AM7" s="68"/>
+      <c r="AN7" s="68"/>
+      <c r="AO7" s="68"/>
+      <c r="AP7" s="68"/>
+      <c r="AQ7" s="68"/>
+      <c r="AR7" s="68"/>
+      <c r="AS7" s="68"/>
+      <c r="AT7" s="68"/>
+      <c r="AU7" s="68"/>
+      <c r="AV7" s="68"/>
+    </row>
+    <row r="8" s="85" customFormat="true" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="74"/>
+      <c r="C8" s="74" t="s">
         <v>160</v>
       </c>
-      <c r="D8" s="62" t="s">
+      <c r="D8" s="74" t="s">
         <v>161</v>
       </c>
-      <c r="E8" s="62"/>
-      <c r="F8" s="62" t="s">
+      <c r="E8" s="74"/>
+      <c r="F8" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="G8" s="62"/>
-      <c r="H8" s="62"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="62" t="s">
+      <c r="G8" s="74"/>
+      <c r="H8" s="74"/>
+      <c r="I8" s="74"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74" t="s">
         <v>162</v>
       </c>
-      <c r="L8" s="62" t="s">
+      <c r="L8" s="74" t="s">
         <v>163</v>
       </c>
-      <c r="M8" s="62" t="s">
+      <c r="M8" s="74" t="s">
         <v>164</v>
       </c>
-      <c r="N8" s="62" t="s">
+      <c r="N8" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="O8" s="62"/>
-      <c r="P8" s="62"/>
-      <c r="Q8" s="62"/>
-      <c r="R8" s="62"/>
-      <c r="S8" s="62" t="s">
+      <c r="O8" s="74"/>
+      <c r="P8" s="74"/>
+      <c r="Q8" s="74"/>
+      <c r="R8" s="74"/>
+      <c r="S8" s="74" t="s">
         <v>165</v>
       </c>
-      <c r="T8" s="62" t="s">
+      <c r="T8" s="74" t="s">
         <v>166</v>
       </c>
-      <c r="U8" s="62" t="s">
+      <c r="U8" s="74" t="s">
         <v>167</v>
       </c>
-      <c r="V8" s="62" t="s">
+      <c r="V8" s="74" t="s">
         <v>168</v>
       </c>
-      <c r="W8" s="62" t="s">
+      <c r="W8" s="74" t="s">
         <v>169</v>
       </c>
-      <c r="X8" s="62" t="s">
+      <c r="X8" s="74" t="s">
         <v>170</v>
       </c>
-      <c r="Y8" s="62" t="s">
+      <c r="Y8" s="74" t="s">
         <v>171</v>
       </c>
-      <c r="Z8" s="62" t="s">
+      <c r="Z8" s="74" t="s">
         <v>172</v>
       </c>
-      <c r="AA8" s="62" t="s">
+      <c r="AA8" s="79" t="s">
         <v>173</v>
       </c>
-      <c r="AB8" s="62"/>
-      <c r="AC8" s="62"/>
-      <c r="AF8" s="53"/>
-      <c r="AG8" s="53"/>
-      <c r="AH8" s="53"/>
-      <c r="AI8" s="0"/>
-      <c r="AJ8" s="0"/>
-      <c r="AK8" s="0"/>
-    </row>
-    <row r="9" s="71" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="70" t="s">
+      <c r="AB8" s="79"/>
+      <c r="AC8" s="79"/>
+      <c r="AD8" s="84"/>
+      <c r="AE8" s="84"/>
+      <c r="AF8" s="57"/>
+      <c r="AG8" s="57"/>
+      <c r="AH8" s="57"/>
+      <c r="AI8" s="58"/>
+      <c r="AJ8" s="58"/>
+      <c r="AK8" s="58"/>
+      <c r="AL8" s="84"/>
+      <c r="AM8" s="84"/>
+      <c r="AN8" s="84"/>
+      <c r="AO8" s="84"/>
+      <c r="AP8" s="84"/>
+      <c r="AQ8" s="84"/>
+      <c r="AR8" s="84"/>
+      <c r="AS8" s="84"/>
+      <c r="AT8" s="84"/>
+      <c r="AU8" s="84"/>
+      <c r="AV8" s="84"/>
+    </row>
+    <row r="9" s="87" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="70"/>
-      <c r="C9" s="70"/>
-      <c r="D9" s="70"/>
-      <c r="E9" s="70"/>
-      <c r="F9" s="70"/>
-      <c r="G9" s="70"/>
-      <c r="H9" s="70"/>
-      <c r="I9" s="70"/>
-      <c r="J9" s="70"/>
-      <c r="K9" s="70"/>
-      <c r="L9" s="70"/>
-      <c r="M9" s="70"/>
-      <c r="N9" s="70"/>
-      <c r="O9" s="70"/>
-      <c r="P9" s="70"/>
-      <c r="Q9" s="70"/>
-      <c r="R9" s="70"/>
-      <c r="S9" s="70"/>
-      <c r="T9" s="70"/>
-      <c r="U9" s="70"/>
-      <c r="V9" s="70"/>
-      <c r="W9" s="70"/>
-      <c r="X9" s="70"/>
-      <c r="Y9" s="70"/>
-      <c r="Z9" s="70"/>
-      <c r="AA9" s="70"/>
-      <c r="AB9" s="70"/>
-      <c r="AC9" s="70"/>
-      <c r="AF9" s="53"/>
-      <c r="AG9" s="53"/>
-      <c r="AH9" s="53"/>
-      <c r="AI9" s="0"/>
-      <c r="AJ9" s="0"/>
-      <c r="AK9" s="0"/>
+      <c r="B9" s="86"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
+      <c r="M9" s="86"/>
+      <c r="N9" s="86"/>
+      <c r="O9" s="86"/>
+      <c r="P9" s="86"/>
+      <c r="Q9" s="86"/>
+      <c r="R9" s="86"/>
+      <c r="S9" s="86"/>
+      <c r="T9" s="86"/>
+      <c r="U9" s="86"/>
+      <c r="V9" s="86"/>
+      <c r="W9" s="86"/>
+      <c r="X9" s="86"/>
+      <c r="Y9" s="86"/>
+      <c r="Z9" s="86"/>
+      <c r="AA9" s="61"/>
+      <c r="AB9" s="61"/>
+      <c r="AC9" s="61"/>
+      <c r="AD9" s="62"/>
+      <c r="AE9" s="62"/>
+      <c r="AF9" s="63"/>
+      <c r="AG9" s="63"/>
+      <c r="AH9" s="63"/>
+      <c r="AI9" s="64"/>
+      <c r="AJ9" s="64"/>
+      <c r="AK9" s="64"/>
+      <c r="AL9" s="62"/>
+      <c r="AM9" s="62"/>
+      <c r="AN9" s="62"/>
+      <c r="AO9" s="62"/>
+      <c r="AP9" s="62"/>
+      <c r="AQ9" s="62"/>
+      <c r="AR9" s="62"/>
+      <c r="AS9" s="62"/>
+      <c r="AT9" s="62"/>
+      <c r="AU9" s="62"/>
+      <c r="AV9" s="62"/>
     </row>
     <row r="10" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="72" t="s">
+      <c r="A10" s="88" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="72" t="s">
+      <c r="B10" s="88" t="s">
         <v>174</v>
       </c>
-      <c r="C10" s="72" t="s">
+      <c r="C10" s="88" t="s">
         <v>175</v>
       </c>
-      <c r="D10" s="72" t="s">
+      <c r="D10" s="88" t="s">
         <v>176</v>
       </c>
-      <c r="E10" s="72" t="s">
+      <c r="E10" s="88" t="s">
         <v>121</v>
       </c>
-      <c r="F10" s="73" t="s">
+      <c r="F10" s="89" t="s">
         <v>177</v>
       </c>
-      <c r="G10" s="73" t="s">
+      <c r="G10" s="89" t="s">
         <v>178</v>
       </c>
-      <c r="H10" s="73" t="s">
+      <c r="H10" s="89" t="s">
         <v>179</v>
       </c>
-      <c r="I10" s="73" t="s">
+      <c r="I10" s="89" t="s">
         <v>180</v>
       </c>
-      <c r="J10" s="73" t="s">
+      <c r="J10" s="89" t="s">
         <v>181</v>
       </c>
-      <c r="K10" s="73" t="s">
+      <c r="K10" s="89" t="s">
         <v>182</v>
       </c>
-      <c r="L10" s="73" t="s">
+      <c r="L10" s="89" t="s">
         <v>183</v>
       </c>
-      <c r="M10" s="73" t="s">
+      <c r="M10" s="89" t="s">
         <v>184</v>
       </c>
-      <c r="N10" s="74" t="s">
+      <c r="N10" s="90" t="s">
         <v>185</v>
       </c>
-      <c r="O10" s="74" t="s">
+      <c r="O10" s="90" t="s">
         <v>186</v>
       </c>
-      <c r="P10" s="74" t="s">
+      <c r="P10" s="90" t="s">
         <v>187</v>
       </c>
-      <c r="Q10" s="74" t="s">
+      <c r="Q10" s="90" t="s">
         <v>188</v>
       </c>
-      <c r="R10" s="74" t="s">
+      <c r="R10" s="90" t="s">
         <v>189</v>
       </c>
-      <c r="S10" s="74" t="s">
+      <c r="S10" s="90" t="s">
         <v>190</v>
       </c>
-      <c r="T10" s="74" t="s">
+      <c r="T10" s="90" t="s">
         <v>191</v>
       </c>
-      <c r="U10" s="74" t="s">
+      <c r="U10" s="90" t="s">
         <v>192</v>
       </c>
-      <c r="V10" s="75" t="s">
+      <c r="V10" s="91" t="s">
         <v>193</v>
       </c>
-      <c r="W10" s="75" t="s">
+      <c r="W10" s="91" t="s">
         <v>194</v>
       </c>
-      <c r="X10" s="75" t="s">
+      <c r="X10" s="91" t="s">
         <v>170</v>
       </c>
-      <c r="Y10" s="75" t="s">
+      <c r="Y10" s="91" t="s">
         <v>195</v>
       </c>
-      <c r="Z10" s="75" t="s">
+      <c r="Z10" s="91" t="s">
         <v>196</v>
       </c>
-      <c r="AA10" s="72" t="s">
+      <c r="AA10" s="92" t="s">
         <v>197</v>
       </c>
-      <c r="AB10" s="76"/>
-      <c r="AC10" s="76"/>
+      <c r="AB10" s="93"/>
+      <c r="AC10" s="93"/>
+      <c r="AD10" s="57"/>
+      <c r="AE10" s="94"/>
+      <c r="AF10" s="57"/>
+      <c r="AG10" s="57"/>
+      <c r="AH10" s="57"/>
+      <c r="AI10" s="58"/>
+      <c r="AJ10" s="58"/>
+      <c r="AK10" s="58"/>
+      <c r="AL10" s="57"/>
+      <c r="AM10" s="57"/>
+      <c r="AN10" s="57"/>
+      <c r="AO10" s="57"/>
+      <c r="AP10" s="57"/>
+      <c r="AQ10" s="57"/>
+      <c r="AR10" s="57"/>
+      <c r="AS10" s="57"/>
+      <c r="AT10" s="57"/>
+      <c r="AU10" s="57"/>
+      <c r="AV10" s="57"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="76" t="s">
+      <c r="A11" s="95" t="s">
         <v>198</v>
       </c>
-      <c r="B11" s="76" t="n">
-        <v>1</v>
-      </c>
-      <c r="C11" s="76" t="n">
+      <c r="B11" s="95" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="95" t="n">
         <v>100</v>
       </c>
-      <c r="D11" s="76" t="n">
+      <c r="D11" s="95" t="n">
         <v>610</v>
       </c>
-      <c r="E11" s="76" t="n">
+      <c r="E11" s="95" t="n">
         <v>60</v>
       </c>
-      <c r="F11" s="76" t="n">
-        <f aca="false">SUM(D11:E11)</f>
-        <v>670</v>
-      </c>
-      <c r="G11" s="76" t="n">
+      <c r="F11" s="95" t="n">
+        <v>5</v>
+      </c>
+      <c r="G11" s="95" t="n">
         <v>35</v>
       </c>
-      <c r="H11" s="76" t="n">
+      <c r="H11" s="95" t="n">
         <v>10</v>
       </c>
-      <c r="I11" s="76" t="n">
+      <c r="I11" s="95" t="n">
         <v>1200</v>
       </c>
-      <c r="J11" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="K11" s="77" t="e">
-        <f aca="false">(F8*H8)/((#REF!+T8+N8+H8+V8)*(I8/1000)*(F8+G8))*10^(8.07-1703/(J8+273.15))/760*1.01325</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L11" s="76" t="n">
+      <c r="J11" s="96" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="96" t="n">
+        <f aca="false">(F11*H11)/((L11+T11+N11+H11+V11)*(I11/1000)*(F11+G11))*10^(8.07-1703/(J11+273.15))/760*1.01325</f>
+        <v>4.85517381623865E-005</v>
+      </c>
+      <c r="L11" s="95" t="n">
         <v>1000</v>
       </c>
-      <c r="M11" s="78" t="b">
-        <v>1</v>
-      </c>
-      <c r="N11" s="76" t="n">
+      <c r="M11" s="97" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N11" s="95" t="n">
         <v>50</v>
       </c>
-      <c r="O11" s="76" t="n">
+      <c r="O11" s="95" t="n">
         <v>3</v>
       </c>
-      <c r="P11" s="76" t="n">
+      <c r="P11" s="95" t="n">
         <v>3</v>
       </c>
-      <c r="Q11" s="76" t="n">
+      <c r="Q11" s="95" t="n">
         <v>0</v>
       </c>
-      <c r="R11" s="77" t="n">
+      <c r="R11" s="96" t="n">
         <v>30</v>
       </c>
-      <c r="S11" s="77" t="n">
+      <c r="S11" s="96" t="n">
         <v>0.0169</v>
       </c>
-      <c r="T11" s="76" t="n">
+      <c r="T11" s="95" t="n">
         <v>1000</v>
       </c>
-      <c r="U11" s="79" t="b">
-        <v>1</v>
-      </c>
-      <c r="V11" s="76" t="n">
+      <c r="U11" s="97" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="V11" s="95" t="n">
         <v>3</v>
       </c>
-      <c r="W11" s="76" t="n">
+      <c r="W11" s="95" t="n">
         <f aca="false">SetUp!F12*E11</f>
         <v>6</v>
       </c>
-      <c r="X11" s="76" t="e">
+      <c r="X11" s="95" t="e">
         <f aca="false">W11/(#REF!+T11+V11+N11+H11)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Y11" s="76" t="n">
+        <v>#REF!</v>
+      </c>
+      <c r="Y11" s="95" t="n">
         <v>200</v>
       </c>
-      <c r="Z11" s="80" t="b">
+      <c r="Z11" s="97" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AA11" s="76" t="n">
+      <c r="AA11" s="93" t="n">
         <v>234</v>
       </c>
-      <c r="AB11" s="76"/>
-      <c r="AC11" s="76"/>
+      <c r="AB11" s="93"/>
+      <c r="AC11" s="93"/>
+      <c r="AD11" s="57"/>
+      <c r="AE11" s="94"/>
+      <c r="AF11" s="57"/>
+      <c r="AG11" s="57"/>
+      <c r="AH11" s="57"/>
+      <c r="AI11" s="58"/>
+      <c r="AJ11" s="58"/>
+      <c r="AK11" s="58"/>
+      <c r="AL11" s="57"/>
+      <c r="AM11" s="57"/>
+      <c r="AN11" s="57"/>
+      <c r="AO11" s="57"/>
+      <c r="AP11" s="57"/>
+      <c r="AQ11" s="57"/>
+      <c r="AR11" s="57"/>
+      <c r="AS11" s="57"/>
+      <c r="AT11" s="57"/>
+      <c r="AU11" s="57"/>
+      <c r="AV11" s="57"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="76" t="s">
+      <c r="A12" s="95" t="s">
         <v>199</v>
       </c>
-      <c r="B12" s="76" t="n">
-        <v>1</v>
-      </c>
-      <c r="C12" s="76" t="n">
+      <c r="B12" s="95" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="95" t="n">
         <v>100</v>
       </c>
-      <c r="D12" s="76" t="n">
+      <c r="D12" s="95" t="n">
         <v>610</v>
       </c>
-      <c r="E12" s="76" t="n">
+      <c r="E12" s="95" t="n">
         <v>60</v>
       </c>
-      <c r="F12" s="76" t="n">
-        <f aca="false">SUM(D12:E12)</f>
-        <v>670</v>
-      </c>
-      <c r="G12" s="76" t="n">
+      <c r="F12" s="95" t="n">
+        <v>5</v>
+      </c>
+      <c r="G12" s="95" t="n">
         <v>35</v>
       </c>
-      <c r="H12" s="76" t="n">
+      <c r="H12" s="95" t="n">
         <v>10</v>
       </c>
-      <c r="I12" s="76" t="n">
+      <c r="I12" s="95" t="n">
         <v>1200</v>
       </c>
-      <c r="J12" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="K12" s="77" t="n">
-        <v>4.86E-005</v>
-      </c>
-      <c r="L12" s="76" t="n">
+      <c r="J12" s="96" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="96" t="n">
+        <f aca="false">(F12*H12)/((L12+T12+N12+H12+V12)*(I12/1000)*(F12+G12))*10^(8.07-1703/(J12+273.15))/760*1.01325</f>
+        <v>4.85517381623865E-005</v>
+      </c>
+      <c r="L12" s="95" t="n">
         <v>1000</v>
       </c>
-      <c r="M12" s="78" t="b">
-        <v>1</v>
-      </c>
-      <c r="N12" s="76" t="n">
+      <c r="M12" s="97" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N12" s="95" t="n">
         <v>50</v>
       </c>
-      <c r="O12" s="76" t="n">
+      <c r="O12" s="95" t="n">
         <v>3</v>
       </c>
-      <c r="P12" s="76" t="n">
+      <c r="P12" s="95" t="n">
         <v>3</v>
       </c>
-      <c r="Q12" s="76" t="n">
+      <c r="Q12" s="95" t="n">
         <v>0</v>
       </c>
-      <c r="R12" s="77" t="n">
+      <c r="R12" s="96" t="n">
         <v>30</v>
       </c>
-      <c r="S12" s="77" t="n">
+      <c r="S12" s="96" t="n">
         <v>0.0169</v>
       </c>
-      <c r="T12" s="76" t="n">
+      <c r="T12" s="95" t="n">
         <v>1000</v>
       </c>
-      <c r="U12" s="79" t="b">
-        <v>1</v>
-      </c>
-      <c r="V12" s="76" t="n">
+      <c r="U12" s="97" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="V12" s="95" t="n">
         <v>3</v>
       </c>
-      <c r="W12" s="76" t="n">
+      <c r="W12" s="95" t="n">
         <v>4</v>
       </c>
-      <c r="X12" s="76" t="e">
+      <c r="X12" s="95" t="e">
         <f aca="false">W12/(#REF!+T12+V12+N12+H12)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Y12" s="76" t="n">
+        <v>#REF!</v>
+      </c>
+      <c r="Y12" s="95" t="n">
         <v>200</v>
       </c>
-      <c r="Z12" s="81" t="b">
+      <c r="Z12" s="97" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AA12" s="76" t="n">
+      <c r="AA12" s="93" t="n">
         <v>234</v>
       </c>
-      <c r="AB12" s="76"/>
-      <c r="AC12" s="76"/>
+      <c r="AB12" s="93"/>
+      <c r="AC12" s="93"/>
+      <c r="AD12" s="57"/>
+      <c r="AE12" s="94"/>
+      <c r="AF12" s="57"/>
+      <c r="AG12" s="57"/>
+      <c r="AH12" s="57"/>
+      <c r="AI12" s="58"/>
+      <c r="AJ12" s="58"/>
+      <c r="AK12" s="58"/>
+      <c r="AL12" s="57"/>
+      <c r="AM12" s="57"/>
+      <c r="AN12" s="57"/>
+      <c r="AO12" s="57"/>
+      <c r="AP12" s="57"/>
+      <c r="AQ12" s="57"/>
+      <c r="AR12" s="57"/>
+      <c r="AS12" s="57"/>
+      <c r="AT12" s="57"/>
+      <c r="AU12" s="57"/>
+      <c r="AV12" s="57"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="76" t="s">
+      <c r="A13" s="95" t="s">
         <v>200</v>
       </c>
-      <c r="B13" s="76" t="n">
-        <v>1</v>
-      </c>
-      <c r="C13" s="76" t="n">
+      <c r="B13" s="95" t="n">
+        <v>3</v>
+      </c>
+      <c r="C13" s="95" t="n">
         <v>100</v>
       </c>
-      <c r="D13" s="76" t="n">
+      <c r="D13" s="95" t="n">
         <v>610</v>
       </c>
-      <c r="E13" s="76" t="n">
+      <c r="E13" s="95" t="n">
         <v>60</v>
       </c>
-      <c r="F13" s="76" t="n">
-        <f aca="false">SUM(D13:E13)</f>
-        <v>670</v>
-      </c>
-      <c r="G13" s="76" t="n">
+      <c r="F13" s="95" t="n">
+        <v>5</v>
+      </c>
+      <c r="G13" s="95" t="n">
         <v>35</v>
       </c>
-      <c r="H13" s="76" t="n">
+      <c r="H13" s="95" t="n">
         <v>10</v>
       </c>
-      <c r="I13" s="76" t="n">
+      <c r="I13" s="95" t="n">
         <v>1200</v>
       </c>
-      <c r="J13" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="K13" s="77" t="n">
-        <v>4.86E-005</v>
-      </c>
-      <c r="L13" s="76" t="n">
+      <c r="J13" s="96" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" s="96" t="n">
+        <f aca="false">(F13*H13)/((L13+T13+N13+H13+V13)*(I13/1000)*(F13+G13))*10^(8.07-1703/(J13+273.15))/760*1.01325</f>
+        <v>4.85517381623865E-005</v>
+      </c>
+      <c r="L13" s="95" t="n">
         <v>1000</v>
       </c>
-      <c r="M13" s="79" t="b">
-        <v>1</v>
-      </c>
-      <c r="N13" s="76" t="n">
+      <c r="M13" s="97" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N13" s="95" t="n">
         <v>50</v>
       </c>
-      <c r="O13" s="76" t="n">
+      <c r="O13" s="95" t="n">
         <v>3</v>
       </c>
-      <c r="P13" s="76" t="n">
+      <c r="P13" s="95" t="n">
         <v>3</v>
       </c>
-      <c r="Q13" s="76" t="n">
+      <c r="Q13" s="95" t="n">
         <v>0</v>
       </c>
-      <c r="R13" s="77" t="n">
+      <c r="R13" s="96" t="n">
         <v>30</v>
       </c>
-      <c r="S13" s="77" t="n">
+      <c r="S13" s="96" t="n">
         <v>0.0169</v>
       </c>
-      <c r="T13" s="76" t="n">
+      <c r="T13" s="95" t="n">
         <v>1000</v>
       </c>
-      <c r="U13" s="79" t="b">
-        <v>1</v>
-      </c>
-      <c r="V13" s="76" t="n">
+      <c r="U13" s="97" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="V13" s="95" t="n">
         <v>3</v>
       </c>
-      <c r="W13" s="76" t="n">
+      <c r="W13" s="95" t="n">
         <v>4</v>
       </c>
-      <c r="X13" s="76" t="e">
+      <c r="X13" s="95" t="e">
         <f aca="false">W13/(#REF!+T13+V13+N13+H13)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Y13" s="76" t="n">
+        <v>#REF!</v>
+      </c>
+      <c r="Y13" s="95" t="n">
         <v>200</v>
       </c>
-      <c r="Z13" s="81" t="b">
+      <c r="Z13" s="97" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AA13" s="76" t="n">
+      <c r="AA13" s="93" t="n">
         <v>234</v>
       </c>
-      <c r="AB13" s="76"/>
-      <c r="AC13" s="76"/>
+      <c r="AB13" s="93"/>
+      <c r="AC13" s="93"/>
+      <c r="AD13" s="57"/>
+      <c r="AE13" s="94"/>
+      <c r="AF13" s="57"/>
+      <c r="AG13" s="57"/>
+      <c r="AH13" s="57"/>
+      <c r="AI13" s="58"/>
+      <c r="AJ13" s="58"/>
+      <c r="AK13" s="58"/>
+      <c r="AL13" s="57"/>
+      <c r="AM13" s="57"/>
+      <c r="AN13" s="57"/>
+      <c r="AO13" s="57"/>
+      <c r="AP13" s="57"/>
+      <c r="AQ13" s="57"/>
+      <c r="AR13" s="57"/>
+      <c r="AS13" s="57"/>
+      <c r="AT13" s="57"/>
+      <c r="AU13" s="57"/>
+      <c r="AV13" s="57"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="76" t="s">
+      <c r="A14" s="95" t="s">
         <v>201</v>
       </c>
-      <c r="B14" s="76" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" s="76" t="n">
+      <c r="B14" s="95" t="n">
+        <v>4</v>
+      </c>
+      <c r="C14" s="95" t="n">
         <v>100</v>
       </c>
-      <c r="D14" s="76" t="n">
+      <c r="D14" s="95" t="n">
         <v>610</v>
       </c>
-      <c r="E14" s="76" t="n">
+      <c r="E14" s="95" t="n">
         <v>60</v>
       </c>
-      <c r="F14" s="76" t="n">
-        <f aca="false">SUM(D14:E14)</f>
-        <v>670</v>
-      </c>
-      <c r="G14" s="76" t="n">
+      <c r="F14" s="95" t="n">
+        <v>5</v>
+      </c>
+      <c r="G14" s="95" t="n">
         <v>35</v>
       </c>
-      <c r="H14" s="76" t="n">
+      <c r="H14" s="95" t="n">
         <v>10</v>
       </c>
-      <c r="I14" s="76" t="n">
+      <c r="I14" s="95" t="n">
         <v>1200</v>
       </c>
-      <c r="J14" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="K14" s="77" t="n">
-        <v>4.86E-005</v>
-      </c>
-      <c r="L14" s="76" t="n">
+      <c r="J14" s="96" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="96" t="n">
+        <f aca="false">(F14*H14)/((L14+T14+N14+H14+V14)*(I14/1000)*(F14+G14))*10^(8.07-1703/(J14+273.15))/760*1.01325</f>
+        <v>4.85517381623865E-005</v>
+      </c>
+      <c r="L14" s="95" t="n">
         <v>1000</v>
       </c>
-      <c r="M14" s="79" t="b">
-        <v>1</v>
-      </c>
-      <c r="N14" s="76" t="n">
+      <c r="M14" s="97" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="N14" s="95" t="n">
         <v>50</v>
       </c>
-      <c r="O14" s="76" t="n">
+      <c r="O14" s="95" t="n">
         <v>3</v>
       </c>
-      <c r="P14" s="76" t="n">
+      <c r="P14" s="95" t="n">
         <v>3</v>
       </c>
-      <c r="Q14" s="76" t="n">
+      <c r="Q14" s="95" t="n">
         <v>0</v>
       </c>
-      <c r="R14" s="77" t="n">
+      <c r="R14" s="96" t="n">
         <v>30</v>
       </c>
-      <c r="S14" s="77" t="n">
+      <c r="S14" s="96" t="n">
         <v>0.0169</v>
       </c>
-      <c r="T14" s="76" t="n">
+      <c r="T14" s="95" t="n">
         <v>1000</v>
       </c>
-      <c r="U14" s="79" t="s">
+      <c r="U14" s="97" t="s">
         <v>202</v>
       </c>
-      <c r="V14" s="76" t="n">
+      <c r="V14" s="95" t="n">
         <v>3</v>
       </c>
-      <c r="W14" s="76" t="n">
+      <c r="W14" s="95" t="n">
         <v>4</v>
       </c>
-      <c r="X14" s="76" t="e">
+      <c r="X14" s="95" t="e">
         <f aca="false">W14/(#REF!+T14+V14+N14+H14)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="Y14" s="76" t="n">
+        <v>#REF!</v>
+      </c>
+      <c r="Y14" s="95" t="n">
         <v>200</v>
       </c>
-      <c r="Z14" s="81" t="b">
+      <c r="Z14" s="97" t="n">
+        <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AA14" s="76" t="n">
+      <c r="AA14" s="93" t="n">
         <v>234</v>
       </c>
-      <c r="AB14" s="76"/>
-      <c r="AC14" s="76"/>
+      <c r="AB14" s="93"/>
+      <c r="AC14" s="93"/>
+      <c r="AD14" s="57"/>
+      <c r="AE14" s="94"/>
+      <c r="AF14" s="57"/>
+      <c r="AG14" s="57"/>
+      <c r="AH14" s="57"/>
+      <c r="AI14" s="58"/>
+      <c r="AJ14" s="58"/>
+      <c r="AK14" s="58"/>
+      <c r="AL14" s="57"/>
+      <c r="AM14" s="57"/>
+      <c r="AN14" s="57"/>
+      <c r="AO14" s="57"/>
+      <c r="AP14" s="57"/>
+      <c r="AQ14" s="57"/>
+      <c r="AR14" s="57"/>
+      <c r="AS14" s="57"/>
+      <c r="AT14" s="57"/>
+      <c r="AU14" s="57"/>
+      <c r="AV14" s="57"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="76"/>
-      <c r="B15" s="76"/>
-      <c r="C15" s="76"/>
-      <c r="D15" s="76"/>
-      <c r="E15" s="76"/>
-      <c r="F15" s="76"/>
-      <c r="G15" s="76"/>
-      <c r="H15" s="76"/>
-      <c r="I15" s="76"/>
-      <c r="J15" s="76"/>
-      <c r="K15" s="76"/>
-      <c r="L15" s="76"/>
-      <c r="M15" s="76"/>
-      <c r="N15" s="76"/>
-      <c r="O15" s="76"/>
-      <c r="P15" s="76"/>
-      <c r="Q15" s="76"/>
-      <c r="R15" s="76"/>
-      <c r="S15" s="76"/>
-      <c r="T15" s="76"/>
-      <c r="U15" s="76"/>
-      <c r="V15" s="76"/>
-      <c r="W15" s="76"/>
-      <c r="X15" s="76"/>
-      <c r="Y15" s="76"/>
-      <c r="Z15" s="76"/>
-      <c r="AA15" s="76"/>
-      <c r="AB15" s="76"/>
-      <c r="AC15" s="76"/>
+      <c r="A15" s="95"/>
+      <c r="B15" s="95"/>
+      <c r="C15" s="95"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="95"/>
+      <c r="F15" s="95"/>
+      <c r="G15" s="95"/>
+      <c r="H15" s="95"/>
+      <c r="I15" s="95"/>
+      <c r="J15" s="95"/>
+      <c r="K15" s="95"/>
+      <c r="L15" s="95"/>
+      <c r="M15" s="95"/>
+      <c r="N15" s="95"/>
+      <c r="O15" s="95"/>
+      <c r="P15" s="95"/>
+      <c r="Q15" s="95"/>
+      <c r="R15" s="95"/>
+      <c r="S15" s="95"/>
+      <c r="T15" s="95"/>
+      <c r="U15" s="95"/>
+      <c r="V15" s="95"/>
+      <c r="W15" s="95"/>
+      <c r="X15" s="95"/>
+      <c r="Y15" s="95"/>
+      <c r="Z15" s="95"/>
+      <c r="AA15" s="93"/>
+      <c r="AB15" s="93"/>
+      <c r="AC15" s="93"/>
+      <c r="AD15" s="57"/>
+      <c r="AE15" s="94"/>
+      <c r="AF15" s="57"/>
+      <c r="AG15" s="57"/>
+      <c r="AH15" s="57"/>
+      <c r="AI15" s="58"/>
+      <c r="AJ15" s="58"/>
+      <c r="AK15" s="58"/>
+      <c r="AL15" s="57"/>
+      <c r="AM15" s="57"/>
+      <c r="AN15" s="57"/>
+      <c r="AO15" s="57"/>
+      <c r="AP15" s="57"/>
+      <c r="AQ15" s="57"/>
+      <c r="AR15" s="57"/>
+      <c r="AS15" s="57"/>
+      <c r="AT15" s="57"/>
+      <c r="AU15" s="57"/>
+      <c r="AV15" s="57"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="76"/>
-      <c r="B16" s="76"/>
-      <c r="C16" s="76"/>
-      <c r="D16" s="76"/>
-      <c r="E16" s="76"/>
-      <c r="F16" s="76"/>
-      <c r="G16" s="76"/>
-      <c r="H16" s="76"/>
-      <c r="I16" s="76"/>
-      <c r="J16" s="76"/>
-      <c r="K16" s="76"/>
-      <c r="L16" s="76"/>
-      <c r="M16" s="76"/>
-      <c r="N16" s="76"/>
-      <c r="O16" s="76"/>
-      <c r="P16" s="76"/>
-      <c r="Q16" s="76"/>
-      <c r="R16" s="76"/>
-      <c r="S16" s="76"/>
-      <c r="T16" s="76"/>
-      <c r="U16" s="76"/>
-      <c r="V16" s="76"/>
-      <c r="W16" s="76"/>
-      <c r="X16" s="76"/>
-      <c r="Y16" s="76"/>
-      <c r="Z16" s="76"/>
-      <c r="AA16" s="76"/>
-      <c r="AB16" s="76"/>
-      <c r="AC16" s="76"/>
+      <c r="A16" s="95"/>
+      <c r="B16" s="95"/>
+      <c r="C16" s="95"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="95"/>
+      <c r="F16" s="95"/>
+      <c r="G16" s="95"/>
+      <c r="H16" s="95"/>
+      <c r="I16" s="95"/>
+      <c r="J16" s="95"/>
+      <c r="K16" s="95"/>
+      <c r="L16" s="95"/>
+      <c r="M16" s="95"/>
+      <c r="N16" s="95"/>
+      <c r="O16" s="95"/>
+      <c r="P16" s="95"/>
+      <c r="Q16" s="95"/>
+      <c r="R16" s="95"/>
+      <c r="S16" s="95"/>
+      <c r="T16" s="95"/>
+      <c r="U16" s="95"/>
+      <c r="V16" s="95"/>
+      <c r="W16" s="95"/>
+      <c r="X16" s="95"/>
+      <c r="Y16" s="95"/>
+      <c r="Z16" s="95"/>
+      <c r="AA16" s="93"/>
+      <c r="AB16" s="93"/>
+      <c r="AC16" s="93"/>
+      <c r="AD16" s="57"/>
+      <c r="AE16" s="94"/>
+      <c r="AF16" s="57"/>
+      <c r="AG16" s="57"/>
+      <c r="AH16" s="57"/>
+      <c r="AI16" s="58"/>
+      <c r="AJ16" s="58"/>
+      <c r="AK16" s="58"/>
+      <c r="AL16" s="57"/>
+      <c r="AM16" s="57"/>
+      <c r="AN16" s="57"/>
+      <c r="AO16" s="57"/>
+      <c r="AP16" s="57"/>
+      <c r="AQ16" s="57"/>
+      <c r="AR16" s="57"/>
+      <c r="AS16" s="57"/>
+      <c r="AT16" s="57"/>
+      <c r="AU16" s="57"/>
+      <c r="AV16" s="57"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="76"/>
-      <c r="B17" s="76"/>
-      <c r="C17" s="76"/>
-      <c r="D17" s="76"/>
-      <c r="E17" s="76"/>
-      <c r="F17" s="76"/>
-      <c r="G17" s="76"/>
-      <c r="H17" s="76"/>
-      <c r="I17" s="76"/>
-      <c r="J17" s="76"/>
-      <c r="K17" s="76"/>
-      <c r="L17" s="76"/>
-      <c r="M17" s="76"/>
-      <c r="N17" s="76"/>
-      <c r="O17" s="76"/>
-      <c r="P17" s="76"/>
-      <c r="Q17" s="76"/>
-      <c r="R17" s="76"/>
-      <c r="S17" s="76"/>
-      <c r="T17" s="76"/>
-      <c r="U17" s="76"/>
-      <c r="V17" s="76"/>
-      <c r="W17" s="76"/>
-      <c r="X17" s="76"/>
-      <c r="Y17" s="76"/>
-      <c r="Z17" s="76"/>
-      <c r="AA17" s="76"/>
-      <c r="AB17" s="76"/>
-      <c r="AC17" s="76"/>
+      <c r="A17" s="95"/>
+      <c r="B17" s="95"/>
+      <c r="C17" s="95"/>
+      <c r="D17" s="95"/>
+      <c r="E17" s="95"/>
+      <c r="F17" s="95"/>
+      <c r="G17" s="95"/>
+      <c r="H17" s="95"/>
+      <c r="I17" s="95"/>
+      <c r="J17" s="95"/>
+      <c r="K17" s="95"/>
+      <c r="L17" s="95"/>
+      <c r="M17" s="95"/>
+      <c r="N17" s="95"/>
+      <c r="O17" s="95"/>
+      <c r="P17" s="95"/>
+      <c r="Q17" s="95"/>
+      <c r="R17" s="95"/>
+      <c r="S17" s="95"/>
+      <c r="T17" s="95"/>
+      <c r="U17" s="95"/>
+      <c r="V17" s="95"/>
+      <c r="W17" s="95"/>
+      <c r="X17" s="95"/>
+      <c r="Y17" s="95"/>
+      <c r="Z17" s="95"/>
+      <c r="AA17" s="93"/>
+      <c r="AB17" s="93"/>
+      <c r="AC17" s="93"/>
+      <c r="AD17" s="57"/>
+      <c r="AE17" s="94"/>
+      <c r="AF17" s="57"/>
+      <c r="AG17" s="57"/>
+      <c r="AH17" s="57"/>
+      <c r="AI17" s="58"/>
+      <c r="AJ17" s="58"/>
+      <c r="AK17" s="58"/>
+      <c r="AL17" s="57"/>
+      <c r="AM17" s="57"/>
+      <c r="AN17" s="57"/>
+      <c r="AO17" s="57"/>
+      <c r="AP17" s="57"/>
+      <c r="AQ17" s="57"/>
+      <c r="AR17" s="57"/>
+      <c r="AS17" s="57"/>
+      <c r="AT17" s="57"/>
+      <c r="AU17" s="57"/>
+      <c r="AV17" s="57"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="76"/>
-      <c r="B18" s="76"/>
-      <c r="C18" s="76"/>
-      <c r="D18" s="76"/>
-      <c r="E18" s="76"/>
-      <c r="F18" s="76"/>
-      <c r="G18" s="76"/>
-      <c r="H18" s="76"/>
-      <c r="I18" s="76"/>
-      <c r="J18" s="76"/>
-      <c r="K18" s="76"/>
-      <c r="L18" s="76"/>
-      <c r="M18" s="76"/>
-      <c r="N18" s="76"/>
-      <c r="O18" s="76"/>
-      <c r="P18" s="76"/>
-      <c r="Q18" s="76"/>
-      <c r="R18" s="76"/>
-      <c r="S18" s="76"/>
-      <c r="T18" s="76"/>
-      <c r="U18" s="76"/>
-      <c r="V18" s="76"/>
-      <c r="W18" s="76"/>
-      <c r="X18" s="76"/>
-      <c r="Y18" s="76"/>
-      <c r="Z18" s="76"/>
-      <c r="AA18" s="76"/>
-      <c r="AB18" s="76"/>
-      <c r="AC18" s="76"/>
+      <c r="A18" s="95"/>
+      <c r="B18" s="95"/>
+      <c r="C18" s="95"/>
+      <c r="D18" s="95"/>
+      <c r="E18" s="95"/>
+      <c r="F18" s="95"/>
+      <c r="G18" s="95"/>
+      <c r="H18" s="95"/>
+      <c r="I18" s="95"/>
+      <c r="J18" s="95"/>
+      <c r="K18" s="95"/>
+      <c r="L18" s="95"/>
+      <c r="M18" s="95"/>
+      <c r="N18" s="95"/>
+      <c r="O18" s="95"/>
+      <c r="P18" s="95"/>
+      <c r="Q18" s="95"/>
+      <c r="R18" s="95"/>
+      <c r="S18" s="95"/>
+      <c r="T18" s="95"/>
+      <c r="U18" s="95"/>
+      <c r="V18" s="95"/>
+      <c r="W18" s="95"/>
+      <c r="X18" s="95"/>
+      <c r="Y18" s="95"/>
+      <c r="Z18" s="95"/>
+      <c r="AA18" s="93"/>
+      <c r="AB18" s="93"/>
+      <c r="AC18" s="93"/>
+      <c r="AD18" s="57"/>
+      <c r="AE18" s="94"/>
+      <c r="AF18" s="57"/>
+      <c r="AG18" s="57"/>
+      <c r="AH18" s="57"/>
+      <c r="AI18" s="58"/>
+      <c r="AJ18" s="58"/>
+      <c r="AK18" s="58"/>
+      <c r="AL18" s="57"/>
+      <c r="AM18" s="57"/>
+      <c r="AN18" s="57"/>
+      <c r="AO18" s="57"/>
+      <c r="AP18" s="57"/>
+      <c r="AQ18" s="57"/>
+      <c r="AR18" s="57"/>
+      <c r="AS18" s="57"/>
+      <c r="AT18" s="57"/>
+      <c r="AU18" s="57"/>
+      <c r="AV18" s="57"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="76"/>
-      <c r="B19" s="76"/>
-      <c r="C19" s="76"/>
-      <c r="D19" s="76"/>
-      <c r="E19" s="76"/>
-      <c r="F19" s="76"/>
-      <c r="G19" s="76"/>
-      <c r="H19" s="76"/>
-      <c r="I19" s="76"/>
-      <c r="J19" s="76"/>
-      <c r="K19" s="76"/>
-      <c r="L19" s="76"/>
-      <c r="M19" s="76"/>
-      <c r="N19" s="76"/>
-      <c r="O19" s="76"/>
-      <c r="P19" s="76"/>
-      <c r="Q19" s="76"/>
-      <c r="R19" s="76"/>
-      <c r="S19" s="76"/>
-      <c r="T19" s="76"/>
-      <c r="U19" s="76"/>
-      <c r="V19" s="76"/>
-      <c r="W19" s="76"/>
-      <c r="X19" s="76"/>
-      <c r="Y19" s="76"/>
-      <c r="Z19" s="76"/>
-      <c r="AA19" s="76"/>
-      <c r="AB19" s="76"/>
-      <c r="AC19" s="76"/>
+      <c r="A19" s="95"/>
+      <c r="B19" s="95"/>
+      <c r="C19" s="95"/>
+      <c r="D19" s="95"/>
+      <c r="E19" s="95"/>
+      <c r="F19" s="95"/>
+      <c r="G19" s="95"/>
+      <c r="H19" s="95"/>
+      <c r="I19" s="95"/>
+      <c r="J19" s="95"/>
+      <c r="K19" s="95"/>
+      <c r="L19" s="95"/>
+      <c r="M19" s="95"/>
+      <c r="N19" s="95"/>
+      <c r="O19" s="95"/>
+      <c r="P19" s="95"/>
+      <c r="Q19" s="95"/>
+      <c r="R19" s="95"/>
+      <c r="S19" s="95"/>
+      <c r="T19" s="95"/>
+      <c r="U19" s="95"/>
+      <c r="V19" s="95"/>
+      <c r="W19" s="95"/>
+      <c r="X19" s="95"/>
+      <c r="Y19" s="95"/>
+      <c r="Z19" s="95"/>
+      <c r="AA19" s="93"/>
+      <c r="AB19" s="93"/>
+      <c r="AC19" s="93"/>
+      <c r="AD19" s="57"/>
+      <c r="AE19" s="94"/>
+      <c r="AF19" s="57"/>
+      <c r="AG19" s="57"/>
+      <c r="AH19" s="57"/>
+      <c r="AI19" s="58"/>
+      <c r="AJ19" s="58"/>
+      <c r="AK19" s="58"/>
+      <c r="AL19" s="57"/>
+      <c r="AM19" s="57"/>
+      <c r="AN19" s="57"/>
+      <c r="AO19" s="57"/>
+      <c r="AP19" s="57"/>
+      <c r="AQ19" s="57"/>
+      <c r="AR19" s="57"/>
+      <c r="AS19" s="57"/>
+      <c r="AT19" s="57"/>
+      <c r="AU19" s="57"/>
+      <c r="AV19" s="57"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="76"/>
-      <c r="B20" s="76"/>
-      <c r="C20" s="76"/>
-      <c r="D20" s="76"/>
-      <c r="E20" s="76"/>
-      <c r="F20" s="76"/>
-      <c r="G20" s="76"/>
-      <c r="H20" s="76"/>
-      <c r="I20" s="76"/>
-      <c r="J20" s="76"/>
-      <c r="K20" s="76"/>
-      <c r="L20" s="76"/>
-      <c r="M20" s="76"/>
-      <c r="N20" s="76"/>
-      <c r="O20" s="76"/>
-      <c r="P20" s="76"/>
-      <c r="Q20" s="76"/>
-      <c r="R20" s="76"/>
-      <c r="S20" s="76"/>
-      <c r="T20" s="76"/>
-      <c r="U20" s="76"/>
-      <c r="V20" s="76"/>
-      <c r="W20" s="76"/>
-      <c r="X20" s="76"/>
-      <c r="Y20" s="76"/>
-      <c r="Z20" s="76"/>
-      <c r="AA20" s="76"/>
-      <c r="AB20" s="76"/>
-      <c r="AC20" s="76"/>
+      <c r="A20" s="95"/>
+      <c r="B20" s="95"/>
+      <c r="C20" s="95"/>
+      <c r="D20" s="95"/>
+      <c r="E20" s="95"/>
+      <c r="F20" s="95"/>
+      <c r="G20" s="95"/>
+      <c r="H20" s="95"/>
+      <c r="I20" s="95"/>
+      <c r="J20" s="95"/>
+      <c r="K20" s="95"/>
+      <c r="L20" s="95"/>
+      <c r="M20" s="95"/>
+      <c r="N20" s="95"/>
+      <c r="O20" s="95"/>
+      <c r="P20" s="95"/>
+      <c r="Q20" s="95"/>
+      <c r="R20" s="95"/>
+      <c r="S20" s="95"/>
+      <c r="T20" s="95"/>
+      <c r="U20" s="95"/>
+      <c r="V20" s="95"/>
+      <c r="W20" s="95"/>
+      <c r="X20" s="95"/>
+      <c r="Y20" s="95"/>
+      <c r="Z20" s="95"/>
+      <c r="AA20" s="93"/>
+      <c r="AB20" s="93"/>
+      <c r="AC20" s="93"/>
+      <c r="AD20" s="57"/>
+      <c r="AE20" s="94"/>
+      <c r="AF20" s="57"/>
+      <c r="AG20" s="57"/>
+      <c r="AH20" s="57"/>
+      <c r="AI20" s="58"/>
+      <c r="AJ20" s="58"/>
+      <c r="AK20" s="58"/>
+      <c r="AL20" s="57"/>
+      <c r="AM20" s="57"/>
+      <c r="AN20" s="57"/>
+      <c r="AO20" s="57"/>
+      <c r="AP20" s="57"/>
+      <c r="AQ20" s="57"/>
+      <c r="AR20" s="57"/>
+      <c r="AS20" s="57"/>
+      <c r="AT20" s="57"/>
+      <c r="AU20" s="57"/>
+      <c r="AV20" s="57"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="82"/>
-      <c r="B21" s="82"/>
-      <c r="C21" s="76"/>
-      <c r="D21" s="82"/>
-      <c r="E21" s="82"/>
-      <c r="F21" s="82"/>
-      <c r="G21" s="82"/>
-      <c r="H21" s="82"/>
-      <c r="I21" s="82"/>
-      <c r="J21" s="82"/>
-      <c r="K21" s="82"/>
-      <c r="L21" s="82"/>
-      <c r="M21" s="82"/>
-      <c r="N21" s="82"/>
-      <c r="O21" s="82"/>
-      <c r="P21" s="82"/>
-      <c r="Q21" s="82"/>
-      <c r="R21" s="82"/>
-      <c r="S21" s="82"/>
-      <c r="T21" s="82"/>
-      <c r="U21" s="82"/>
-      <c r="V21" s="82"/>
-      <c r="W21" s="82"/>
-      <c r="X21" s="82"/>
-      <c r="Y21" s="82"/>
-      <c r="Z21" s="82"/>
-      <c r="AA21" s="82"/>
-      <c r="AB21" s="82"/>
-      <c r="AC21" s="82"/>
+      <c r="A21" s="98"/>
+      <c r="B21" s="98"/>
+      <c r="C21" s="95"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="98"/>
+      <c r="F21" s="98"/>
+      <c r="G21" s="98"/>
+      <c r="H21" s="98"/>
+      <c r="I21" s="98"/>
+      <c r="J21" s="98"/>
+      <c r="K21" s="98"/>
+      <c r="L21" s="98"/>
+      <c r="M21" s="98"/>
+      <c r="N21" s="98"/>
+      <c r="O21" s="98"/>
+      <c r="P21" s="98"/>
+      <c r="Q21" s="98"/>
+      <c r="R21" s="98"/>
+      <c r="S21" s="98"/>
+      <c r="T21" s="98"/>
+      <c r="U21" s="98"/>
+      <c r="V21" s="98"/>
+      <c r="W21" s="98"/>
+      <c r="X21" s="98"/>
+      <c r="Y21" s="98"/>
+      <c r="Z21" s="98"/>
+      <c r="AA21" s="99"/>
+      <c r="AB21" s="99"/>
+      <c r="AC21" s="99"/>
+      <c r="AD21" s="57"/>
+      <c r="AE21" s="94"/>
+      <c r="AF21" s="57"/>
+      <c r="AG21" s="57"/>
+      <c r="AH21" s="57"/>
+      <c r="AI21" s="58"/>
+      <c r="AJ21" s="58"/>
+      <c r="AK21" s="58"/>
+      <c r="AL21" s="57"/>
+      <c r="AM21" s="57"/>
+      <c r="AN21" s="57"/>
+      <c r="AO21" s="57"/>
+      <c r="AP21" s="57"/>
+      <c r="AQ21" s="57"/>
+      <c r="AR21" s="57"/>
+      <c r="AS21" s="57"/>
+      <c r="AT21" s="57"/>
+      <c r="AU21" s="57"/>
+      <c r="AV21" s="57"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="82"/>
-      <c r="B22" s="82"/>
-      <c r="C22" s="76"/>
-      <c r="D22" s="82"/>
-      <c r="E22" s="82"/>
-      <c r="F22" s="82"/>
-      <c r="G22" s="82"/>
-      <c r="H22" s="82"/>
-      <c r="I22" s="82"/>
-      <c r="J22" s="82"/>
-      <c r="K22" s="82"/>
-      <c r="L22" s="82"/>
-      <c r="M22" s="82"/>
-      <c r="N22" s="82"/>
-      <c r="O22" s="82"/>
-      <c r="P22" s="82"/>
-      <c r="Q22" s="82"/>
-      <c r="R22" s="82"/>
-      <c r="S22" s="82"/>
-      <c r="T22" s="82"/>
-      <c r="U22" s="82"/>
-      <c r="V22" s="82"/>
-      <c r="W22" s="82"/>
-      <c r="X22" s="82"/>
-      <c r="Y22" s="82"/>
-      <c r="Z22" s="82"/>
-      <c r="AA22" s="82"/>
-      <c r="AB22" s="82"/>
-      <c r="AC22" s="82"/>
+      <c r="A22" s="98"/>
+      <c r="B22" s="98"/>
+      <c r="C22" s="95"/>
+      <c r="D22" s="98"/>
+      <c r="E22" s="98"/>
+      <c r="F22" s="98"/>
+      <c r="G22" s="98"/>
+      <c r="H22" s="98"/>
+      <c r="I22" s="98"/>
+      <c r="J22" s="98"/>
+      <c r="K22" s="98"/>
+      <c r="L22" s="98"/>
+      <c r="M22" s="98"/>
+      <c r="N22" s="98"/>
+      <c r="O22" s="98"/>
+      <c r="P22" s="98"/>
+      <c r="Q22" s="98"/>
+      <c r="R22" s="98"/>
+      <c r="S22" s="98"/>
+      <c r="T22" s="98"/>
+      <c r="U22" s="98"/>
+      <c r="V22" s="98"/>
+      <c r="W22" s="98"/>
+      <c r="X22" s="98"/>
+      <c r="Y22" s="98"/>
+      <c r="Z22" s="98"/>
+      <c r="AA22" s="99"/>
+      <c r="AB22" s="99"/>
+      <c r="AC22" s="99"/>
+      <c r="AD22" s="57"/>
+      <c r="AE22" s="94"/>
+      <c r="AF22" s="57"/>
+      <c r="AG22" s="57"/>
+      <c r="AH22" s="57"/>
+      <c r="AI22" s="58"/>
+      <c r="AJ22" s="58"/>
+      <c r="AK22" s="58"/>
+      <c r="AL22" s="57"/>
+      <c r="AM22" s="57"/>
+      <c r="AN22" s="57"/>
+      <c r="AO22" s="57"/>
+      <c r="AP22" s="57"/>
+      <c r="AQ22" s="57"/>
+      <c r="AR22" s="57"/>
+      <c r="AS22" s="57"/>
+      <c r="AT22" s="57"/>
+      <c r="AU22" s="57"/>
+      <c r="AV22" s="57"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="82"/>
-      <c r="B23" s="82"/>
-      <c r="C23" s="76"/>
-      <c r="D23" s="82"/>
-      <c r="E23" s="82"/>
-      <c r="F23" s="82"/>
-      <c r="G23" s="82"/>
-      <c r="H23" s="82"/>
-      <c r="I23" s="82"/>
-      <c r="J23" s="82"/>
-      <c r="K23" s="82"/>
-      <c r="L23" s="82"/>
-      <c r="M23" s="82"/>
-      <c r="N23" s="82"/>
-      <c r="O23" s="82"/>
-      <c r="P23" s="82"/>
-      <c r="Q23" s="82"/>
-      <c r="R23" s="82"/>
-      <c r="S23" s="82"/>
-      <c r="T23" s="82"/>
-      <c r="U23" s="82"/>
-      <c r="V23" s="82"/>
-      <c r="W23" s="82"/>
-      <c r="X23" s="82"/>
-      <c r="Y23" s="82"/>
-      <c r="Z23" s="82"/>
-      <c r="AA23" s="82"/>
-      <c r="AB23" s="82"/>
-      <c r="AC23" s="82"/>
+      <c r="A23" s="98"/>
+      <c r="B23" s="98"/>
+      <c r="C23" s="95"/>
+      <c r="D23" s="98"/>
+      <c r="E23" s="98"/>
+      <c r="F23" s="98"/>
+      <c r="G23" s="98"/>
+      <c r="H23" s="98"/>
+      <c r="I23" s="98"/>
+      <c r="J23" s="98"/>
+      <c r="K23" s="98"/>
+      <c r="L23" s="98"/>
+      <c r="M23" s="98"/>
+      <c r="N23" s="98"/>
+      <c r="O23" s="98"/>
+      <c r="P23" s="98"/>
+      <c r="Q23" s="98"/>
+      <c r="R23" s="98"/>
+      <c r="S23" s="98"/>
+      <c r="T23" s="98"/>
+      <c r="U23" s="98"/>
+      <c r="V23" s="98"/>
+      <c r="W23" s="98"/>
+      <c r="X23" s="98"/>
+      <c r="Y23" s="98"/>
+      <c r="Z23" s="98"/>
+      <c r="AA23" s="99"/>
+      <c r="AB23" s="99"/>
+      <c r="AC23" s="99"/>
+      <c r="AD23" s="57"/>
+      <c r="AE23" s="94"/>
+      <c r="AF23" s="57"/>
+      <c r="AG23" s="57"/>
+      <c r="AH23" s="57"/>
+      <c r="AI23" s="58"/>
+      <c r="AJ23" s="58"/>
+      <c r="AK23" s="58"/>
+      <c r="AL23" s="57"/>
+      <c r="AM23" s="57"/>
+      <c r="AN23" s="57"/>
+      <c r="AO23" s="57"/>
+      <c r="AP23" s="57"/>
+      <c r="AQ23" s="57"/>
+      <c r="AR23" s="57"/>
+      <c r="AS23" s="57"/>
+      <c r="AT23" s="57"/>
+      <c r="AU23" s="57"/>
+      <c r="AV23" s="57"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="82"/>
-      <c r="B24" s="82"/>
-      <c r="C24" s="76"/>
-      <c r="D24" s="82"/>
-      <c r="E24" s="82"/>
-      <c r="F24" s="82"/>
-      <c r="G24" s="82"/>
-      <c r="H24" s="82"/>
-      <c r="I24" s="82"/>
-      <c r="J24" s="82"/>
-      <c r="K24" s="82"/>
-      <c r="L24" s="82"/>
-      <c r="M24" s="82"/>
-      <c r="N24" s="82"/>
-      <c r="O24" s="82"/>
-      <c r="P24" s="82"/>
-      <c r="Q24" s="82"/>
-      <c r="R24" s="82"/>
-      <c r="S24" s="82"/>
-      <c r="T24" s="82"/>
-      <c r="U24" s="82"/>
-      <c r="V24" s="82"/>
-      <c r="W24" s="82"/>
-      <c r="X24" s="82"/>
-      <c r="Y24" s="82"/>
-      <c r="Z24" s="82"/>
-      <c r="AA24" s="82"/>
-      <c r="AB24" s="82"/>
-      <c r="AC24" s="82"/>
+      <c r="A24" s="98"/>
+      <c r="B24" s="98"/>
+      <c r="C24" s="95"/>
+      <c r="D24" s="98"/>
+      <c r="E24" s="98"/>
+      <c r="F24" s="98"/>
+      <c r="G24" s="98"/>
+      <c r="H24" s="98"/>
+      <c r="I24" s="98"/>
+      <c r="J24" s="98"/>
+      <c r="K24" s="98"/>
+      <c r="L24" s="98"/>
+      <c r="M24" s="98"/>
+      <c r="N24" s="98"/>
+      <c r="O24" s="98"/>
+      <c r="P24" s="98"/>
+      <c r="Q24" s="98"/>
+      <c r="R24" s="98"/>
+      <c r="S24" s="98"/>
+      <c r="T24" s="98"/>
+      <c r="U24" s="98"/>
+      <c r="V24" s="98"/>
+      <c r="W24" s="98"/>
+      <c r="X24" s="98"/>
+      <c r="Y24" s="98"/>
+      <c r="Z24" s="98"/>
+      <c r="AA24" s="99"/>
+      <c r="AB24" s="99"/>
+      <c r="AC24" s="99"/>
+      <c r="AD24" s="57"/>
+      <c r="AE24" s="94"/>
+      <c r="AF24" s="57"/>
+      <c r="AG24" s="57"/>
+      <c r="AH24" s="57"/>
+      <c r="AI24" s="58"/>
+      <c r="AJ24" s="58"/>
+      <c r="AK24" s="58"/>
+      <c r="AL24" s="57"/>
+      <c r="AM24" s="57"/>
+      <c r="AN24" s="57"/>
+      <c r="AO24" s="57"/>
+      <c r="AP24" s="57"/>
+      <c r="AQ24" s="57"/>
+      <c r="AR24" s="57"/>
+      <c r="AS24" s="57"/>
+      <c r="AT24" s="57"/>
+      <c r="AU24" s="57"/>
+      <c r="AV24" s="57"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="82"/>
-      <c r="B25" s="82"/>
-      <c r="C25" s="76"/>
-      <c r="D25" s="82"/>
-      <c r="E25" s="82"/>
-      <c r="F25" s="82"/>
-      <c r="G25" s="82"/>
-      <c r="H25" s="82"/>
-      <c r="I25" s="82"/>
-      <c r="J25" s="82"/>
-      <c r="K25" s="82"/>
-      <c r="L25" s="82"/>
-      <c r="M25" s="82"/>
-      <c r="N25" s="82"/>
-      <c r="O25" s="82"/>
-      <c r="P25" s="82"/>
-      <c r="Q25" s="82"/>
-      <c r="R25" s="82"/>
-      <c r="S25" s="82"/>
-      <c r="T25" s="82"/>
-      <c r="U25" s="82"/>
-      <c r="V25" s="82"/>
-      <c r="W25" s="82"/>
-      <c r="X25" s="82"/>
-      <c r="Y25" s="82"/>
-      <c r="Z25" s="82"/>
-      <c r="AA25" s="82"/>
-      <c r="AB25" s="82"/>
-      <c r="AC25" s="82"/>
+      <c r="A25" s="98"/>
+      <c r="B25" s="98"/>
+      <c r="C25" s="95"/>
+      <c r="D25" s="98"/>
+      <c r="E25" s="98"/>
+      <c r="F25" s="98"/>
+      <c r="G25" s="98"/>
+      <c r="H25" s="98"/>
+      <c r="I25" s="98"/>
+      <c r="J25" s="98"/>
+      <c r="K25" s="98"/>
+      <c r="L25" s="98"/>
+      <c r="M25" s="98"/>
+      <c r="N25" s="98"/>
+      <c r="O25" s="98"/>
+      <c r="P25" s="98"/>
+      <c r="Q25" s="98"/>
+      <c r="R25" s="98"/>
+      <c r="S25" s="98"/>
+      <c r="T25" s="98"/>
+      <c r="U25" s="98"/>
+      <c r="V25" s="98"/>
+      <c r="W25" s="98"/>
+      <c r="X25" s="98"/>
+      <c r="Y25" s="98"/>
+      <c r="Z25" s="98"/>
+      <c r="AA25" s="99"/>
+      <c r="AB25" s="99"/>
+      <c r="AC25" s="99"/>
+      <c r="AD25" s="57"/>
+      <c r="AE25" s="94"/>
+      <c r="AF25" s="57"/>
+      <c r="AG25" s="57"/>
+      <c r="AH25" s="57"/>
+      <c r="AI25" s="58"/>
+      <c r="AJ25" s="58"/>
+      <c r="AK25" s="58"/>
+      <c r="AL25" s="57"/>
+      <c r="AM25" s="57"/>
+      <c r="AN25" s="57"/>
+      <c r="AO25" s="57"/>
+      <c r="AP25" s="57"/>
+      <c r="AQ25" s="57"/>
+      <c r="AR25" s="57"/>
+      <c r="AS25" s="57"/>
+      <c r="AT25" s="57"/>
+      <c r="AU25" s="57"/>
+      <c r="AV25" s="57"/>
+    </row>
+    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA26" s="94"/>
+      <c r="AB26" s="94"/>
+      <c r="AC26" s="94"/>
+      <c r="AD26" s="57"/>
+      <c r="AE26" s="94"/>
+      <c r="AF26" s="57"/>
+      <c r="AG26" s="57"/>
+      <c r="AH26" s="57"/>
+      <c r="AI26" s="58"/>
+      <c r="AJ26" s="58"/>
+      <c r="AK26" s="58"/>
+      <c r="AL26" s="57"/>
+      <c r="AM26" s="57"/>
+      <c r="AN26" s="57"/>
+      <c r="AO26" s="57"/>
+      <c r="AP26" s="57"/>
+      <c r="AQ26" s="57"/>
+      <c r="AR26" s="57"/>
+      <c r="AS26" s="57"/>
+      <c r="AT26" s="57"/>
+      <c r="AU26" s="57"/>
+      <c r="AV26" s="57"/>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA27" s="94"/>
+      <c r="AB27" s="94"/>
+      <c r="AC27" s="94"/>
+      <c r="AD27" s="57"/>
+      <c r="AE27" s="94"/>
+      <c r="AF27" s="57"/>
+      <c r="AG27" s="57"/>
+      <c r="AH27" s="57"/>
+      <c r="AI27" s="58"/>
+      <c r="AJ27" s="58"/>
+      <c r="AK27" s="58"/>
+      <c r="AL27" s="57"/>
+      <c r="AM27" s="57"/>
+      <c r="AN27" s="57"/>
+      <c r="AO27" s="57"/>
+      <c r="AP27" s="57"/>
+      <c r="AQ27" s="57"/>
+      <c r="AR27" s="57"/>
+      <c r="AS27" s="57"/>
+      <c r="AT27" s="57"/>
+      <c r="AU27" s="57"/>
+      <c r="AV27" s="57"/>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA28" s="94"/>
+      <c r="AB28" s="94"/>
+      <c r="AC28" s="94"/>
+      <c r="AD28" s="57"/>
+      <c r="AE28" s="94"/>
+      <c r="AF28" s="57"/>
+      <c r="AG28" s="57"/>
+      <c r="AH28" s="57"/>
+      <c r="AI28" s="58"/>
+      <c r="AJ28" s="58"/>
+      <c r="AK28" s="58"/>
+      <c r="AL28" s="57"/>
+      <c r="AM28" s="57"/>
+      <c r="AN28" s="57"/>
+      <c r="AO28" s="57"/>
+      <c r="AP28" s="57"/>
+      <c r="AQ28" s="57"/>
+      <c r="AR28" s="57"/>
+      <c r="AS28" s="57"/>
+      <c r="AT28" s="57"/>
+      <c r="AU28" s="57"/>
+      <c r="AV28" s="57"/>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA29" s="94"/>
+      <c r="AB29" s="94"/>
+      <c r="AC29" s="94"/>
+      <c r="AD29" s="57"/>
+      <c r="AE29" s="94"/>
+      <c r="AF29" s="57"/>
+      <c r="AG29" s="57"/>
+      <c r="AH29" s="57"/>
+      <c r="AI29" s="58"/>
+      <c r="AJ29" s="58"/>
+      <c r="AK29" s="58"/>
+      <c r="AL29" s="57"/>
+      <c r="AM29" s="57"/>
+      <c r="AN29" s="57"/>
+      <c r="AO29" s="57"/>
+      <c r="AP29" s="57"/>
+      <c r="AQ29" s="57"/>
+      <c r="AR29" s="57"/>
+      <c r="AS29" s="57"/>
+      <c r="AT29" s="57"/>
+      <c r="AU29" s="57"/>
+      <c r="AV29" s="57"/>
+    </row>
+    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA30" s="94"/>
+      <c r="AB30" s="94"/>
+      <c r="AC30" s="94"/>
+      <c r="AD30" s="57"/>
+      <c r="AE30" s="94"/>
+      <c r="AF30" s="57"/>
+      <c r="AG30" s="57"/>
+      <c r="AH30" s="57"/>
+      <c r="AI30" s="58"/>
+      <c r="AJ30" s="58"/>
+      <c r="AK30" s="58"/>
+      <c r="AL30" s="57"/>
+      <c r="AM30" s="57"/>
+      <c r="AN30" s="57"/>
+      <c r="AO30" s="57"/>
+      <c r="AP30" s="57"/>
+      <c r="AQ30" s="57"/>
+      <c r="AR30" s="57"/>
+      <c r="AS30" s="57"/>
+      <c r="AT30" s="57"/>
+      <c r="AU30" s="57"/>
+      <c r="AV30" s="57"/>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA31" s="94"/>
+      <c r="AB31" s="94"/>
+      <c r="AC31" s="94"/>
+      <c r="AD31" s="57"/>
+      <c r="AE31" s="94"/>
+      <c r="AF31" s="57"/>
+      <c r="AG31" s="57"/>
+      <c r="AH31" s="57"/>
+      <c r="AI31" s="58"/>
+      <c r="AJ31" s="58"/>
+      <c r="AK31" s="58"/>
+      <c r="AL31" s="57"/>
+      <c r="AM31" s="57"/>
+      <c r="AN31" s="57"/>
+      <c r="AO31" s="57"/>
+      <c r="AP31" s="57"/>
+      <c r="AQ31" s="57"/>
+      <c r="AR31" s="57"/>
+      <c r="AS31" s="57"/>
+      <c r="AT31" s="57"/>
+      <c r="AU31" s="57"/>
+      <c r="AV31" s="57"/>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA32" s="94"/>
+      <c r="AB32" s="94"/>
+      <c r="AC32" s="94"/>
+      <c r="AD32" s="57"/>
+      <c r="AE32" s="94"/>
+      <c r="AF32" s="57"/>
+      <c r="AG32" s="57"/>
+      <c r="AH32" s="57"/>
+      <c r="AI32" s="58"/>
+      <c r="AJ32" s="58"/>
+      <c r="AK32" s="58"/>
+      <c r="AL32" s="57"/>
+      <c r="AM32" s="57"/>
+      <c r="AN32" s="57"/>
+      <c r="AO32" s="57"/>
+      <c r="AP32" s="57"/>
+      <c r="AQ32" s="57"/>
+      <c r="AR32" s="57"/>
+      <c r="AS32" s="57"/>
+      <c r="AT32" s="57"/>
+      <c r="AU32" s="57"/>
+      <c r="AV32" s="57"/>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA33" s="94"/>
+      <c r="AB33" s="94"/>
+      <c r="AC33" s="94"/>
+      <c r="AD33" s="57"/>
+      <c r="AE33" s="94"/>
+      <c r="AF33" s="57"/>
+      <c r="AG33" s="57"/>
+      <c r="AH33" s="57"/>
+      <c r="AI33" s="58"/>
+      <c r="AJ33" s="58"/>
+      <c r="AK33" s="58"/>
+      <c r="AL33" s="57"/>
+      <c r="AM33" s="57"/>
+      <c r="AN33" s="57"/>
+      <c r="AO33" s="57"/>
+      <c r="AP33" s="57"/>
+      <c r="AQ33" s="57"/>
+      <c r="AR33" s="57"/>
+      <c r="AS33" s="57"/>
+      <c r="AT33" s="57"/>
+      <c r="AU33" s="57"/>
+      <c r="AV33" s="57"/>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA34" s="94"/>
+      <c r="AB34" s="94"/>
+      <c r="AC34" s="94"/>
+      <c r="AD34" s="57"/>
+      <c r="AE34" s="94"/>
+      <c r="AF34" s="57"/>
+      <c r="AG34" s="57"/>
+      <c r="AH34" s="57"/>
+      <c r="AI34" s="58"/>
+      <c r="AJ34" s="58"/>
+      <c r="AK34" s="58"/>
+      <c r="AL34" s="57"/>
+      <c r="AM34" s="57"/>
+      <c r="AN34" s="57"/>
+      <c r="AO34" s="57"/>
+      <c r="AP34" s="57"/>
+      <c r="AQ34" s="57"/>
+      <c r="AR34" s="57"/>
+      <c r="AS34" s="57"/>
+      <c r="AT34" s="57"/>
+      <c r="AU34" s="57"/>
+      <c r="AV34" s="57"/>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA35" s="94"/>
+      <c r="AB35" s="94"/>
+      <c r="AC35" s="94"/>
+      <c r="AD35" s="57"/>
+      <c r="AE35" s="94"/>
+      <c r="AF35" s="57"/>
+      <c r="AG35" s="57"/>
+      <c r="AH35" s="57"/>
+      <c r="AI35" s="58"/>
+      <c r="AJ35" s="58"/>
+      <c r="AK35" s="58"/>
+      <c r="AL35" s="57"/>
+      <c r="AM35" s="57"/>
+      <c r="AN35" s="57"/>
+      <c r="AO35" s="57"/>
+      <c r="AP35" s="57"/>
+      <c r="AQ35" s="57"/>
+      <c r="AR35" s="57"/>
+      <c r="AS35" s="57"/>
+      <c r="AT35" s="57"/>
+      <c r="AU35" s="57"/>
+      <c r="AV35" s="57"/>
+    </row>
+    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA36" s="94"/>
+      <c r="AB36" s="94"/>
+      <c r="AC36" s="94"/>
+      <c r="AD36" s="57"/>
+      <c r="AE36" s="94"/>
+      <c r="AF36" s="57"/>
+      <c r="AG36" s="57"/>
+      <c r="AH36" s="57"/>
+      <c r="AI36" s="58"/>
+      <c r="AJ36" s="58"/>
+      <c r="AK36" s="58"/>
+      <c r="AL36" s="57"/>
+      <c r="AM36" s="57"/>
+      <c r="AN36" s="57"/>
+      <c r="AO36" s="57"/>
+      <c r="AP36" s="57"/>
+      <c r="AQ36" s="57"/>
+      <c r="AR36" s="57"/>
+      <c r="AS36" s="57"/>
+      <c r="AT36" s="57"/>
+      <c r="AU36" s="57"/>
+      <c r="AV36" s="57"/>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA37" s="94"/>
+      <c r="AB37" s="94"/>
+      <c r="AC37" s="94"/>
+      <c r="AD37" s="57"/>
+      <c r="AE37" s="94"/>
+      <c r="AF37" s="57"/>
+      <c r="AG37" s="57"/>
+      <c r="AH37" s="57"/>
+      <c r="AI37" s="58"/>
+      <c r="AJ37" s="58"/>
+      <c r="AK37" s="58"/>
+      <c r="AL37" s="57"/>
+      <c r="AM37" s="57"/>
+      <c r="AN37" s="57"/>
+      <c r="AO37" s="57"/>
+      <c r="AP37" s="57"/>
+      <c r="AQ37" s="57"/>
+      <c r="AR37" s="57"/>
+      <c r="AS37" s="57"/>
+      <c r="AT37" s="57"/>
+      <c r="AU37" s="57"/>
+      <c r="AV37" s="57"/>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA38" s="94"/>
+      <c r="AB38" s="94"/>
+      <c r="AC38" s="94"/>
+      <c r="AD38" s="57"/>
+      <c r="AE38" s="94"/>
+      <c r="AF38" s="57"/>
+      <c r="AG38" s="57"/>
+      <c r="AH38" s="57"/>
+      <c r="AI38" s="58"/>
+      <c r="AJ38" s="58"/>
+      <c r="AK38" s="58"/>
+      <c r="AL38" s="57"/>
+      <c r="AM38" s="57"/>
+      <c r="AN38" s="57"/>
+      <c r="AO38" s="57"/>
+      <c r="AP38" s="57"/>
+      <c r="AQ38" s="57"/>
+      <c r="AR38" s="57"/>
+      <c r="AS38" s="57"/>
+      <c r="AT38" s="57"/>
+      <c r="AU38" s="57"/>
+      <c r="AV38" s="57"/>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA39" s="94"/>
+      <c r="AB39" s="94"/>
+      <c r="AC39" s="94"/>
+      <c r="AD39" s="57"/>
+      <c r="AE39" s="94"/>
+      <c r="AF39" s="57"/>
+      <c r="AG39" s="57"/>
+      <c r="AH39" s="57"/>
+      <c r="AI39" s="58"/>
+      <c r="AJ39" s="58"/>
+      <c r="AK39" s="58"/>
+      <c r="AL39" s="57"/>
+      <c r="AM39" s="57"/>
+      <c r="AN39" s="57"/>
+      <c r="AO39" s="57"/>
+      <c r="AP39" s="57"/>
+      <c r="AQ39" s="57"/>
+      <c r="AR39" s="57"/>
+      <c r="AS39" s="57"/>
+      <c r="AT39" s="57"/>
+      <c r="AU39" s="57"/>
+      <c r="AV39" s="57"/>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA40" s="94"/>
+      <c r="AB40" s="94"/>
+      <c r="AC40" s="94"/>
+      <c r="AD40" s="57"/>
+      <c r="AE40" s="94"/>
+      <c r="AF40" s="57"/>
+      <c r="AG40" s="57"/>
+      <c r="AH40" s="57"/>
+      <c r="AI40" s="58"/>
+      <c r="AJ40" s="58"/>
+      <c r="AK40" s="58"/>
+      <c r="AL40" s="57"/>
+      <c r="AM40" s="57"/>
+      <c r="AN40" s="57"/>
+      <c r="AO40" s="57"/>
+      <c r="AP40" s="57"/>
+      <c r="AQ40" s="57"/>
+      <c r="AR40" s="57"/>
+      <c r="AS40" s="57"/>
+      <c r="AT40" s="57"/>
+      <c r="AU40" s="57"/>
+      <c r="AV40" s="57"/>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA41" s="94"/>
+      <c r="AB41" s="94"/>
+      <c r="AC41" s="94"/>
+      <c r="AD41" s="57"/>
+      <c r="AE41" s="94"/>
+      <c r="AF41" s="57"/>
+      <c r="AG41" s="57"/>
+      <c r="AH41" s="57"/>
+      <c r="AI41" s="58"/>
+      <c r="AJ41" s="58"/>
+      <c r="AK41" s="58"/>
+      <c r="AL41" s="57"/>
+      <c r="AM41" s="57"/>
+      <c r="AN41" s="57"/>
+      <c r="AO41" s="57"/>
+      <c r="AP41" s="57"/>
+      <c r="AQ41" s="57"/>
+      <c r="AR41" s="57"/>
+      <c r="AS41" s="57"/>
+      <c r="AT41" s="57"/>
+      <c r="AU41" s="57"/>
+      <c r="AV41" s="57"/>
+    </row>
+    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA42" s="94"/>
+      <c r="AB42" s="94"/>
+      <c r="AC42" s="94"/>
+      <c r="AD42" s="57"/>
+      <c r="AE42" s="94"/>
+      <c r="AF42" s="57"/>
+      <c r="AG42" s="57"/>
+      <c r="AH42" s="57"/>
+      <c r="AI42" s="58"/>
+      <c r="AJ42" s="58"/>
+      <c r="AK42" s="58"/>
+      <c r="AL42" s="57"/>
+      <c r="AM42" s="57"/>
+      <c r="AN42" s="57"/>
+      <c r="AO42" s="57"/>
+      <c r="AP42" s="57"/>
+      <c r="AQ42" s="57"/>
+      <c r="AR42" s="57"/>
+      <c r="AS42" s="57"/>
+      <c r="AT42" s="57"/>
+      <c r="AU42" s="57"/>
+      <c r="AV42" s="57"/>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA43" s="94"/>
+      <c r="AB43" s="94"/>
+      <c r="AC43" s="94"/>
+      <c r="AD43" s="57"/>
+      <c r="AE43" s="94"/>
+      <c r="AF43" s="57"/>
+      <c r="AG43" s="57"/>
+      <c r="AH43" s="57"/>
+      <c r="AI43" s="58"/>
+      <c r="AJ43" s="58"/>
+      <c r="AK43" s="58"/>
+      <c r="AL43" s="57"/>
+      <c r="AM43" s="57"/>
+      <c r="AN43" s="57"/>
+      <c r="AO43" s="57"/>
+      <c r="AP43" s="57"/>
+      <c r="AQ43" s="57"/>
+      <c r="AR43" s="57"/>
+      <c r="AS43" s="57"/>
+      <c r="AT43" s="57"/>
+      <c r="AU43" s="57"/>
+      <c r="AV43" s="57"/>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA44" s="94"/>
+      <c r="AB44" s="94"/>
+      <c r="AC44" s="94"/>
+      <c r="AD44" s="57"/>
+      <c r="AE44" s="94"/>
+      <c r="AF44" s="57"/>
+      <c r="AG44" s="57"/>
+      <c r="AH44" s="57"/>
+      <c r="AI44" s="58"/>
+      <c r="AJ44" s="58"/>
+      <c r="AK44" s="58"/>
+      <c r="AL44" s="57"/>
+      <c r="AM44" s="57"/>
+      <c r="AN44" s="57"/>
+      <c r="AO44" s="57"/>
+      <c r="AP44" s="57"/>
+      <c r="AQ44" s="57"/>
+      <c r="AR44" s="57"/>
+      <c r="AS44" s="57"/>
+      <c r="AT44" s="57"/>
+      <c r="AU44" s="57"/>
+      <c r="AV44" s="57"/>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA45" s="94"/>
+      <c r="AB45" s="94"/>
+      <c r="AC45" s="94"/>
+      <c r="AD45" s="57"/>
+      <c r="AE45" s="94"/>
+      <c r="AF45" s="57"/>
+      <c r="AG45" s="57"/>
+      <c r="AH45" s="57"/>
+      <c r="AI45" s="58"/>
+      <c r="AJ45" s="58"/>
+      <c r="AK45" s="58"/>
+      <c r="AL45" s="57"/>
+      <c r="AM45" s="57"/>
+      <c r="AN45" s="57"/>
+      <c r="AO45" s="57"/>
+      <c r="AP45" s="57"/>
+      <c r="AQ45" s="57"/>
+      <c r="AR45" s="57"/>
+      <c r="AS45" s="57"/>
+      <c r="AT45" s="57"/>
+      <c r="AU45" s="57"/>
+      <c r="AV45" s="57"/>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA46" s="94"/>
+      <c r="AB46" s="94"/>
+      <c r="AC46" s="94"/>
+      <c r="AD46" s="57"/>
+      <c r="AE46" s="94"/>
+      <c r="AF46" s="57"/>
+      <c r="AG46" s="57"/>
+      <c r="AH46" s="57"/>
+      <c r="AI46" s="58"/>
+      <c r="AJ46" s="58"/>
+      <c r="AK46" s="58"/>
+      <c r="AL46" s="57"/>
+      <c r="AM46" s="57"/>
+      <c r="AN46" s="57"/>
+      <c r="AO46" s="57"/>
+      <c r="AP46" s="57"/>
+      <c r="AQ46" s="57"/>
+      <c r="AR46" s="57"/>
+      <c r="AS46" s="57"/>
+      <c r="AT46" s="57"/>
+      <c r="AU46" s="57"/>
+      <c r="AV46" s="57"/>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AA47" s="94"/>
+      <c r="AB47" s="94"/>
+      <c r="AC47" s="94"/>
+      <c r="AD47" s="57"/>
+      <c r="AE47" s="94"/>
+      <c r="AF47" s="57"/>
+      <c r="AG47" s="57"/>
+      <c r="AH47" s="57"/>
+      <c r="AI47" s="58"/>
+      <c r="AJ47" s="58"/>
+      <c r="AK47" s="58"/>
+      <c r="AL47" s="57"/>
+      <c r="AM47" s="57"/>
+      <c r="AN47" s="57"/>
+      <c r="AO47" s="57"/>
+      <c r="AP47" s="57"/>
+      <c r="AQ47" s="57"/>
+      <c r="AR47" s="57"/>
+      <c r="AS47" s="57"/>
+      <c r="AT47" s="57"/>
+      <c r="AU47" s="57"/>
+      <c r="AV47" s="57"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -5849,17 +6885,17 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.76953125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.78515625" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="17.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="23.77"/>
@@ -5874,22 +6910,22 @@
       <c r="A1" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="83" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="83" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="83" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="83" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="83" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="83" t="s">
+      <c r="B1" s="100" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="100" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="100" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="100" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="100" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="100" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="4"/>
@@ -5905,22 +6941,22 @@
       <c r="A2" s="30" t="s">
         <v>204</v>
       </c>
-      <c r="B2" s="83" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="83" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="83" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="83" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="83" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="83" t="s">
+      <c r="B2" s="100" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="100" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="100" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="100" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="100" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="100" t="s">
         <v>1</v>
       </c>
       <c r="H2" s="4"/>
@@ -6139,23 +7175,23 @@
       <c r="Q10" s="20"/>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="84" t="s">
+      <c r="A11" s="101" t="s">
         <v>211</v>
       </c>
-      <c r="B11" s="85" t="s">
+      <c r="B11" s="102" t="s">
         <v>212</v>
       </c>
-      <c r="C11" s="84" t="s">
+      <c r="C11" s="101" t="s">
         <v>213</v>
       </c>
-      <c r="D11" s="84" t="s">
+      <c r="D11" s="101" t="s">
         <v>214</v>
       </c>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84" t="s">
+      <c r="E11" s="101"/>
+      <c r="F11" s="101" t="s">
         <v>94</v>
       </c>
-      <c r="G11" s="84" t="s">
+      <c r="G11" s="101" t="s">
         <v>215</v>
       </c>
     </row>
@@ -6196,17 +7232,17 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="51.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="30.83"/>
@@ -6216,7 +7252,7 @@
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="103" t="s">
         <v>203</v>
       </c>
       <c r="B1" s="38" t="s">
@@ -6715,17 +7751,17 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.7578125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.77734375" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="26" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="26" width="25.21"/>
@@ -6738,28 +7774,28 @@
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="104" t="s">
         <v>203</v>
       </c>
-      <c r="B1" s="88" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="88" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="89" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="89" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="89" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="88" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="88" t="s">
+      <c r="B1" s="105" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="105" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="106" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="106" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="106" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="105" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="105" t="s">
         <v>1</v>
       </c>
       <c r="I1" s="12"/>
@@ -6771,28 +7807,28 @@
       <c r="Q1" s="4"/>
     </row>
     <row r="2" s="3" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="89" t="s">
+      <c r="A2" s="106" t="s">
         <v>230</v>
       </c>
-      <c r="B2" s="88" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="88" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="89" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="89" t="s">
-        <v>1</v>
-      </c>
-      <c r="F2" s="89" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="88" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="88" t="s">
+      <c r="B2" s="105" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="105" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="106" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="106" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="106" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="105" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="105" t="s">
         <v>1</v>
       </c>
       <c r="I2" s="12"/>
@@ -7016,24 +8052,24 @@
       <c r="AB8" s="17"/>
     </row>
     <row r="9" s="17" customFormat="true" ht="15.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="90" t="s">
+      <c r="A9" s="107" t="s">
         <v>232</v>
       </c>
-      <c r="B9" s="90" t="s">
+      <c r="B9" s="107" t="s">
         <v>219</v>
       </c>
-      <c r="C9" s="90"/>
-      <c r="D9" s="90"/>
-      <c r="E9" s="90" t="s">
+      <c r="C9" s="107"/>
+      <c r="D9" s="107"/>
+      <c r="E9" s="107" t="s">
         <v>233</v>
       </c>
-      <c r="F9" s="90" t="s">
+      <c r="F9" s="107" t="s">
         <v>234</v>
       </c>
-      <c r="G9" s="90" t="s">
+      <c r="G9" s="107" t="s">
         <v>235</v>
       </c>
-      <c r="H9" s="90" t="s">
+      <c r="H9" s="107" t="s">
         <v>236</v>
       </c>
       <c r="I9" s="10"/>
@@ -7090,33 +8126,33 @@
       <c r="AB10" s="21"/>
     </row>
     <row r="11" s="21" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="91" t="s">
+      <c r="A11" s="108" t="s">
         <v>224</v>
       </c>
-      <c r="B11" s="91" t="s">
+      <c r="B11" s="108" t="s">
         <v>237</v>
       </c>
-      <c r="C11" s="91" t="s">
+      <c r="C11" s="108" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="91" t="s">
+      <c r="D11" s="108" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="91" t="s">
+      <c r="E11" s="108" t="s">
         <v>238</v>
       </c>
-      <c r="F11" s="91" t="s">
+      <c r="F11" s="108" t="s">
         <v>239</v>
       </c>
-      <c r="G11" s="91" t="s">
+      <c r="G11" s="108" t="s">
         <v>240</v>
       </c>
-      <c r="H11" s="91" t="s">
+      <c r="H11" s="108" t="s">
         <v>241</v>
       </c>
-      <c r="I11" s="89"/>
-      <c r="J11" s="89"/>
-      <c r="K11" s="89"/>
+      <c r="I11" s="106"/>
+      <c r="J11" s="106"/>
+      <c r="K11" s="106"/>
       <c r="L11" s="26"/>
       <c r="M11" s="26"/>
       <c r="N11" s="26"/>
@@ -7139,88 +8175,88 @@
       <c r="A12" s="25" t="s">
         <v>242</v>
       </c>
-      <c r="B12" s="92"/>
-      <c r="C12" s="93" t="s">
+      <c r="B12" s="109"/>
+      <c r="C12" s="110" t="s">
         <v>243</v>
       </c>
-      <c r="D12" s="93" t="s">
+      <c r="D12" s="110" t="s">
         <v>244</v>
       </c>
-      <c r="E12" s="94"/>
+      <c r="E12" s="111"/>
       <c r="F12" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="G12" s="94"/>
-      <c r="H12" s="94"/>
-      <c r="I12" s="89"/>
-      <c r="J12" s="89"/>
-      <c r="K12" s="89"/>
+      <c r="G12" s="111"/>
+      <c r="H12" s="111"/>
+      <c r="I12" s="106"/>
+      <c r="J12" s="106"/>
+      <c r="K12" s="106"/>
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="25" t="s">
         <v>245</v>
       </c>
-      <c r="B13" s="92"/>
-      <c r="C13" s="93" t="s">
+      <c r="B13" s="109"/>
+      <c r="C13" s="110" t="s">
         <v>243</v>
       </c>
-      <c r="D13" s="93" t="s">
+      <c r="D13" s="110" t="s">
         <v>246</v>
       </c>
-      <c r="E13" s="94"/>
+      <c r="E13" s="111"/>
       <c r="F13" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="G13" s="94"/>
-      <c r="H13" s="94"/>
-      <c r="I13" s="89"/>
-      <c r="J13" s="89"/>
-      <c r="K13" s="89"/>
+      <c r="G13" s="111"/>
+      <c r="H13" s="111"/>
+      <c r="I13" s="106"/>
+      <c r="J13" s="106"/>
+      <c r="K13" s="106"/>
     </row>
     <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="25" t="s">
         <v>247</v>
       </c>
-      <c r="B14" s="92"/>
-      <c r="C14" s="93" t="s">
+      <c r="B14" s="109"/>
+      <c r="C14" s="110" t="s">
         <v>243</v>
       </c>
-      <c r="D14" s="93" t="s">
+      <c r="D14" s="110" t="s">
         <v>248</v>
       </c>
-      <c r="E14" s="94"/>
+      <c r="E14" s="111"/>
       <c r="F14" s="25" t="n">
         <v>3</v>
       </c>
-      <c r="G14" s="94"/>
-      <c r="H14" s="94"/>
-      <c r="I14" s="88"/>
-      <c r="J14" s="88"/>
-      <c r="K14" s="88"/>
+      <c r="G14" s="111"/>
+      <c r="H14" s="111"/>
+      <c r="I14" s="105"/>
+      <c r="J14" s="105"/>
+      <c r="K14" s="105"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D15" s="26"/>
       <c r="E15" s="26"/>
       <c r="F15" s="26"/>
-      <c r="I15" s="88"/>
-      <c r="J15" s="88"/>
-      <c r="K15" s="88"/>
+      <c r="I15" s="105"/>
+      <c r="J15" s="105"/>
+      <c r="K15" s="105"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D16" s="26"/>
       <c r="E16" s="26"/>
       <c r="F16" s="26"/>
-      <c r="I16" s="88"/>
-      <c r="J16" s="88"/>
-      <c r="K16" s="88"/>
+      <c r="I16" s="105"/>
+      <c r="J16" s="105"/>
+      <c r="K16" s="105"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D17" s="26"/>
       <c r="E17" s="26"/>
       <c r="F17" s="26"/>
-      <c r="I17" s="88"/>
-      <c r="J17" s="88"/>
-      <c r="K17" s="88"/>
+      <c r="I17" s="105"/>
+      <c r="J17" s="105"/>
+      <c r="K17" s="105"/>
     </row>
     <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
updated IMEM-CNR excel file
</commit_message>
<xml_diff>
--- a/movpe_CNR/Parma_datafile_nomad.xlsx
+++ b/movpe_CNR/Parma_datafile_nomad.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="264">
   <si>
     <t xml:space="preserve"># COMMENTS:</t>
   </si>
@@ -571,12 +571,12 @@
     <t xml:space="preserve">vent line flow</t>
   </si>
   <si>
+    <t xml:space="preserve">percentage value</t>
+  </si>
+  <si>
     <t xml:space="preserve">Silane  valve open?</t>
   </si>
   <si>
-    <t xml:space="preserve">percentage value</t>
-  </si>
-  <si>
     <t xml:space="preserve">Step</t>
   </si>
   <si>
@@ -632,9 +632,6 @@
   </si>
   <si>
     <t xml:space="preserve">vent flow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Silane valve</t>
   </si>
   <si>
     <t xml:space="preserve">Cylinder pressure</t>
@@ -2355,7 +2352,7 @@
       <c r="D5" s="43"/>
       <c r="E5" s="43"/>
       <c r="F5" s="43" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G5" s="42"/>
       <c r="H5" s="43"/>
@@ -2391,15 +2388,15 @@
         <v>1</v>
       </c>
       <c r="B7" s="42" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C7" s="42"/>
       <c r="D7" s="42"/>
       <c r="E7" s="43" t="s">
+        <v>257</v>
+      </c>
+      <c r="F7" s="43" t="s">
         <v>258</v>
-      </c>
-      <c r="F7" s="43" t="s">
-        <v>259</v>
       </c>
       <c r="G7" s="43"/>
       <c r="H7" s="119"/>
@@ -2445,10 +2442,10 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="124" t="s">
+        <v>259</v>
+      </c>
+      <c r="B9" s="18" t="s">
         <v>260</v>
-      </c>
-      <c r="B9" s="18" t="s">
-        <v>261</v>
       </c>
       <c r="C9" s="18" t="s">
         <v>30</v>
@@ -2457,10 +2454,10 @@
         <v>31</v>
       </c>
       <c r="E9" s="124" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F9" s="124" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G9" s="124"/>
       <c r="H9" s="117"/>
@@ -2471,10 +2468,10 @@
       <c r="A10" s="125"/>
       <c r="B10" s="126"/>
       <c r="C10" s="127" t="s">
+        <v>262</v>
+      </c>
+      <c r="D10" s="127" t="s">
         <v>263</v>
-      </c>
-      <c r="D10" s="127" t="s">
-        <v>264</v>
       </c>
       <c r="E10" s="117"/>
       <c r="F10" s="117"/>
@@ -5169,10 +5166,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:BC47"/>
+  <dimension ref="A1:AMJ47"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M37" activeCellId="0" sqref="M37"/>
+      <selection pane="topLeft" activeCell="AF23" activeCellId="0" sqref="AF23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5204,17 +5201,17 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="58" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="58" width="9.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="58" width="6.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="58" width="7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="32" style="58" width="10"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="58" width="18.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="58" width="17.33"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="37" min="37" style="60" width="11.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="58" width="14.16"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="41" min="39" style="60" width="11.91"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="45" style="60" width="11.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="31" style="58" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="58" width="7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="58" width="18.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="58" width="17.33"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="36" min="36" style="60" width="11.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="58" width="14.16"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="40" min="38" style="60" width="11.91"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1023" min="44" style="60" width="11.91"/>
   </cols>
   <sheetData>
-    <row r="1" s="66" customFormat="true" ht="49.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="66" customFormat="true" ht="60.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
@@ -5254,15 +5251,15 @@
       <c r="AG1" s="61"/>
       <c r="AH1" s="62"/>
       <c r="AI1" s="62"/>
-      <c r="AJ1" s="62"/>
+      <c r="AJ1" s="63"/>
       <c r="AK1" s="63"/>
-      <c r="AL1" s="63"/>
+      <c r="AL1" s="64"/>
       <c r="AM1" s="64"/>
       <c r="AN1" s="64"/>
-      <c r="AO1" s="64"/>
+      <c r="AO1" s="65"/>
       <c r="AP1" s="65"/>
       <c r="AQ1" s="65"/>
-      <c r="AR1" s="65"/>
+      <c r="AR1" s="63"/>
       <c r="AS1" s="63"/>
       <c r="AT1" s="63"/>
       <c r="AU1" s="63"/>
@@ -5273,7 +5270,7 @@
       <c r="AZ1" s="63"/>
       <c r="BA1" s="63"/>
       <c r="BB1" s="63"/>
-      <c r="BC1" s="63"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" s="72" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="67" t="s">
@@ -5313,15 +5310,15 @@
       <c r="AG2" s="67"/>
       <c r="AH2" s="68"/>
       <c r="AI2" s="68"/>
-      <c r="AJ2" s="68"/>
+      <c r="AJ2" s="69"/>
       <c r="AK2" s="69"/>
-      <c r="AL2" s="69"/>
+      <c r="AL2" s="70"/>
       <c r="AM2" s="70"/>
       <c r="AN2" s="70"/>
-      <c r="AO2" s="70"/>
+      <c r="AO2" s="71"/>
       <c r="AP2" s="71"/>
       <c r="AQ2" s="71"/>
-      <c r="AR2" s="71"/>
+      <c r="AR2" s="69"/>
       <c r="AS2" s="69"/>
       <c r="AT2" s="69"/>
       <c r="AU2" s="69"/>
@@ -5332,7 +5329,7 @@
       <c r="AZ2" s="69"/>
       <c r="BA2" s="69"/>
       <c r="BB2" s="69"/>
-      <c r="BC2" s="69"/>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" s="78" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="73" t="s">
@@ -5372,15 +5369,15 @@
       <c r="AG3" s="73"/>
       <c r="AH3" s="74"/>
       <c r="AI3" s="74"/>
-      <c r="AJ3" s="74"/>
+      <c r="AJ3" s="75"/>
       <c r="AK3" s="75"/>
-      <c r="AL3" s="75"/>
+      <c r="AL3" s="76"/>
       <c r="AM3" s="76"/>
       <c r="AN3" s="76"/>
-      <c r="AO3" s="76"/>
+      <c r="AO3" s="77"/>
       <c r="AP3" s="77"/>
       <c r="AQ3" s="77"/>
-      <c r="AR3" s="77"/>
+      <c r="AR3" s="75"/>
       <c r="AS3" s="75"/>
       <c r="AT3" s="75"/>
       <c r="AU3" s="75"/>
@@ -5391,7 +5388,7 @@
       <c r="AZ3" s="75"/>
       <c r="BA3" s="75"/>
       <c r="BB3" s="75"/>
-      <c r="BC3" s="75"/>
+      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" s="83" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="79" t="s">
@@ -5479,25 +5476,25 @@
         <v>10</v>
       </c>
       <c r="AE4" s="82" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AF4" s="82" t="s">
         <v>10</v>
       </c>
       <c r="AG4" s="82" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="AH4" s="62"/>
       <c r="AI4" s="62"/>
-      <c r="AJ4" s="62"/>
+      <c r="AJ4" s="63"/>
       <c r="AK4" s="63"/>
-      <c r="AL4" s="63"/>
+      <c r="AL4" s="64"/>
       <c r="AM4" s="64"/>
       <c r="AN4" s="64"/>
-      <c r="AO4" s="64"/>
+      <c r="AO4" s="65"/>
       <c r="AP4" s="65"/>
       <c r="AQ4" s="65"/>
-      <c r="AR4" s="65"/>
+      <c r="AR4" s="63"/>
       <c r="AS4" s="63"/>
       <c r="AT4" s="63"/>
       <c r="AU4" s="63"/>
@@ -5508,7 +5505,7 @@
       <c r="AZ4" s="63"/>
       <c r="BA4" s="63"/>
       <c r="BB4" s="63"/>
-      <c r="BC4" s="63"/>
+      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" s="85" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="73" t="s">
@@ -5548,15 +5545,15 @@
       <c r="AG5" s="73"/>
       <c r="AH5" s="74"/>
       <c r="AI5" s="74"/>
-      <c r="AJ5" s="74"/>
+      <c r="AJ5" s="84"/>
       <c r="AK5" s="84"/>
-      <c r="AL5" s="84"/>
+      <c r="AL5" s="76"/>
       <c r="AM5" s="76"/>
       <c r="AN5" s="76"/>
-      <c r="AO5" s="76"/>
+      <c r="AO5" s="77"/>
       <c r="AP5" s="77"/>
       <c r="AQ5" s="77"/>
-      <c r="AR5" s="77"/>
+      <c r="AR5" s="84"/>
       <c r="AS5" s="84"/>
       <c r="AT5" s="84"/>
       <c r="AU5" s="84"/>
@@ -5567,7 +5564,7 @@
       <c r="AZ5" s="84"/>
       <c r="BA5" s="84"/>
       <c r="BB5" s="84"/>
-      <c r="BC5" s="84"/>
+      <c r="AMJ5" s="0"/>
     </row>
     <row r="6" s="89" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="79" t="s">
@@ -5655,23 +5652,23 @@
         <v>139</v>
       </c>
       <c r="AE6" s="81" t="s">
+        <v>111</v>
+      </c>
+      <c r="AF6" s="81"/>
+      <c r="AG6" s="81" t="s">
         <v>13</v>
       </c>
-      <c r="AF6" s="81" t="s">
-        <v>111</v>
-      </c>
-      <c r="AG6" s="81"/>
       <c r="AH6" s="86"/>
       <c r="AI6" s="86"/>
-      <c r="AJ6" s="86"/>
+      <c r="AJ6" s="88"/>
       <c r="AK6" s="88"/>
-      <c r="AL6" s="88"/>
+      <c r="AL6" s="64"/>
       <c r="AM6" s="64"/>
       <c r="AN6" s="64"/>
-      <c r="AO6" s="64"/>
+      <c r="AO6" s="65"/>
       <c r="AP6" s="65"/>
       <c r="AQ6" s="65"/>
-      <c r="AR6" s="65"/>
+      <c r="AR6" s="88"/>
       <c r="AS6" s="88"/>
       <c r="AT6" s="88"/>
       <c r="AU6" s="88"/>
@@ -5682,7 +5679,7 @@
       <c r="AZ6" s="88"/>
       <c r="BA6" s="88"/>
       <c r="BB6" s="88"/>
-      <c r="BC6" s="88"/>
+      <c r="AMJ6" s="0"/>
     </row>
     <row r="7" s="91" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="90" t="s">
@@ -5722,15 +5719,15 @@
       <c r="AG7" s="90"/>
       <c r="AH7" s="74"/>
       <c r="AI7" s="74"/>
-      <c r="AJ7" s="74"/>
+      <c r="AJ7" s="75"/>
       <c r="AK7" s="75"/>
-      <c r="AL7" s="75"/>
+      <c r="AL7" s="76"/>
       <c r="AM7" s="76"/>
       <c r="AN7" s="76"/>
-      <c r="AO7" s="76"/>
+      <c r="AO7" s="77"/>
       <c r="AP7" s="77"/>
       <c r="AQ7" s="77"/>
-      <c r="AR7" s="77"/>
+      <c r="AR7" s="75"/>
       <c r="AS7" s="75"/>
       <c r="AT7" s="75"/>
       <c r="AU7" s="75"/>
@@ -5741,7 +5738,7 @@
       <c r="AZ7" s="75"/>
       <c r="BA7" s="75"/>
       <c r="BB7" s="75"/>
-      <c r="BC7" s="75"/>
+      <c r="AMJ7" s="0"/>
     </row>
     <row r="8" s="93" customFormat="true" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="81" t="s">
@@ -5808,24 +5805,24 @@
       <c r="AD8" s="81" t="s">
         <v>179</v>
       </c>
-      <c r="AE8" s="81" t="s">
+      <c r="AE8" s="81"/>
+      <c r="AF8" s="81" t="s">
         <v>180</v>
       </c>
-      <c r="AF8" s="81"/>
       <c r="AG8" s="81" t="s">
         <v>181</v>
       </c>
       <c r="AH8" s="86"/>
       <c r="AI8" s="86"/>
-      <c r="AJ8" s="86"/>
+      <c r="AJ8" s="92"/>
       <c r="AK8" s="92"/>
-      <c r="AL8" s="92"/>
+      <c r="AL8" s="64"/>
       <c r="AM8" s="64"/>
       <c r="AN8" s="64"/>
-      <c r="AO8" s="64"/>
+      <c r="AO8" s="65"/>
       <c r="AP8" s="65"/>
       <c r="AQ8" s="65"/>
-      <c r="AR8" s="65"/>
+      <c r="AR8" s="92"/>
       <c r="AS8" s="92"/>
       <c r="AT8" s="92"/>
       <c r="AU8" s="92"/>
@@ -5836,7 +5833,7 @@
       <c r="AZ8" s="92"/>
       <c r="BA8" s="92"/>
       <c r="BB8" s="92"/>
-      <c r="BC8" s="92"/>
+      <c r="AMJ8" s="0"/>
     </row>
     <row r="9" s="95" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="94" t="s">
@@ -5876,15 +5873,15 @@
       <c r="AG9" s="94"/>
       <c r="AH9" s="68"/>
       <c r="AI9" s="68"/>
-      <c r="AJ9" s="68"/>
+      <c r="AJ9" s="69"/>
       <c r="AK9" s="69"/>
-      <c r="AL9" s="69"/>
+      <c r="AL9" s="70"/>
       <c r="AM9" s="70"/>
       <c r="AN9" s="70"/>
-      <c r="AO9" s="70"/>
+      <c r="AO9" s="71"/>
       <c r="AP9" s="71"/>
       <c r="AQ9" s="71"/>
-      <c r="AR9" s="71"/>
+      <c r="AR9" s="69"/>
       <c r="AS9" s="69"/>
       <c r="AT9" s="69"/>
       <c r="AU9" s="69"/>
@@ -5895,7 +5892,7 @@
       <c r="AZ9" s="69"/>
       <c r="BA9" s="69"/>
       <c r="BB9" s="69"/>
-      <c r="BC9" s="69"/>
+      <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="21.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="96" t="s">
@@ -5988,26 +5985,26 @@
       <c r="AD10" s="103" t="s">
         <v>200</v>
       </c>
-      <c r="AE10" s="103" t="s">
+      <c r="AE10" s="102" t="s">
         <v>201</v>
       </c>
       <c r="AF10" s="102" t="s">
         <v>202</v>
       </c>
-      <c r="AG10" s="102" t="s">
-        <v>203</v>
-      </c>
-      <c r="AH10" s="97"/>
+      <c r="AG10" s="103" t="s">
+        <v>195</v>
+      </c>
+      <c r="AH10" s="104"/>
       <c r="AI10" s="104"/>
-      <c r="AJ10" s="104"/>
-      <c r="AK10" s="64"/>
-      <c r="AL10" s="105"/>
+      <c r="AJ10" s="64"/>
+      <c r="AK10" s="105"/>
+      <c r="AL10" s="64"/>
       <c r="AM10" s="64"/>
       <c r="AN10" s="64"/>
-      <c r="AO10" s="64"/>
+      <c r="AO10" s="65"/>
       <c r="AP10" s="65"/>
       <c r="AQ10" s="65"/>
-      <c r="AR10" s="65"/>
+      <c r="AR10" s="64"/>
       <c r="AS10" s="64"/>
       <c r="AT10" s="64"/>
       <c r="AU10" s="64"/>
@@ -6018,11 +6015,10 @@
       <c r="AZ10" s="64"/>
       <c r="BA10" s="64"/>
       <c r="BB10" s="64"/>
-      <c r="BC10" s="64"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="106" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B11" s="106" t="n">
         <v>1</v>
@@ -6040,7 +6036,7 @@
         <v>234</v>
       </c>
       <c r="G11" s="107" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H11" s="106" t="n">
         <v>5</v>
@@ -6101,13 +6097,13 @@
         <v>1</v>
       </c>
       <c r="Z11" s="109" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AA11" s="106" t="n">
         <v>3</v>
       </c>
       <c r="AB11" s="106" t="n">
-        <f aca="false">AG11*AA11</f>
+        <f aca="false">AF11*AA11</f>
         <v>0.0015</v>
       </c>
       <c r="AC11" s="106" t="n">
@@ -6117,27 +6113,27 @@
       <c r="AD11" s="106" t="n">
         <v>200</v>
       </c>
-      <c r="AE11" s="109" t="n">
+      <c r="AE11" s="110" t="n">
+        <v>321</v>
+      </c>
+      <c r="AF11" s="110" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="AG11" s="109" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AF11" s="110" t="n">
-        <v>321</v>
-      </c>
-      <c r="AG11" s="110" t="n">
-        <v>0.0005</v>
-      </c>
       <c r="AH11" s="104"/>
       <c r="AI11" s="104"/>
-      <c r="AJ11" s="104"/>
-      <c r="AK11" s="64"/>
-      <c r="AL11" s="105"/>
+      <c r="AJ11" s="64"/>
+      <c r="AK11" s="105"/>
+      <c r="AL11" s="64"/>
       <c r="AM11" s="64"/>
       <c r="AN11" s="64"/>
-      <c r="AO11" s="64"/>
+      <c r="AO11" s="65"/>
       <c r="AP11" s="65"/>
       <c r="AQ11" s="65"/>
-      <c r="AR11" s="65"/>
+      <c r="AR11" s="64"/>
       <c r="AS11" s="64"/>
       <c r="AT11" s="64"/>
       <c r="AU11" s="64"/>
@@ -6148,11 +6144,10 @@
       <c r="AZ11" s="64"/>
       <c r="BA11" s="64"/>
       <c r="BB11" s="64"/>
-      <c r="BC11" s="64"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="106" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B12" s="106" t="n">
         <v>2</v>
@@ -6170,7 +6165,7 @@
         <v>234</v>
       </c>
       <c r="G12" s="107" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H12" s="106" t="n">
         <v>5</v>
@@ -6231,13 +6226,13 @@
         <v>1</v>
       </c>
       <c r="Z12" s="109" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AA12" s="106" t="n">
         <v>3</v>
       </c>
       <c r="AB12" s="106" t="n">
-        <f aca="false">AG12*AA12</f>
+        <f aca="false">AF12*AA12</f>
         <v>0.0015</v>
       </c>
       <c r="AC12" s="106" t="n">
@@ -6247,27 +6242,27 @@
       <c r="AD12" s="106" t="n">
         <v>200</v>
       </c>
-      <c r="AE12" s="109" t="n">
+      <c r="AE12" s="110" t="n">
+        <v>321</v>
+      </c>
+      <c r="AF12" s="110" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="AG12" s="109" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AF12" s="110" t="n">
-        <v>321</v>
-      </c>
-      <c r="AG12" s="110" t="n">
-        <v>0.0005</v>
-      </c>
       <c r="AH12" s="104"/>
       <c r="AI12" s="104"/>
-      <c r="AJ12" s="104"/>
-      <c r="AK12" s="64"/>
-      <c r="AL12" s="105"/>
+      <c r="AJ12" s="64"/>
+      <c r="AK12" s="105"/>
+      <c r="AL12" s="64"/>
       <c r="AM12" s="64"/>
       <c r="AN12" s="64"/>
-      <c r="AO12" s="64"/>
+      <c r="AO12" s="65"/>
       <c r="AP12" s="65"/>
       <c r="AQ12" s="65"/>
-      <c r="AR12" s="65"/>
+      <c r="AR12" s="64"/>
       <c r="AS12" s="64"/>
       <c r="AT12" s="64"/>
       <c r="AU12" s="64"/>
@@ -6278,11 +6273,10 @@
       <c r="AZ12" s="64"/>
       <c r="BA12" s="64"/>
       <c r="BB12" s="64"/>
-      <c r="BC12" s="64"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="106" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B13" s="106" t="n">
         <v>3</v>
@@ -6300,7 +6294,7 @@
         <v>234</v>
       </c>
       <c r="G13" s="107" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H13" s="106" t="n">
         <v>5</v>
@@ -6361,13 +6355,13 @@
         <v>1</v>
       </c>
       <c r="Z13" s="109" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AA13" s="106" t="n">
         <v>3</v>
       </c>
       <c r="AB13" s="106" t="n">
-        <f aca="false">AG13*AA13</f>
+        <f aca="false">AF13*AA13</f>
         <v>0.0015</v>
       </c>
       <c r="AC13" s="106" t="n">
@@ -6377,27 +6371,27 @@
       <c r="AD13" s="106" t="n">
         <v>200</v>
       </c>
-      <c r="AE13" s="109" t="n">
+      <c r="AE13" s="110" t="n">
+        <v>321</v>
+      </c>
+      <c r="AF13" s="110" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="AG13" s="109" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AF13" s="110" t="n">
-        <v>321</v>
-      </c>
-      <c r="AG13" s="110" t="n">
-        <v>0.0005</v>
-      </c>
       <c r="AH13" s="104"/>
       <c r="AI13" s="104"/>
-      <c r="AJ13" s="104"/>
-      <c r="AK13" s="64"/>
-      <c r="AL13" s="105"/>
+      <c r="AJ13" s="64"/>
+      <c r="AK13" s="105"/>
+      <c r="AL13" s="64"/>
       <c r="AM13" s="64"/>
       <c r="AN13" s="64"/>
-      <c r="AO13" s="64"/>
+      <c r="AO13" s="65"/>
       <c r="AP13" s="65"/>
       <c r="AQ13" s="65"/>
-      <c r="AR13" s="65"/>
+      <c r="AR13" s="64"/>
       <c r="AS13" s="64"/>
       <c r="AT13" s="64"/>
       <c r="AU13" s="64"/>
@@ -6408,11 +6402,10 @@
       <c r="AZ13" s="64"/>
       <c r="BA13" s="64"/>
       <c r="BB13" s="64"/>
-      <c r="BC13" s="64"/>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="106" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B14" s="106" t="n">
         <v>4</v>
@@ -6430,7 +6423,7 @@
         <v>234</v>
       </c>
       <c r="G14" s="107" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="H14" s="106" t="n">
         <v>5</v>
@@ -6487,16 +6480,16 @@
         <v>1000</v>
       </c>
       <c r="Y14" s="109" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="Z14" s="109" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="AA14" s="106" t="n">
         <v>3</v>
       </c>
       <c r="AB14" s="106" t="n">
-        <f aca="false">AG14*AA14</f>
+        <f aca="false">AF14*AA14</f>
         <v>0.0015</v>
       </c>
       <c r="AC14" s="106" t="n">
@@ -6506,27 +6499,27 @@
       <c r="AD14" s="106" t="n">
         <v>200</v>
       </c>
-      <c r="AE14" s="109" t="n">
+      <c r="AE14" s="110" t="n">
+        <v>321</v>
+      </c>
+      <c r="AF14" s="110" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="AG14" s="109" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="AF14" s="110" t="n">
-        <v>321</v>
-      </c>
-      <c r="AG14" s="110" t="n">
-        <v>0.0005</v>
-      </c>
       <c r="AH14" s="104"/>
       <c r="AI14" s="104"/>
-      <c r="AJ14" s="104"/>
-      <c r="AK14" s="64"/>
-      <c r="AL14" s="105"/>
+      <c r="AJ14" s="64"/>
+      <c r="AK14" s="105"/>
+      <c r="AL14" s="64"/>
       <c r="AM14" s="64"/>
       <c r="AN14" s="64"/>
-      <c r="AO14" s="64"/>
+      <c r="AO14" s="65"/>
       <c r="AP14" s="65"/>
       <c r="AQ14" s="65"/>
-      <c r="AR14" s="65"/>
+      <c r="AR14" s="64"/>
       <c r="AS14" s="64"/>
       <c r="AT14" s="64"/>
       <c r="AU14" s="64"/>
@@ -6537,7 +6530,6 @@
       <c r="AZ14" s="64"/>
       <c r="BA14" s="64"/>
       <c r="BB14" s="64"/>
-      <c r="BC14" s="64"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="106"/>
@@ -6575,15 +6567,15 @@
       <c r="AG15" s="106"/>
       <c r="AH15" s="104"/>
       <c r="AI15" s="104"/>
-      <c r="AJ15" s="104"/>
-      <c r="AK15" s="64"/>
-      <c r="AL15" s="105"/>
+      <c r="AJ15" s="64"/>
+      <c r="AK15" s="105"/>
+      <c r="AL15" s="64"/>
       <c r="AM15" s="64"/>
       <c r="AN15" s="64"/>
-      <c r="AO15" s="64"/>
+      <c r="AO15" s="65"/>
       <c r="AP15" s="65"/>
       <c r="AQ15" s="65"/>
-      <c r="AR15" s="65"/>
+      <c r="AR15" s="64"/>
       <c r="AS15" s="64"/>
       <c r="AT15" s="64"/>
       <c r="AU15" s="64"/>
@@ -6594,7 +6586,6 @@
       <c r="AZ15" s="64"/>
       <c r="BA15" s="64"/>
       <c r="BB15" s="64"/>
-      <c r="BC15" s="64"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="106"/>
@@ -6632,15 +6623,15 @@
       <c r="AG16" s="106"/>
       <c r="AH16" s="104"/>
       <c r="AI16" s="104"/>
-      <c r="AJ16" s="104"/>
-      <c r="AK16" s="64"/>
-      <c r="AL16" s="105"/>
+      <c r="AJ16" s="64"/>
+      <c r="AK16" s="105"/>
+      <c r="AL16" s="64"/>
       <c r="AM16" s="64"/>
       <c r="AN16" s="64"/>
-      <c r="AO16" s="64"/>
+      <c r="AO16" s="65"/>
       <c r="AP16" s="65"/>
       <c r="AQ16" s="65"/>
-      <c r="AR16" s="65"/>
+      <c r="AR16" s="64"/>
       <c r="AS16" s="64"/>
       <c r="AT16" s="64"/>
       <c r="AU16" s="64"/>
@@ -6651,7 +6642,6 @@
       <c r="AZ16" s="64"/>
       <c r="BA16" s="64"/>
       <c r="BB16" s="64"/>
-      <c r="BC16" s="64"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="106"/>
@@ -6689,15 +6679,15 @@
       <c r="AG17" s="106"/>
       <c r="AH17" s="104"/>
       <c r="AI17" s="104"/>
-      <c r="AJ17" s="104"/>
-      <c r="AK17" s="64"/>
-      <c r="AL17" s="105"/>
+      <c r="AJ17" s="64"/>
+      <c r="AK17" s="105"/>
+      <c r="AL17" s="64"/>
       <c r="AM17" s="64"/>
       <c r="AN17" s="64"/>
-      <c r="AO17" s="64"/>
+      <c r="AO17" s="65"/>
       <c r="AP17" s="65"/>
       <c r="AQ17" s="65"/>
-      <c r="AR17" s="65"/>
+      <c r="AR17" s="64"/>
       <c r="AS17" s="64"/>
       <c r="AT17" s="64"/>
       <c r="AU17" s="64"/>
@@ -6708,7 +6698,6 @@
       <c r="AZ17" s="64"/>
       <c r="BA17" s="64"/>
       <c r="BB17" s="64"/>
-      <c r="BC17" s="64"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="106"/>
@@ -6746,15 +6735,15 @@
       <c r="AG18" s="106"/>
       <c r="AH18" s="104"/>
       <c r="AI18" s="104"/>
-      <c r="AJ18" s="104"/>
-      <c r="AK18" s="64"/>
-      <c r="AL18" s="105"/>
+      <c r="AJ18" s="64"/>
+      <c r="AK18" s="105"/>
+      <c r="AL18" s="64"/>
       <c r="AM18" s="64"/>
       <c r="AN18" s="64"/>
-      <c r="AO18" s="64"/>
+      <c r="AO18" s="65"/>
       <c r="AP18" s="65"/>
       <c r="AQ18" s="65"/>
-      <c r="AR18" s="65"/>
+      <c r="AR18" s="64"/>
       <c r="AS18" s="64"/>
       <c r="AT18" s="64"/>
       <c r="AU18" s="64"/>
@@ -6765,7 +6754,6 @@
       <c r="AZ18" s="64"/>
       <c r="BA18" s="64"/>
       <c r="BB18" s="64"/>
-      <c r="BC18" s="64"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="106"/>
@@ -6803,15 +6791,15 @@
       <c r="AG19" s="106"/>
       <c r="AH19" s="104"/>
       <c r="AI19" s="104"/>
-      <c r="AJ19" s="104"/>
-      <c r="AK19" s="64"/>
-      <c r="AL19" s="105"/>
+      <c r="AJ19" s="64"/>
+      <c r="AK19" s="105"/>
+      <c r="AL19" s="64"/>
       <c r="AM19" s="64"/>
       <c r="AN19" s="64"/>
-      <c r="AO19" s="64"/>
+      <c r="AO19" s="65"/>
       <c r="AP19" s="65"/>
       <c r="AQ19" s="65"/>
-      <c r="AR19" s="65"/>
+      <c r="AR19" s="64"/>
       <c r="AS19" s="64"/>
       <c r="AT19" s="64"/>
       <c r="AU19" s="64"/>
@@ -6822,7 +6810,6 @@
       <c r="AZ19" s="64"/>
       <c r="BA19" s="64"/>
       <c r="BB19" s="64"/>
-      <c r="BC19" s="64"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="106"/>
@@ -6860,15 +6847,15 @@
       <c r="AG20" s="106"/>
       <c r="AH20" s="104"/>
       <c r="AI20" s="104"/>
-      <c r="AJ20" s="104"/>
-      <c r="AK20" s="64"/>
-      <c r="AL20" s="105"/>
+      <c r="AJ20" s="64"/>
+      <c r="AK20" s="105"/>
+      <c r="AL20" s="64"/>
       <c r="AM20" s="64"/>
       <c r="AN20" s="64"/>
-      <c r="AO20" s="64"/>
+      <c r="AO20" s="65"/>
       <c r="AP20" s="65"/>
       <c r="AQ20" s="65"/>
-      <c r="AR20" s="65"/>
+      <c r="AR20" s="64"/>
       <c r="AS20" s="64"/>
       <c r="AT20" s="64"/>
       <c r="AU20" s="64"/>
@@ -6879,7 +6866,6 @@
       <c r="AZ20" s="64"/>
       <c r="BA20" s="64"/>
       <c r="BB20" s="64"/>
-      <c r="BC20" s="64"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="111"/>
@@ -6917,15 +6903,15 @@
       <c r="AG21" s="111"/>
       <c r="AH21" s="112"/>
       <c r="AI21" s="112"/>
-      <c r="AJ21" s="112"/>
-      <c r="AK21" s="64"/>
-      <c r="AL21" s="105"/>
+      <c r="AJ21" s="64"/>
+      <c r="AK21" s="105"/>
+      <c r="AL21" s="64"/>
       <c r="AM21" s="64"/>
       <c r="AN21" s="64"/>
-      <c r="AO21" s="64"/>
+      <c r="AO21" s="65"/>
       <c r="AP21" s="65"/>
       <c r="AQ21" s="65"/>
-      <c r="AR21" s="65"/>
+      <c r="AR21" s="64"/>
       <c r="AS21" s="64"/>
       <c r="AT21" s="64"/>
       <c r="AU21" s="64"/>
@@ -6936,7 +6922,6 @@
       <c r="AZ21" s="64"/>
       <c r="BA21" s="64"/>
       <c r="BB21" s="64"/>
-      <c r="BC21" s="64"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="111"/>
@@ -6974,15 +6959,15 @@
       <c r="AG22" s="111"/>
       <c r="AH22" s="112"/>
       <c r="AI22" s="112"/>
-      <c r="AJ22" s="112"/>
-      <c r="AK22" s="64"/>
-      <c r="AL22" s="105"/>
+      <c r="AJ22" s="64"/>
+      <c r="AK22" s="105"/>
+      <c r="AL22" s="64"/>
       <c r="AM22" s="64"/>
       <c r="AN22" s="64"/>
-      <c r="AO22" s="64"/>
+      <c r="AO22" s="65"/>
       <c r="AP22" s="65"/>
       <c r="AQ22" s="65"/>
-      <c r="AR22" s="65"/>
+      <c r="AR22" s="64"/>
       <c r="AS22" s="64"/>
       <c r="AT22" s="64"/>
       <c r="AU22" s="64"/>
@@ -6993,7 +6978,6 @@
       <c r="AZ22" s="64"/>
       <c r="BA22" s="64"/>
       <c r="BB22" s="64"/>
-      <c r="BC22" s="64"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="111"/>
@@ -7031,15 +7015,15 @@
       <c r="AG23" s="111"/>
       <c r="AH23" s="112"/>
       <c r="AI23" s="112"/>
-      <c r="AJ23" s="112"/>
-      <c r="AK23" s="64"/>
-      <c r="AL23" s="105"/>
+      <c r="AJ23" s="64"/>
+      <c r="AK23" s="105"/>
+      <c r="AL23" s="64"/>
       <c r="AM23" s="64"/>
       <c r="AN23" s="64"/>
-      <c r="AO23" s="64"/>
+      <c r="AO23" s="65"/>
       <c r="AP23" s="65"/>
       <c r="AQ23" s="65"/>
-      <c r="AR23" s="65"/>
+      <c r="AR23" s="64"/>
       <c r="AS23" s="64"/>
       <c r="AT23" s="64"/>
       <c r="AU23" s="64"/>
@@ -7050,7 +7034,6 @@
       <c r="AZ23" s="64"/>
       <c r="BA23" s="64"/>
       <c r="BB23" s="64"/>
-      <c r="BC23" s="64"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="111"/>
@@ -7088,15 +7071,15 @@
       <c r="AG24" s="111"/>
       <c r="AH24" s="112"/>
       <c r="AI24" s="112"/>
-      <c r="AJ24" s="112"/>
-      <c r="AK24" s="64"/>
-      <c r="AL24" s="105"/>
+      <c r="AJ24" s="64"/>
+      <c r="AK24" s="105"/>
+      <c r="AL24" s="64"/>
       <c r="AM24" s="64"/>
       <c r="AN24" s="64"/>
-      <c r="AO24" s="64"/>
+      <c r="AO24" s="65"/>
       <c r="AP24" s="65"/>
       <c r="AQ24" s="65"/>
-      <c r="AR24" s="65"/>
+      <c r="AR24" s="64"/>
       <c r="AS24" s="64"/>
       <c r="AT24" s="64"/>
       <c r="AU24" s="64"/>
@@ -7107,7 +7090,6 @@
       <c r="AZ24" s="64"/>
       <c r="BA24" s="64"/>
       <c r="BB24" s="64"/>
-      <c r="BC24" s="64"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="111"/>
@@ -7145,15 +7127,15 @@
       <c r="AG25" s="111"/>
       <c r="AH25" s="112"/>
       <c r="AI25" s="112"/>
-      <c r="AJ25" s="112"/>
-      <c r="AK25" s="64"/>
-      <c r="AL25" s="105"/>
+      <c r="AJ25" s="64"/>
+      <c r="AK25" s="105"/>
+      <c r="AL25" s="64"/>
       <c r="AM25" s="64"/>
       <c r="AN25" s="64"/>
-      <c r="AO25" s="64"/>
+      <c r="AO25" s="65"/>
       <c r="AP25" s="65"/>
       <c r="AQ25" s="65"/>
-      <c r="AR25" s="65"/>
+      <c r="AR25" s="64"/>
       <c r="AS25" s="64"/>
       <c r="AT25" s="64"/>
       <c r="AU25" s="64"/>
@@ -7164,22 +7146,21 @@
       <c r="AZ25" s="64"/>
       <c r="BA25" s="64"/>
       <c r="BB25" s="64"/>
-      <c r="BC25" s="64"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F26" s="105"/>
       <c r="G26" s="105"/>
       <c r="AH26" s="105"/>
       <c r="AI26" s="105"/>
-      <c r="AJ26" s="105"/>
-      <c r="AK26" s="64"/>
-      <c r="AL26" s="105"/>
+      <c r="AJ26" s="64"/>
+      <c r="AK26" s="105"/>
+      <c r="AL26" s="64"/>
       <c r="AM26" s="64"/>
       <c r="AN26" s="64"/>
-      <c r="AO26" s="64"/>
+      <c r="AO26" s="65"/>
       <c r="AP26" s="65"/>
       <c r="AQ26" s="65"/>
-      <c r="AR26" s="65"/>
+      <c r="AR26" s="64"/>
       <c r="AS26" s="64"/>
       <c r="AT26" s="64"/>
       <c r="AU26" s="64"/>
@@ -7190,22 +7171,21 @@
       <c r="AZ26" s="64"/>
       <c r="BA26" s="64"/>
       <c r="BB26" s="64"/>
-      <c r="BC26" s="64"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F27" s="105"/>
       <c r="G27" s="105"/>
       <c r="AH27" s="105"/>
       <c r="AI27" s="105"/>
-      <c r="AJ27" s="105"/>
-      <c r="AK27" s="64"/>
-      <c r="AL27" s="105"/>
+      <c r="AJ27" s="64"/>
+      <c r="AK27" s="105"/>
+      <c r="AL27" s="64"/>
       <c r="AM27" s="64"/>
       <c r="AN27" s="64"/>
-      <c r="AO27" s="64"/>
+      <c r="AO27" s="65"/>
       <c r="AP27" s="65"/>
       <c r="AQ27" s="65"/>
-      <c r="AR27" s="65"/>
+      <c r="AR27" s="64"/>
       <c r="AS27" s="64"/>
       <c r="AT27" s="64"/>
       <c r="AU27" s="64"/>
@@ -7216,22 +7196,21 @@
       <c r="AZ27" s="64"/>
       <c r="BA27" s="64"/>
       <c r="BB27" s="64"/>
-      <c r="BC27" s="64"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F28" s="105"/>
       <c r="G28" s="105"/>
       <c r="AH28" s="105"/>
       <c r="AI28" s="105"/>
-      <c r="AJ28" s="105"/>
-      <c r="AK28" s="64"/>
-      <c r="AL28" s="105"/>
+      <c r="AJ28" s="64"/>
+      <c r="AK28" s="105"/>
+      <c r="AL28" s="64"/>
       <c r="AM28" s="64"/>
       <c r="AN28" s="64"/>
-      <c r="AO28" s="64"/>
+      <c r="AO28" s="65"/>
       <c r="AP28" s="65"/>
       <c r="AQ28" s="65"/>
-      <c r="AR28" s="65"/>
+      <c r="AR28" s="64"/>
       <c r="AS28" s="64"/>
       <c r="AT28" s="64"/>
       <c r="AU28" s="64"/>
@@ -7242,22 +7221,21 @@
       <c r="AZ28" s="64"/>
       <c r="BA28" s="64"/>
       <c r="BB28" s="64"/>
-      <c r="BC28" s="64"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F29" s="105"/>
       <c r="G29" s="105"/>
       <c r="AH29" s="105"/>
       <c r="AI29" s="105"/>
-      <c r="AJ29" s="105"/>
-      <c r="AK29" s="64"/>
-      <c r="AL29" s="105"/>
+      <c r="AJ29" s="64"/>
+      <c r="AK29" s="105"/>
+      <c r="AL29" s="64"/>
       <c r="AM29" s="64"/>
       <c r="AN29" s="64"/>
-      <c r="AO29" s="64"/>
+      <c r="AO29" s="65"/>
       <c r="AP29" s="65"/>
       <c r="AQ29" s="65"/>
-      <c r="AR29" s="65"/>
+      <c r="AR29" s="64"/>
       <c r="AS29" s="64"/>
       <c r="AT29" s="64"/>
       <c r="AU29" s="64"/>
@@ -7268,22 +7246,21 @@
       <c r="AZ29" s="64"/>
       <c r="BA29" s="64"/>
       <c r="BB29" s="64"/>
-      <c r="BC29" s="64"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F30" s="105"/>
       <c r="G30" s="105"/>
       <c r="AH30" s="105"/>
       <c r="AI30" s="105"/>
-      <c r="AJ30" s="105"/>
-      <c r="AK30" s="64"/>
-      <c r="AL30" s="105"/>
+      <c r="AJ30" s="64"/>
+      <c r="AK30" s="105"/>
+      <c r="AL30" s="64"/>
       <c r="AM30" s="64"/>
       <c r="AN30" s="64"/>
-      <c r="AO30" s="64"/>
+      <c r="AO30" s="65"/>
       <c r="AP30" s="65"/>
       <c r="AQ30" s="65"/>
-      <c r="AR30" s="65"/>
+      <c r="AR30" s="64"/>
       <c r="AS30" s="64"/>
       <c r="AT30" s="64"/>
       <c r="AU30" s="64"/>
@@ -7294,22 +7271,21 @@
       <c r="AZ30" s="64"/>
       <c r="BA30" s="64"/>
       <c r="BB30" s="64"/>
-      <c r="BC30" s="64"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F31" s="105"/>
       <c r="G31" s="105"/>
       <c r="AH31" s="105"/>
       <c r="AI31" s="105"/>
-      <c r="AJ31" s="105"/>
-      <c r="AK31" s="64"/>
-      <c r="AL31" s="105"/>
+      <c r="AJ31" s="64"/>
+      <c r="AK31" s="105"/>
+      <c r="AL31" s="64"/>
       <c r="AM31" s="64"/>
       <c r="AN31" s="64"/>
-      <c r="AO31" s="64"/>
+      <c r="AO31" s="65"/>
       <c r="AP31" s="65"/>
       <c r="AQ31" s="65"/>
-      <c r="AR31" s="65"/>
+      <c r="AR31" s="64"/>
       <c r="AS31" s="64"/>
       <c r="AT31" s="64"/>
       <c r="AU31" s="64"/>
@@ -7320,22 +7296,21 @@
       <c r="AZ31" s="64"/>
       <c r="BA31" s="64"/>
       <c r="BB31" s="64"/>
-      <c r="BC31" s="64"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F32" s="105"/>
       <c r="G32" s="105"/>
       <c r="AH32" s="105"/>
       <c r="AI32" s="105"/>
-      <c r="AJ32" s="105"/>
-      <c r="AK32" s="64"/>
-      <c r="AL32" s="105"/>
+      <c r="AJ32" s="64"/>
+      <c r="AK32" s="105"/>
+      <c r="AL32" s="64"/>
       <c r="AM32" s="64"/>
       <c r="AN32" s="64"/>
-      <c r="AO32" s="64"/>
+      <c r="AO32" s="65"/>
       <c r="AP32" s="65"/>
       <c r="AQ32" s="65"/>
-      <c r="AR32" s="65"/>
+      <c r="AR32" s="64"/>
       <c r="AS32" s="64"/>
       <c r="AT32" s="64"/>
       <c r="AU32" s="64"/>
@@ -7346,22 +7321,21 @@
       <c r="AZ32" s="64"/>
       <c r="BA32" s="64"/>
       <c r="BB32" s="64"/>
-      <c r="BC32" s="64"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F33" s="105"/>
       <c r="G33" s="105"/>
       <c r="AH33" s="105"/>
       <c r="AI33" s="105"/>
-      <c r="AJ33" s="105"/>
-      <c r="AK33" s="64"/>
-      <c r="AL33" s="105"/>
+      <c r="AJ33" s="64"/>
+      <c r="AK33" s="105"/>
+      <c r="AL33" s="64"/>
       <c r="AM33" s="64"/>
       <c r="AN33" s="64"/>
-      <c r="AO33" s="64"/>
+      <c r="AO33" s="65"/>
       <c r="AP33" s="65"/>
       <c r="AQ33" s="65"/>
-      <c r="AR33" s="65"/>
+      <c r="AR33" s="64"/>
       <c r="AS33" s="64"/>
       <c r="AT33" s="64"/>
       <c r="AU33" s="64"/>
@@ -7372,22 +7346,21 @@
       <c r="AZ33" s="64"/>
       <c r="BA33" s="64"/>
       <c r="BB33" s="64"/>
-      <c r="BC33" s="64"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F34" s="105"/>
       <c r="G34" s="105"/>
       <c r="AH34" s="105"/>
       <c r="AI34" s="105"/>
-      <c r="AJ34" s="105"/>
-      <c r="AK34" s="64"/>
-      <c r="AL34" s="105"/>
+      <c r="AJ34" s="64"/>
+      <c r="AK34" s="105"/>
+      <c r="AL34" s="64"/>
       <c r="AM34" s="64"/>
       <c r="AN34" s="64"/>
-      <c r="AO34" s="64"/>
+      <c r="AO34" s="65"/>
       <c r="AP34" s="65"/>
       <c r="AQ34" s="65"/>
-      <c r="AR34" s="65"/>
+      <c r="AR34" s="64"/>
       <c r="AS34" s="64"/>
       <c r="AT34" s="64"/>
       <c r="AU34" s="64"/>
@@ -7398,22 +7371,21 @@
       <c r="AZ34" s="64"/>
       <c r="BA34" s="64"/>
       <c r="BB34" s="64"/>
-      <c r="BC34" s="64"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F35" s="105"/>
       <c r="G35" s="105"/>
       <c r="AH35" s="105"/>
       <c r="AI35" s="105"/>
-      <c r="AJ35" s="105"/>
-      <c r="AK35" s="64"/>
-      <c r="AL35" s="105"/>
+      <c r="AJ35" s="64"/>
+      <c r="AK35" s="105"/>
+      <c r="AL35" s="64"/>
       <c r="AM35" s="64"/>
       <c r="AN35" s="64"/>
-      <c r="AO35" s="64"/>
+      <c r="AO35" s="65"/>
       <c r="AP35" s="65"/>
       <c r="AQ35" s="65"/>
-      <c r="AR35" s="65"/>
+      <c r="AR35" s="64"/>
       <c r="AS35" s="64"/>
       <c r="AT35" s="64"/>
       <c r="AU35" s="64"/>
@@ -7424,22 +7396,21 @@
       <c r="AZ35" s="64"/>
       <c r="BA35" s="64"/>
       <c r="BB35" s="64"/>
-      <c r="BC35" s="64"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F36" s="105"/>
       <c r="G36" s="105"/>
       <c r="AH36" s="105"/>
       <c r="AI36" s="105"/>
-      <c r="AJ36" s="105"/>
-      <c r="AK36" s="64"/>
-      <c r="AL36" s="105"/>
+      <c r="AJ36" s="64"/>
+      <c r="AK36" s="105"/>
+      <c r="AL36" s="64"/>
       <c r="AM36" s="64"/>
       <c r="AN36" s="64"/>
-      <c r="AO36" s="64"/>
+      <c r="AO36" s="65"/>
       <c r="AP36" s="65"/>
       <c r="AQ36" s="65"/>
-      <c r="AR36" s="65"/>
+      <c r="AR36" s="64"/>
       <c r="AS36" s="64"/>
       <c r="AT36" s="64"/>
       <c r="AU36" s="64"/>
@@ -7450,22 +7421,21 @@
       <c r="AZ36" s="64"/>
       <c r="BA36" s="64"/>
       <c r="BB36" s="64"/>
-      <c r="BC36" s="64"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F37" s="105"/>
       <c r="G37" s="105"/>
       <c r="AH37" s="105"/>
       <c r="AI37" s="105"/>
-      <c r="AJ37" s="105"/>
-      <c r="AK37" s="64"/>
-      <c r="AL37" s="105"/>
+      <c r="AJ37" s="64"/>
+      <c r="AK37" s="105"/>
+      <c r="AL37" s="64"/>
       <c r="AM37" s="64"/>
       <c r="AN37" s="64"/>
-      <c r="AO37" s="64"/>
+      <c r="AO37" s="65"/>
       <c r="AP37" s="65"/>
       <c r="AQ37" s="65"/>
-      <c r="AR37" s="65"/>
+      <c r="AR37" s="64"/>
       <c r="AS37" s="64"/>
       <c r="AT37" s="64"/>
       <c r="AU37" s="64"/>
@@ -7476,22 +7446,21 @@
       <c r="AZ37" s="64"/>
       <c r="BA37" s="64"/>
       <c r="BB37" s="64"/>
-      <c r="BC37" s="64"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F38" s="105"/>
       <c r="G38" s="105"/>
       <c r="AH38" s="105"/>
       <c r="AI38" s="105"/>
-      <c r="AJ38" s="105"/>
-      <c r="AK38" s="64"/>
-      <c r="AL38" s="105"/>
+      <c r="AJ38" s="64"/>
+      <c r="AK38" s="105"/>
+      <c r="AL38" s="64"/>
       <c r="AM38" s="64"/>
       <c r="AN38" s="64"/>
-      <c r="AO38" s="64"/>
+      <c r="AO38" s="65"/>
       <c r="AP38" s="65"/>
       <c r="AQ38" s="65"/>
-      <c r="AR38" s="65"/>
+      <c r="AR38" s="64"/>
       <c r="AS38" s="64"/>
       <c r="AT38" s="64"/>
       <c r="AU38" s="64"/>
@@ -7502,22 +7471,21 @@
       <c r="AZ38" s="64"/>
       <c r="BA38" s="64"/>
       <c r="BB38" s="64"/>
-      <c r="BC38" s="64"/>
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F39" s="105"/>
       <c r="G39" s="105"/>
       <c r="AH39" s="105"/>
       <c r="AI39" s="105"/>
-      <c r="AJ39" s="105"/>
-      <c r="AK39" s="64"/>
-      <c r="AL39" s="105"/>
+      <c r="AJ39" s="64"/>
+      <c r="AK39" s="105"/>
+      <c r="AL39" s="64"/>
       <c r="AM39" s="64"/>
       <c r="AN39" s="64"/>
-      <c r="AO39" s="64"/>
+      <c r="AO39" s="65"/>
       <c r="AP39" s="65"/>
       <c r="AQ39" s="65"/>
-      <c r="AR39" s="65"/>
+      <c r="AR39" s="64"/>
       <c r="AS39" s="64"/>
       <c r="AT39" s="64"/>
       <c r="AU39" s="64"/>
@@ -7528,22 +7496,21 @@
       <c r="AZ39" s="64"/>
       <c r="BA39" s="64"/>
       <c r="BB39" s="64"/>
-      <c r="BC39" s="64"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F40" s="105"/>
       <c r="G40" s="105"/>
       <c r="AH40" s="105"/>
       <c r="AI40" s="105"/>
-      <c r="AJ40" s="105"/>
-      <c r="AK40" s="64"/>
-      <c r="AL40" s="105"/>
+      <c r="AJ40" s="64"/>
+      <c r="AK40" s="105"/>
+      <c r="AL40" s="64"/>
       <c r="AM40" s="64"/>
       <c r="AN40" s="64"/>
-      <c r="AO40" s="64"/>
+      <c r="AO40" s="65"/>
       <c r="AP40" s="65"/>
       <c r="AQ40" s="65"/>
-      <c r="AR40" s="65"/>
+      <c r="AR40" s="64"/>
       <c r="AS40" s="64"/>
       <c r="AT40" s="64"/>
       <c r="AU40" s="64"/>
@@ -7554,22 +7521,21 @@
       <c r="AZ40" s="64"/>
       <c r="BA40" s="64"/>
       <c r="BB40" s="64"/>
-      <c r="BC40" s="64"/>
     </row>
     <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F41" s="105"/>
       <c r="G41" s="105"/>
       <c r="AH41" s="105"/>
       <c r="AI41" s="105"/>
-      <c r="AJ41" s="105"/>
-      <c r="AK41" s="64"/>
-      <c r="AL41" s="105"/>
+      <c r="AJ41" s="64"/>
+      <c r="AK41" s="105"/>
+      <c r="AL41" s="64"/>
       <c r="AM41" s="64"/>
       <c r="AN41" s="64"/>
-      <c r="AO41" s="64"/>
+      <c r="AO41" s="65"/>
       <c r="AP41" s="65"/>
       <c r="AQ41" s="65"/>
-      <c r="AR41" s="65"/>
+      <c r="AR41" s="64"/>
       <c r="AS41" s="64"/>
       <c r="AT41" s="64"/>
       <c r="AU41" s="64"/>
@@ -7580,22 +7546,21 @@
       <c r="AZ41" s="64"/>
       <c r="BA41" s="64"/>
       <c r="BB41" s="64"/>
-      <c r="BC41" s="64"/>
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F42" s="105"/>
       <c r="G42" s="105"/>
       <c r="AH42" s="105"/>
       <c r="AI42" s="105"/>
-      <c r="AJ42" s="105"/>
-      <c r="AK42" s="64"/>
-      <c r="AL42" s="105"/>
+      <c r="AJ42" s="64"/>
+      <c r="AK42" s="105"/>
+      <c r="AL42" s="64"/>
       <c r="AM42" s="64"/>
       <c r="AN42" s="64"/>
-      <c r="AO42" s="64"/>
+      <c r="AO42" s="65"/>
       <c r="AP42" s="65"/>
       <c r="AQ42" s="65"/>
-      <c r="AR42" s="65"/>
+      <c r="AR42" s="64"/>
       <c r="AS42" s="64"/>
       <c r="AT42" s="64"/>
       <c r="AU42" s="64"/>
@@ -7606,22 +7571,21 @@
       <c r="AZ42" s="64"/>
       <c r="BA42" s="64"/>
       <c r="BB42" s="64"/>
-      <c r="BC42" s="64"/>
     </row>
     <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F43" s="105"/>
       <c r="G43" s="105"/>
       <c r="AH43" s="105"/>
       <c r="AI43" s="105"/>
-      <c r="AJ43" s="105"/>
-      <c r="AK43" s="64"/>
-      <c r="AL43" s="105"/>
+      <c r="AJ43" s="64"/>
+      <c r="AK43" s="105"/>
+      <c r="AL43" s="64"/>
       <c r="AM43" s="64"/>
       <c r="AN43" s="64"/>
-      <c r="AO43" s="64"/>
+      <c r="AO43" s="65"/>
       <c r="AP43" s="65"/>
       <c r="AQ43" s="65"/>
-      <c r="AR43" s="65"/>
+      <c r="AR43" s="64"/>
       <c r="AS43" s="64"/>
       <c r="AT43" s="64"/>
       <c r="AU43" s="64"/>
@@ -7632,22 +7596,21 @@
       <c r="AZ43" s="64"/>
       <c r="BA43" s="64"/>
       <c r="BB43" s="64"/>
-      <c r="BC43" s="64"/>
     </row>
     <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F44" s="105"/>
       <c r="G44" s="105"/>
       <c r="AH44" s="105"/>
       <c r="AI44" s="105"/>
-      <c r="AJ44" s="105"/>
-      <c r="AK44" s="64"/>
-      <c r="AL44" s="105"/>
+      <c r="AJ44" s="64"/>
+      <c r="AK44" s="105"/>
+      <c r="AL44" s="64"/>
       <c r="AM44" s="64"/>
       <c r="AN44" s="64"/>
-      <c r="AO44" s="64"/>
+      <c r="AO44" s="65"/>
       <c r="AP44" s="65"/>
       <c r="AQ44" s="65"/>
-      <c r="AR44" s="65"/>
+      <c r="AR44" s="64"/>
       <c r="AS44" s="64"/>
       <c r="AT44" s="64"/>
       <c r="AU44" s="64"/>
@@ -7658,22 +7621,21 @@
       <c r="AZ44" s="64"/>
       <c r="BA44" s="64"/>
       <c r="BB44" s="64"/>
-      <c r="BC44" s="64"/>
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F45" s="105"/>
       <c r="G45" s="105"/>
       <c r="AH45" s="105"/>
       <c r="AI45" s="105"/>
-      <c r="AJ45" s="105"/>
-      <c r="AK45" s="64"/>
-      <c r="AL45" s="105"/>
+      <c r="AJ45" s="64"/>
+      <c r="AK45" s="105"/>
+      <c r="AL45" s="64"/>
       <c r="AM45" s="64"/>
       <c r="AN45" s="64"/>
-      <c r="AO45" s="64"/>
+      <c r="AO45" s="65"/>
       <c r="AP45" s="65"/>
       <c r="AQ45" s="65"/>
-      <c r="AR45" s="65"/>
+      <c r="AR45" s="64"/>
       <c r="AS45" s="64"/>
       <c r="AT45" s="64"/>
       <c r="AU45" s="64"/>
@@ -7684,22 +7646,21 @@
       <c r="AZ45" s="64"/>
       <c r="BA45" s="64"/>
       <c r="BB45" s="64"/>
-      <c r="BC45" s="64"/>
     </row>
     <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F46" s="105"/>
       <c r="G46" s="105"/>
       <c r="AH46" s="105"/>
       <c r="AI46" s="105"/>
-      <c r="AJ46" s="105"/>
-      <c r="AK46" s="64"/>
-      <c r="AL46" s="105"/>
+      <c r="AJ46" s="64"/>
+      <c r="AK46" s="105"/>
+      <c r="AL46" s="64"/>
       <c r="AM46" s="64"/>
       <c r="AN46" s="64"/>
-      <c r="AO46" s="64"/>
+      <c r="AO46" s="65"/>
       <c r="AP46" s="65"/>
       <c r="AQ46" s="65"/>
-      <c r="AR46" s="65"/>
+      <c r="AR46" s="64"/>
       <c r="AS46" s="64"/>
       <c r="AT46" s="64"/>
       <c r="AU46" s="64"/>
@@ -7710,22 +7671,21 @@
       <c r="AZ46" s="64"/>
       <c r="BA46" s="64"/>
       <c r="BB46" s="64"/>
-      <c r="BC46" s="64"/>
     </row>
     <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F47" s="105"/>
       <c r="G47" s="105"/>
       <c r="AH47" s="105"/>
       <c r="AI47" s="105"/>
-      <c r="AJ47" s="105"/>
-      <c r="AK47" s="64"/>
-      <c r="AL47" s="105"/>
+      <c r="AJ47" s="64"/>
+      <c r="AK47" s="105"/>
+      <c r="AL47" s="64"/>
       <c r="AM47" s="64"/>
       <c r="AN47" s="64"/>
-      <c r="AO47" s="64"/>
+      <c r="AO47" s="65"/>
       <c r="AP47" s="65"/>
       <c r="AQ47" s="65"/>
-      <c r="AR47" s="65"/>
+      <c r="AR47" s="64"/>
       <c r="AS47" s="64"/>
       <c r="AT47" s="64"/>
       <c r="AU47" s="64"/>
@@ -7736,7 +7696,6 @@
       <c r="AZ47" s="64"/>
       <c r="BA47" s="64"/>
       <c r="BB47" s="64"/>
-      <c r="BC47" s="64"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -7773,7 +7732,7 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="31" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B1" s="50" t="s">
         <v>1</v>
@@ -7804,7 +7763,7 @@
     </row>
     <row r="2" s="3" customFormat="true" ht="131.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="30" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B2" s="50" t="s">
         <v>1</v>
@@ -7981,22 +7940,22 @@
         <v>1</v>
       </c>
       <c r="B9" s="10" t="s">
+        <v>212</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>213</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="E9" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>217</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>218</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
@@ -8041,28 +8000,28 @@
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="113" t="s">
+        <v>218</v>
+      </c>
+      <c r="B11" s="114" t="s">
         <v>219</v>
       </c>
-      <c r="B11" s="114" t="s">
+      <c r="C11" s="113" t="s">
         <v>220</v>
       </c>
-      <c r="C11" s="113" t="s">
+      <c r="D11" s="113" t="s">
         <v>221</v>
-      </c>
-      <c r="D11" s="113" t="s">
-        <v>222</v>
       </c>
       <c r="E11" s="113"/>
       <c r="F11" s="113" t="s">
         <v>94</v>
       </c>
       <c r="G11" s="113" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="26" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -8118,7 +8077,7 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="115" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B1" s="38" t="s">
         <v>1</v>
@@ -8149,7 +8108,7 @@
     </row>
     <row r="2" s="3" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="40" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B2" s="38" t="s">
         <v>1</v>
@@ -8388,23 +8347,23 @@
     </row>
     <row r="9" s="17" customFormat="true" ht="15.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="B9" s="10" t="s">
         <v>226</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>227</v>
       </c>
       <c r="C9" s="10"/>
       <c r="D9" s="10" t="s">
+        <v>227</v>
+      </c>
+      <c r="E9" s="10" t="s">
         <v>228</v>
       </c>
-      <c r="E9" s="10" t="s">
+      <c r="F9" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="F9" s="10" t="s">
+      <c r="G9" s="10" t="s">
         <v>230</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>231</v>
       </c>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
@@ -8462,7 +8421,7 @@
     </row>
     <row r="11" s="21" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="56" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B11" s="56" t="s">
         <v>29</v>
@@ -8474,13 +8433,13 @@
         <v>58</v>
       </c>
       <c r="E11" s="56" t="s">
+        <v>228</v>
+      </c>
+      <c r="F11" s="56" t="s">
         <v>229</v>
       </c>
-      <c r="F11" s="56" t="s">
+      <c r="G11" s="56" t="s">
         <v>230</v>
-      </c>
-      <c r="G11" s="56" t="s">
-        <v>231</v>
       </c>
       <c r="H11" s="47"/>
       <c r="I11" s="47"/>
@@ -8506,16 +8465,16 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="38" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B12" s="38" t="s">
         <v>40</v>
       </c>
       <c r="C12" s="38" t="s">
+        <v>233</v>
+      </c>
+      <c r="D12" s="38" t="s">
         <v>234</v>
-      </c>
-      <c r="D12" s="38" t="s">
-        <v>235</v>
       </c>
       <c r="E12" s="38" t="n">
         <v>3</v>
@@ -8524,23 +8483,23 @@
         <v>3</v>
       </c>
       <c r="G12" s="38" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H12" s="47"/>
       <c r="I12" s="47"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="38" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B13" s="38" t="s">
         <v>40</v>
       </c>
       <c r="C13" s="38" t="s">
+        <v>233</v>
+      </c>
+      <c r="D13" s="38" t="s">
         <v>234</v>
-      </c>
-      <c r="D13" s="38" t="s">
-        <v>235</v>
       </c>
       <c r="E13" s="38" t="n">
         <v>3</v>
@@ -8549,7 +8508,7 @@
         <v>3</v>
       </c>
       <c r="G13" s="38" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="H13" s="47"/>
       <c r="I13" s="47"/>
@@ -8640,7 +8599,7 @@
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="116" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B1" s="117" t="s">
         <v>1</v>
@@ -8673,7 +8632,7 @@
     </row>
     <row r="2" s="3" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="118" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B2" s="117" t="s">
         <v>1</v>
@@ -8857,11 +8816,11 @@
       <c r="D7" s="43"/>
       <c r="E7" s="43"/>
       <c r="F7" s="43" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G7" s="43"/>
       <c r="H7" s="43" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="I7" s="43"/>
       <c r="J7" s="10"/>
@@ -8918,24 +8877,24 @@
     </row>
     <row r="9" s="17" customFormat="true" ht="15.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="119" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B9" s="119" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C9" s="119"/>
       <c r="D9" s="119"/>
       <c r="E9" s="119" t="s">
+        <v>240</v>
+      </c>
+      <c r="F9" s="119" t="s">
         <v>241</v>
       </c>
-      <c r="F9" s="119" t="s">
+      <c r="G9" s="119" t="s">
         <v>242</v>
       </c>
-      <c r="G9" s="119" t="s">
+      <c r="H9" s="119" t="s">
         <v>243</v>
-      </c>
-      <c r="H9" s="119" t="s">
-        <v>244</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
@@ -8992,10 +8951,10 @@
     </row>
     <row r="11" s="21" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="120" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B11" s="120" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C11" s="120" t="s">
         <v>30</v>
@@ -9004,16 +8963,16 @@
         <v>31</v>
       </c>
       <c r="E11" s="120" t="s">
+        <v>245</v>
+      </c>
+      <c r="F11" s="120" t="s">
         <v>246</v>
       </c>
-      <c r="F11" s="120" t="s">
+      <c r="G11" s="120" t="s">
         <v>247</v>
       </c>
-      <c r="G11" s="120" t="s">
+      <c r="H11" s="120" t="s">
         <v>248</v>
-      </c>
-      <c r="H11" s="120" t="s">
-        <v>249</v>
       </c>
       <c r="I11" s="118"/>
       <c r="J11" s="118"/>
@@ -9038,14 +8997,14 @@
     </row>
     <row r="12" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="25" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B12" s="121"/>
       <c r="C12" s="122" t="s">
+        <v>250</v>
+      </c>
+      <c r="D12" s="122" t="s">
         <v>251</v>
-      </c>
-      <c r="D12" s="122" t="s">
-        <v>252</v>
       </c>
       <c r="E12" s="123"/>
       <c r="F12" s="25" t="n">
@@ -9059,14 +9018,14 @@
     </row>
     <row r="13" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="25" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B13" s="121"/>
       <c r="C13" s="122" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D13" s="122" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E13" s="123"/>
       <c r="F13" s="25" t="n">
@@ -9080,14 +9039,14 @@
     </row>
     <row r="14" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="25" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B14" s="121"/>
       <c r="C14" s="122" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D14" s="122" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="E14" s="123"/>
       <c r="F14" s="25" t="n">

</xml_diff>

<commit_message>
refinements to xlsx file in MOVPE CNR
</commit_message>
<xml_diff>
--- a/movpe_CNR/Parma_datafile_nomad.xlsx
+++ b/movpe_CNR/Parma_datafile_nomad.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,8 +13,8 @@
     <sheet name="Substrate" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Mist" sheetId="4" state="visible" r:id="rId5"/>
     <sheet name="Pregrowth" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="Growthrun" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="Sample-cut" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="GrowthRun" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="SampleCut" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="HRXRD" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="AFMReflectanceSEM" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="Contacts" sheetId="10" state="visible" r:id="rId11"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="257">
   <si>
     <t xml:space="preserve"># start Header</t>
   </si>
@@ -600,7 +600,7 @@
     <t xml:space="preserve">Rotation</t>
   </si>
   <si>
-    <t xml:space="preserve">Bubbler material</t>
+    <t xml:space="preserve">Bubbler Material</t>
   </si>
   <si>
     <t xml:space="preserve">Bubbler Flow</t>
@@ -633,34 +633,25 @@
     <t xml:space="preserve">Outer Valve</t>
   </si>
   <si>
-    <t xml:space="preserve">Bubbler flow</t>
-  </si>
-  <si>
     <t xml:space="preserve">Gas Cylinder Material</t>
   </si>
   <si>
-    <t xml:space="preserve">dilution in cylinder</t>
+    <t xml:space="preserve">Dilution in Cylinder</t>
   </si>
   <si>
     <t xml:space="preserve">Flow  from MFC</t>
   </si>
   <si>
-    <t xml:space="preserve">Effective  flow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">partial pressure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">carrier flow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cylinder pressure</t>
+    <t xml:space="preserve">Effective  Flow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cylinder Pressure</t>
   </si>
   <si>
     <t xml:space="preserve">MIST Source 1</t>
   </si>
   <si>
-    <t xml:space="preserve">MIST flow MFC</t>
+    <t xml:space="preserve">MIST Flow MFC</t>
   </si>
   <si>
     <t xml:space="preserve">Purge Flow</t>
@@ -1979,7 +1970,7 @@
   </sheetPr>
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J23" activeCellId="0" sqref="J23"/>
     </sheetView>
   </sheetViews>
@@ -2277,7 +2268,7 @@
         <v>42</v>
       </c>
       <c r="J10" s="32" t="n">
-        <f aca="false">Growthrun!Y10/Growthrun!N10</f>
+        <f aca="false">GrowthRun!Y10/GrowthRun!N10</f>
         <v>217.407738991397</v>
       </c>
       <c r="K10" s="12" t="n">
@@ -2421,11 +2412,11 @@
   </sheetPr>
   <dimension ref="A1:AB108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.15"/>
@@ -2539,7 +2530,7 @@
       <c r="D5" s="63"/>
       <c r="E5" s="63"/>
       <c r="F5" s="63" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G5" s="62"/>
       <c r="H5" s="63"/>
@@ -2575,15 +2566,15 @@
         <v>117</v>
       </c>
       <c r="B7" s="62" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C7" s="62"/>
       <c r="D7" s="62"/>
       <c r="E7" s="63" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F7" s="63" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="G7" s="63"/>
       <c r="H7" s="183"/>
@@ -2629,10 +2620,10 @@
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="184" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="C9" s="21" t="s">
         <v>26</v>
@@ -2641,10 +2632,10 @@
         <v>27</v>
       </c>
       <c r="E9" s="184" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F9" s="184" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="G9" s="184"/>
       <c r="H9" s="182"/>
@@ -2655,10 +2646,10 @@
       <c r="A10" s="185"/>
       <c r="B10" s="186"/>
       <c r="C10" s="187" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D10" s="187" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="E10" s="182"/>
       <c r="F10" s="182"/>
@@ -3024,13 +3015,13 @@
   </sheetPr>
   <dimension ref="A1:P97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.09375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.51"/>
@@ -3792,7 +3783,7 @@
   </sheetPr>
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -4312,11 +4303,11 @@
   </sheetPr>
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="61" width="22.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.66"/>
@@ -4739,11 +4730,11 @@
   </sheetPr>
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.09375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.33"/>
@@ -5236,8 +5227,8 @@
   </sheetPr>
   <dimension ref="A1:BF47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AW11" activeCellId="0" sqref="AW11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="V1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AE29" activeCellId="0" sqref="AE29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6060,7 +6051,7 @@
         <v>189</v>
       </c>
       <c r="T9" s="134" t="s">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="U9" s="134" t="s">
         <v>191</v>
@@ -6090,46 +6081,46 @@
         <v>199</v>
       </c>
       <c r="AD9" s="135" t="s">
+        <v>200</v>
+      </c>
+      <c r="AE9" s="135" t="s">
         <v>201</v>
       </c>
-      <c r="AE9" s="135" t="s">
+      <c r="AF9" s="135" t="s">
         <v>202</v>
       </c>
-      <c r="AF9" s="135" t="s">
+      <c r="AG9" s="135" t="s">
         <v>203</v>
       </c>
-      <c r="AG9" s="135" t="s">
+      <c r="AH9" s="135" t="s">
+        <v>195</v>
+      </c>
+      <c r="AI9" s="135" t="s">
+        <v>196</v>
+      </c>
+      <c r="AJ9" s="135" t="s">
         <v>204</v>
-      </c>
-      <c r="AH9" s="135" t="s">
-        <v>205</v>
-      </c>
-      <c r="AI9" s="135" t="s">
-        <v>206</v>
-      </c>
-      <c r="AJ9" s="135" t="s">
-        <v>207</v>
       </c>
       <c r="AK9" s="135" t="s">
         <v>197</v>
       </c>
       <c r="AL9" s="136" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="AM9" s="136" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="AN9" s="136" t="s">
         <v>197</v>
       </c>
       <c r="AO9" s="137" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="AP9" s="137" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="AQ9" s="137" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="AR9" s="25" t="s">
         <v>35</v>
@@ -6151,7 +6142,7 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="138" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="B10" s="139" t="n">
         <v>1</v>
@@ -6173,7 +6164,7 @@
         <v>Helium</v>
       </c>
       <c r="H10" s="140" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="I10" s="139" t="n">
         <v>7</v>
@@ -6243,7 +6234,7 @@
         <v>0</v>
       </c>
       <c r="AD10" s="143" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="AE10" s="139" t="n">
         <v>0.0005</v>
@@ -6727,7 +6718,7 @@
   </sheetPr>
   <dimension ref="A1:AC19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -6906,28 +6897,28 @@
     </row>
     <row r="7" s="157" customFormat="true" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="152" t="s">
+        <v>213</v>
+      </c>
+      <c r="B7" s="152" t="s">
+        <v>214</v>
+      </c>
+      <c r="C7" s="152" t="s">
+        <v>215</v>
+      </c>
+      <c r="D7" s="152" t="s">
         <v>216</v>
       </c>
-      <c r="B7" s="152" t="s">
+      <c r="E7" s="152" t="s">
         <v>217</v>
       </c>
-      <c r="C7" s="152" t="s">
+      <c r="F7" s="152" t="s">
         <v>218</v>
       </c>
-      <c r="D7" s="152" t="s">
+      <c r="G7" s="152" t="s">
         <v>219</v>
       </c>
-      <c r="E7" s="152" t="s">
+      <c r="H7" s="152" t="s">
         <v>220</v>
-      </c>
-      <c r="F7" s="152" t="s">
-        <v>221</v>
-      </c>
-      <c r="G7" s="152" t="s">
-        <v>222</v>
-      </c>
-      <c r="H7" s="152" t="s">
-        <v>223</v>
       </c>
       <c r="I7" s="152"/>
       <c r="J7" s="152"/>
@@ -6973,26 +6964,26 @@
     </row>
     <row r="9" customFormat="false" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="158" t="s">
+        <v>221</v>
+      </c>
+      <c r="B9" s="158" t="s">
+        <v>222</v>
+      </c>
+      <c r="C9" s="159" t="s">
+        <v>223</v>
+      </c>
+      <c r="D9" s="158" t="s">
         <v>224</v>
       </c>
-      <c r="B9" s="158" t="s">
+      <c r="E9" s="158" t="s">
         <v>225</v>
-      </c>
-      <c r="C9" s="159" t="s">
-        <v>226</v>
-      </c>
-      <c r="D9" s="158" t="s">
-        <v>227</v>
-      </c>
-      <c r="E9" s="158" t="s">
-        <v>228</v>
       </c>
       <c r="F9" s="158"/>
       <c r="G9" s="158" t="s">
         <v>103</v>
       </c>
       <c r="H9" s="158" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7117,11 +7108,11 @@
   </sheetPr>
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.31"/>
@@ -7342,26 +7333,26 @@
     </row>
     <row r="7" s="19" customFormat="true" ht="35.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C7" s="9"/>
       <c r="D7" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="G7" s="9" t="s">
         <v>232</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="H7" s="9" t="s">
         <v>233</v>
-      </c>
-      <c r="F7" s="9" t="s">
-        <v>234</v>
-      </c>
-      <c r="G7" s="9" t="s">
-        <v>235</v>
-      </c>
-      <c r="H7" s="9" t="s">
-        <v>236</v>
       </c>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
@@ -7418,7 +7409,7 @@
     </row>
     <row r="9" s="24" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="163" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B9" s="163" t="s">
         <v>25</v>
@@ -7430,13 +7421,13 @@
         <v>57</v>
       </c>
       <c r="E9" s="163" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="F9" s="163" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="G9" s="163" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="H9" s="67" t="s">
         <v>35</v>
@@ -7942,11 +7933,11 @@
   </sheetPr>
   <dimension ref="A1:AB123"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.16"/>
@@ -8075,11 +8066,11 @@
       <c r="D5" s="166"/>
       <c r="E5" s="166"/>
       <c r="F5" s="166" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="G5" s="166"/>
       <c r="H5" s="166" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="I5" s="166"/>
       <c r="J5" s="12"/>
@@ -8136,24 +8127,24 @@
     </row>
     <row r="7" s="162" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="34" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="B7" s="34" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34" t="s">
+        <v>237</v>
+      </c>
+      <c r="F7" s="34" t="s">
+        <v>238</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>239</v>
+      </c>
+      <c r="H7" s="34" t="s">
         <v>240</v>
-      </c>
-      <c r="F7" s="34" t="s">
-        <v>241</v>
-      </c>
-      <c r="G7" s="34" t="s">
-        <v>242</v>
-      </c>
-      <c r="H7" s="34" t="s">
-        <v>243</v>
       </c>
       <c r="I7" s="31" t="s">
         <v>131</v>
@@ -8212,10 +8203,10 @@
     </row>
     <row r="9" s="11" customFormat="true" ht="16.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="27" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="B9" s="27" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>26</v>
@@ -8224,16 +8215,16 @@
         <v>27</v>
       </c>
       <c r="E9" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="F9" s="27" t="s">
+        <v>243</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>244</v>
+      </c>
+      <c r="H9" s="27" t="s">
         <v>245</v>
-      </c>
-      <c r="F9" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="G9" s="27" t="s">
-        <v>247</v>
-      </c>
-      <c r="H9" s="27" t="s">
-        <v>248</v>
       </c>
       <c r="I9" s="175"/>
       <c r="J9" s="175"/>
@@ -8247,13 +8238,13 @@
         <v>44986</v>
       </c>
       <c r="C10" s="178" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D10" s="179" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E10" s="180" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="F10" s="34"/>
       <c r="G10" s="181"/>

</xml_diff>

<commit_message>
started updating MOVPE CNR schema after Tutorial 8
</commit_message>
<xml_diff>
--- a/movpe_CNR/Parma_datafile_nomad.xlsx
+++ b/movpe_CNR/Parma_datafile_nomad.xlsx
@@ -130,7 +130,7 @@
     <t xml:space="preserve">Carrier Gas</t>
   </si>
   <si>
-    <t xml:space="preserve">VI III ratio</t>
+    <t xml:space="preserve">VI III Ratio</t>
   </si>
   <si>
     <t xml:space="preserve">Growth Time</t>
@@ -1970,8 +1970,8 @@
   </sheetPr>
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K9" activeCellId="0" sqref="K9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="27.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2412,11 +2412,11 @@
   </sheetPr>
   <dimension ref="A1:AB108"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.15"/>
@@ -3015,13 +3015,13 @@
   </sheetPr>
   <dimension ref="A1:P97"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="I25" activeCellId="0" sqref="I25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.15625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.51"/>
@@ -3783,7 +3783,7 @@
   </sheetPr>
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E18" activeCellId="0" sqref="E18"/>
     </sheetView>
   </sheetViews>
@@ -4303,11 +4303,11 @@
   </sheetPr>
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="61" width="22.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.66"/>
@@ -4730,11 +4730,11 @@
   </sheetPr>
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H40" activeCellId="0" sqref="H40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.15625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.33"/>
@@ -5227,7 +5227,7 @@
   </sheetPr>
   <dimension ref="A1:BF47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G12" activeCellId="0" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -6718,7 +6718,7 @@
   </sheetPr>
   <dimension ref="A1:AC19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -7108,11 +7108,11 @@
   </sheetPr>
   <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.31"/>
@@ -7933,11 +7933,11 @@
   </sheetPr>
   <dimension ref="A1:AB123"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J11" activeCellId="0" sqref="J11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.00390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.16"/>

</xml_diff>

<commit_message>
typos in MOVPE schema
</commit_message>
<xml_diff>
--- a/movpe_CNR/Parma_datafile_nomad.xlsx
+++ b/movpe_CNR/Parma_datafile_nomad.xlsx
@@ -1151,7 +1151,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="202">
+  <cellXfs count="201">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1954,10 +1954,6 @@
     </xf>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2039,7 +2035,7 @@
   </sheetPr>
   <dimension ref="A1:Q46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -2479,10 +2475,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB108"/>
+  <dimension ref="A1:AB1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F22" activeCellId="0" sqref="F22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.01953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2697,345 +2693,345 @@
       <c r="I10" s="198"/>
       <c r="J10" s="198"/>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="198"/>
-      <c r="B11" s="201"/>
-      <c r="C11" s="198"/>
-      <c r="D11" s="198"/>
-      <c r="E11" s="198"/>
-      <c r="F11" s="198"/>
-      <c r="G11" s="198"/>
-      <c r="H11" s="198"/>
-      <c r="I11" s="198"/>
-      <c r="J11" s="198"/>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="198"/>
-      <c r="B12" s="201"/>
-      <c r="C12" s="198"/>
-      <c r="D12" s="198"/>
-      <c r="E12" s="198"/>
-      <c r="F12" s="198"/>
-      <c r="G12" s="198"/>
-      <c r="H12" s="198"/>
-      <c r="I12" s="198"/>
-      <c r="J12" s="198"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="198"/>
-      <c r="B13" s="201"/>
-      <c r="C13" s="198"/>
-      <c r="D13" s="198"/>
-      <c r="E13" s="198"/>
-      <c r="F13" s="198"/>
-      <c r="G13" s="198"/>
-      <c r="H13" s="198"/>
-      <c r="I13" s="198"/>
-      <c r="J13" s="198"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="198"/>
-      <c r="B14" s="201"/>
-      <c r="C14" s="198"/>
-      <c r="D14" s="198"/>
-      <c r="E14" s="198"/>
-      <c r="F14" s="198"/>
-      <c r="G14" s="198"/>
-      <c r="H14" s="198"/>
-      <c r="I14" s="198"/>
-      <c r="J14" s="198"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="198"/>
-      <c r="B15" s="201"/>
-      <c r="C15" s="198"/>
-      <c r="D15" s="198"/>
-      <c r="E15" s="198"/>
-      <c r="F15" s="198"/>
-      <c r="G15" s="198"/>
-      <c r="H15" s="198"/>
-      <c r="I15" s="198"/>
-      <c r="J15" s="198"/>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="57"/>
-    </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="57"/>
-    </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="57"/>
-    </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="57"/>
-    </row>
-    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="57"/>
-    </row>
-    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="57"/>
-    </row>
-    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="57"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="57"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="57"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="57"/>
-    </row>
-    <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="57"/>
-    </row>
-    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="57"/>
-    </row>
-    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="57"/>
-    </row>
-    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="57"/>
-    </row>
-    <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="57"/>
-    </row>
-    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="57"/>
-    </row>
-    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="57"/>
-    </row>
-    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="57"/>
-    </row>
-    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="57"/>
-    </row>
-    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="57"/>
-    </row>
-    <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="57"/>
-    </row>
-    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="57"/>
-    </row>
-    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="57"/>
-    </row>
-    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="57"/>
-    </row>
-    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="57"/>
-    </row>
-    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="57"/>
-    </row>
-    <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="57"/>
-    </row>
-    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="57"/>
-    </row>
-    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="57"/>
-    </row>
-    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="57"/>
-    </row>
-    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="57"/>
-    </row>
-    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="57"/>
-    </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="57"/>
-    </row>
-    <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="57"/>
-    </row>
-    <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="57"/>
-    </row>
-    <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B51" s="57"/>
-    </row>
-    <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B52" s="57"/>
-    </row>
-    <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B53" s="57"/>
-    </row>
-    <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B54" s="57"/>
-    </row>
-    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B55" s="57"/>
-    </row>
-    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B56" s="57"/>
-    </row>
-    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B57" s="57"/>
-    </row>
-    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B58" s="57"/>
-    </row>
-    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B59" s="57"/>
-    </row>
-    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B60" s="57"/>
-    </row>
-    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B61" s="57"/>
-    </row>
-    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B62" s="57"/>
-    </row>
-    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B63" s="57"/>
-    </row>
-    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="57"/>
-    </row>
-    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="57"/>
-    </row>
-    <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B66" s="57"/>
-    </row>
-    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="57"/>
-    </row>
-    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="57"/>
-    </row>
-    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="57"/>
-    </row>
-    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="57"/>
-    </row>
-    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="57"/>
-    </row>
-    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="57"/>
-    </row>
-    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="57"/>
-    </row>
-    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="57"/>
-    </row>
-    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="57"/>
-    </row>
-    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="57"/>
-    </row>
-    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="57"/>
-    </row>
-    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="57"/>
-    </row>
-    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="57"/>
-    </row>
-    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="57"/>
-    </row>
-    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="57"/>
-    </row>
-    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="57"/>
-    </row>
-    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="57"/>
-    </row>
-    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="57"/>
-    </row>
-    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="57"/>
-    </row>
-    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="57"/>
-    </row>
-    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="57"/>
-    </row>
-    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="57"/>
-    </row>
-    <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="57"/>
-    </row>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="57"/>
-    </row>
-    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="57"/>
-    </row>
-    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="57"/>
-    </row>
-    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="57"/>
-    </row>
-    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="57"/>
-    </row>
-    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="57"/>
-    </row>
-    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="57"/>
-    </row>
-    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="57"/>
-    </row>
-    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="57"/>
-    </row>
-    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="57"/>
-    </row>
-    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="57"/>
-    </row>
-    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="57"/>
-    </row>
-    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="57"/>
-    </row>
-    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="57"/>
-    </row>
-    <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="57"/>
-    </row>
-    <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="57"/>
-    </row>
-    <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B106" s="57"/>
-    </row>
-    <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="57"/>
-    </row>
-    <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="57"/>
-    </row>
+    <row r="1048238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048240" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048241" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048242" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048258" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048273" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048279" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048283" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048297" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048298" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048299" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048300" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048301" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048302" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048303" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048304" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048305" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048306" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048307" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048308" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048309" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048310" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048311" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048312" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048313" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048314" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048315" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048316" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048317" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048318" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048319" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048320" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048321" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048322" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048323" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048324" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048325" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048326" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048327" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048328" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048329" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048330" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048331" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048332" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048333" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048334" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048335" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048338" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048339" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048340" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048341" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048342" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048343" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048344" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048345" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048346" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048347" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048348" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048349" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048350" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048351" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048352" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048353" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048354" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048355" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048356" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048357" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048358" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048359" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048360" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048361" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048362" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048363" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048364" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048365" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048366" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048367" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048368" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048369" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048370" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048371" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048372" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048373" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048374" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048375" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048376" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048377" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048378" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048379" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048380" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048381" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048382" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048383" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048384" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048385" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048386" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048387" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048388" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048389" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048390" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048391" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048392" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048393" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048394" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048395" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048396" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048397" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048398" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048399" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048400" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048401" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048402" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048403" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048404" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048405" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048406" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048407" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048408" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048409" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048410" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048411" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048412" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048413" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048414" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048415" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048416" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048417" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048418" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048419" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048420" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048421" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048422" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048423" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048424" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048425" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048426" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048427" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048428" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048429" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048430" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048431" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048432" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048433" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048434" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048435" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048436" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048437" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048438" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048439" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048440" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048441" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048442" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048443" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048444" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048445" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048446" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048447" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048448" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048449" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048450" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048451" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048452" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048453" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048454" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048455" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048456" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048457" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048458" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048459" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048460" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048461" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048462" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048463" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048464" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048465" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048466" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048467" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048468" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048469" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048470" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048471" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048472" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048473" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048474" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048475" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048476" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048477" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048478" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048479" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048480" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048481" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048482" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048483" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048484" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048485" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048486" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048487" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048488" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048489" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048490" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048491" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048492" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048493" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048494" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048495" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048496" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048497" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048498" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048499" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048500" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048501" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048502" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048503" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048504" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048505" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048506" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048507" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048508" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048509" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048510" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048511" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048512" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048513" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048514" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048515" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048516" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048517" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048518" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048519" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048520" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048521" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048522" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048523" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048524" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048525" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048526" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048527" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048528" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048529" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048530" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048531" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048532" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048533" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048534" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048535" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048536" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048537" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048538" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048539" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048540" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048541" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048542" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048543" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048544" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048545" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048546" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048547" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048548" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048549" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048550" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048551" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048552" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511811023622047" footer="0.511811023622047"/>
@@ -3054,7 +3050,7 @@
   </sheetPr>
   <dimension ref="A1:L85"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
@@ -3655,7 +3651,7 @@
   </sheetPr>
   <dimension ref="A1:S46"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -4175,11 +4171,11 @@
   </sheetPr>
   <dimension ref="A1:Q43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.70703125" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="76" width="22.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="77" width="14.66"/>
@@ -4626,11 +4622,11 @@
   </sheetPr>
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="77" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="77" width="20.33"/>
@@ -5123,7 +5119,7 @@
   </sheetPr>
   <dimension ref="A1:BF47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C33" activeCellId="0" sqref="C33"/>
     </sheetView>
   </sheetViews>
@@ -6614,7 +6610,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -6997,11 +6993,11 @@
   </sheetPr>
   <dimension ref="A1:AC156"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="77" width="19.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="77" width="24.31"/>
@@ -7843,11 +7839,11 @@
   </sheetPr>
   <dimension ref="A1:AB123"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.01953125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="77" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="77" width="25.16"/>

</xml_diff>

<commit_message>
updated movpe CNR excel file
</commit_message>
<xml_diff>
--- a/movpe_CNR/Parma_datafile_nomad.xlsx
+++ b/movpe_CNR/Parma_datafile_nomad.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId2"/>
@@ -18,7 +18,11 @@
     <sheet name="HRXRD" sheetId="8" state="visible" r:id="rId9"/>
     <sheet name="AFMReflectanceSEM" sheetId="9" state="visible" r:id="rId10"/>
     <sheet name="Contacts" sheetId="10" state="visible" r:id="rId11"/>
+    <sheet name="ElectroOptical" sheetId="11" state="visible" r:id="rId12"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId13"/>
+  </externalReferences>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
@@ -29,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="265">
   <si>
     <t xml:space="preserve"># start Header</t>
   </si>
@@ -720,7 +724,7 @@
     <t xml:space="preserve">Peak position</t>
   </si>
   <si>
-    <t xml:space="preserve">Peak FWHM</t>
+    <t xml:space="preserve">Peak FWHM Rocking Curve</t>
   </si>
   <si>
     <t xml:space="preserve">Peak assignment</t>
@@ -744,6 +748,9 @@
     <t xml:space="preserve">nm</t>
   </si>
   <si>
+    <t xml:space="preserve">nm/min</t>
+  </si>
+  <si>
     <t xml:space="preserve"># ID of the sample</t>
   </si>
   <si>
@@ -759,6 +766,9 @@
     <t xml:space="preserve">Thickness from Reflectance</t>
   </si>
   <si>
+    <t xml:space="preserve">Growth rate calculated</t>
+  </si>
+  <si>
     <t xml:space="preserve">Surface State</t>
   </si>
   <si>
@@ -771,16 +781,25 @@
     <t xml:space="preserve">Thickness</t>
   </si>
   <si>
-    <t xml:space="preserve">optical microscopy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Particulates observed on the surface</t>
+    <t xml:space="preserve">Growth Rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optical Reflectance</t>
   </si>
   <si>
     <t xml:space="preserve">rough</t>
   </si>
   <si>
-    <t xml:space="preserve">002</t>
+    <t xml:space="preserve">center</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mid-point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">side</t>
+  </si>
+  <si>
+    <t xml:space="preserve">border</t>
   </si>
   <si>
     <t xml:space="preserve">Date of contact deposition</t>
@@ -1016,7 +1035,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1069,6 +1088,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDBEEF4"/>
+        <bgColor rgb="FFCCFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -1151,7 +1176,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="201">
+  <cellXfs count="209">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1916,7 +1941,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="25" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1924,6 +1949,10 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="167" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="167" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1932,8 +1961,36 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="174" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="9" fillId="4" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -1986,7 +2043,7 @@
       <rgbColor rgb="FF729FCF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFDBEEF4"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
@@ -2028,6 +2085,50 @@
 </styleSheet>
 </file>
 
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Overview"/>
+      <sheetName val="Precursors"/>
+      <sheetName val="Substrate"/>
+      <sheetName val="Mist"/>
+      <sheetName val="Pregrowth"/>
+      <sheetName val="GrowthRun"/>
+      <sheetName val="SampleCut"/>
+      <sheetName val="HRXRD"/>
+      <sheetName val="AFMReflectanceSEM"/>
+      <sheetName val="Contacts"/>
+      <sheetName val="ElectroOptical"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5">
+        <row r="10">
+          <cell r="N10">
+            <v>0.000339054768966123</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="Y10">
+            <v>0.0737131307151752</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -2607,18 +2708,18 @@
         <v>109</v>
       </c>
       <c r="B7" s="78" t="s">
-        <v>250</v>
+        <v>255</v>
       </c>
       <c r="C7" s="78"/>
       <c r="D7" s="78"/>
       <c r="E7" s="79" t="s">
-        <v>251</v>
+        <v>256</v>
       </c>
       <c r="F7" s="79" t="s">
-        <v>252</v>
+        <v>257</v>
       </c>
       <c r="G7" s="79"/>
-      <c r="H7" s="196"/>
+      <c r="H7" s="204"/>
       <c r="I7" s="9"/>
       <c r="J7" s="9"/>
       <c r="K7" s="9"/>
@@ -2646,11 +2747,11 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="197" t="s">
-        <v>253</v>
+      <c r="A9" s="205" t="s">
+        <v>258</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>254</v>
+        <v>259</v>
       </c>
       <c r="C9" s="22" t="s">
         <v>26</v>
@@ -2658,40 +2759,40 @@
       <c r="D9" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="197" t="s">
-        <v>251</v>
-      </c>
-      <c r="F9" s="197" t="s">
-        <v>255</v>
-      </c>
-      <c r="G9" s="197"/>
-      <c r="H9" s="198"/>
-      <c r="I9" s="198"/>
-      <c r="J9" s="198"/>
+      <c r="E9" s="205" t="s">
+        <v>256</v>
+      </c>
+      <c r="F9" s="205" t="s">
+        <v>260</v>
+      </c>
+      <c r="G9" s="205"/>
+      <c r="H9" s="206"/>
+      <c r="I9" s="206"/>
+      <c r="J9" s="206"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="176" t="s">
-        <v>256</v>
-      </c>
-      <c r="B10" s="199" t="n">
+        <v>261</v>
+      </c>
+      <c r="B10" s="207" t="n">
         <v>45008</v>
       </c>
-      <c r="C10" s="200" t="s">
-        <v>257</v>
-      </c>
-      <c r="D10" s="200" t="s">
-        <v>258</v>
-      </c>
-      <c r="E10" s="198" t="s">
-        <v>259</v>
-      </c>
-      <c r="F10" s="198" t="n">
+      <c r="C10" s="208" t="s">
+        <v>262</v>
+      </c>
+      <c r="D10" s="208" t="s">
+        <v>263</v>
+      </c>
+      <c r="E10" s="206" t="s">
+        <v>264</v>
+      </c>
+      <c r="F10" s="206" t="n">
         <v>23</v>
       </c>
-      <c r="G10" s="198"/>
-      <c r="H10" s="198"/>
-      <c r="I10" s="198"/>
-      <c r="J10" s="198"/>
+      <c r="G10" s="206"/>
+      <c r="H10" s="206"/>
+      <c r="I10" s="206"/>
+      <c r="J10" s="206"/>
     </row>
     <row r="1048238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048239" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3043,6 +3144,334 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:Q14"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="131" zoomScaleNormal="131" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H30" activeCellId="0" sqref="H30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="4"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+    </row>
+    <row r="2" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="7"/>
+      <c r="O2" s="6"/>
+      <c r="P2" s="6"/>
+    </row>
+    <row r="3" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="L3" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+    </row>
+    <row r="4" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="13"/>
+      <c r="O4" s="15"/>
+      <c r="P4" s="15"/>
+    </row>
+    <row r="5" s="17" customFormat="true" ht="23.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="K5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="L5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="O5" s="9"/>
+      <c r="P5" s="9"/>
+    </row>
+    <row r="6" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="18" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="18"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+      <c r="L6" s="7"/>
+      <c r="O6" s="18"/>
+      <c r="P6" s="18"/>
+    </row>
+    <row r="7" s="21" customFormat="true" ht="101.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C7" s="9"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="K7" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="L7" s="20"/>
+      <c r="O7" s="22"/>
+      <c r="P7" s="22"/>
+    </row>
+    <row r="8" s="24" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="23" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="23"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="23"/>
+      <c r="E8" s="23"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="23"/>
+      <c r="J8" s="23"/>
+      <c r="K8" s="23"/>
+      <c r="L8" s="4"/>
+      <c r="O8" s="23"/>
+      <c r="P8" s="23"/>
+    </row>
+    <row r="9" s="27" customFormat="true" ht="23.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="L9" s="25" t="s">
+        <v>35</v>
+      </c>
+      <c r="M9" s="26"/>
+      <c r="N9" s="26"/>
+      <c r="Q9" s="26"/>
+    </row>
+    <row r="10" s="26" customFormat="true" ht="34.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B10" s="29" t="n">
+        <v>44986</v>
+      </c>
+      <c r="C10" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="12" t="n">
+        <v>50</v>
+      </c>
+      <c r="I10" s="31" t="s">
+        <v>42</v>
+      </c>
+      <c r="J10" s="32" t="n">
+        <f aca="false">[1]GrowthRun!Y10/[1]GrowthRun!N10</f>
+        <v>217.407738991397</v>
+      </c>
+      <c r="K10" s="12" t="n">
+        <v>300</v>
+      </c>
+      <c r="L10" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="O10" s="34"/>
+      <c r="P10" s="34"/>
+    </row>
+    <row r="11" s="35" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L11" s="33"/>
+      <c r="O11" s="36"/>
+      <c r="P11" s="36"/>
+      <c r="Q11" s="36"/>
+    </row>
+    <row r="12" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L12" s="33"/>
+      <c r="O12" s="38"/>
+      <c r="P12" s="38"/>
+      <c r="Q12" s="38"/>
+    </row>
+    <row r="13" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L13" s="39"/>
+    </row>
+    <row r="14" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L14" s="39"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -4175,7 +4604,7 @@
       <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.72265625" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.7421875" defaultRowHeight="18.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="76" width="22.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="77" width="14.66"/>
@@ -4626,7 +5055,7 @@
       <selection pane="topLeft" activeCell="F27" activeCellId="0" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.2109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.2265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="77" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="77" width="20.33"/>
@@ -6610,7 +7039,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A6" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
@@ -6993,11 +7422,11 @@
   </sheetPr>
   <dimension ref="A1:AC156"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F28" activeCellId="0" sqref="F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="77" width="19.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="77" width="24.31"/>
@@ -7837,13 +8266,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AB123"/>
+  <dimension ref="A1:AC123"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I11" activeCellId="0" sqref="I11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.0390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.0546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="77" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="77" width="25.16"/>
@@ -7853,10 +8282,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="77" width="29.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="77" width="25.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="77" width="58.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="77" width="25.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="77" width="58.49"/>
   </cols>
   <sheetData>
-    <row r="1" s="5" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" s="5" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
@@ -7870,12 +8300,13 @@
       <c r="I1" s="23"/>
       <c r="J1" s="23"/>
       <c r="K1" s="23"/>
-      <c r="L1" s="3"/>
+      <c r="L1" s="23"/>
       <c r="M1" s="3"/>
-      <c r="P1" s="3"/>
+      <c r="N1" s="3"/>
       <c r="Q1" s="3"/>
-    </row>
-    <row r="2" s="19" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R1" s="3"/>
+    </row>
+    <row r="2" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
@@ -7891,11 +8322,11 @@
       <c r="K2" s="6"/>
       <c r="L2" s="6"/>
       <c r="M2" s="6"/>
-      <c r="N2" s="8"/>
+      <c r="N2" s="6"/>
       <c r="O2" s="8"/>
-      <c r="P2" s="6"/>
+      <c r="P2" s="8"/>
       <c r="Q2" s="6"/>
-      <c r="R2" s="8"/>
+      <c r="R2" s="6"/>
       <c r="S2" s="8"/>
       <c r="T2" s="8"/>
       <c r="U2" s="8"/>
@@ -7906,8 +8337,9 @@
       <c r="Z2" s="8"/>
       <c r="AA2" s="8"/>
       <c r="AB2" s="8"/>
-    </row>
-    <row r="3" s="11" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC2" s="8"/>
+    </row>
+    <row r="3" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="175" t="s">
         <v>109</v>
       </c>
@@ -7932,17 +8364,20 @@
       <c r="H3" s="176" t="s">
         <v>5</v>
       </c>
-      <c r="I3" s="184" t="s">
+      <c r="I3" s="176" t="s">
+        <v>5</v>
+      </c>
+      <c r="J3" s="184" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="12"/>
       <c r="K3" s="12"/>
       <c r="L3" s="12"/>
       <c r="M3" s="12"/>
-      <c r="P3" s="12"/>
+      <c r="N3" s="12"/>
       <c r="Q3" s="12"/>
-    </row>
-    <row r="4" s="8" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R3" s="12"/>
+    </row>
+    <row r="4" s="8" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
@@ -7958,10 +8393,11 @@
       <c r="K4" s="6"/>
       <c r="L4" s="6"/>
       <c r="M4" s="6"/>
-      <c r="P4" s="6"/>
+      <c r="N4" s="6"/>
       <c r="Q4" s="6"/>
-    </row>
-    <row r="5" s="177" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="R4" s="6"/>
+    </row>
+    <row r="5" s="177" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="175" t="s">
         <v>109</v>
       </c>
@@ -7987,17 +8423,19 @@
         <v>236</v>
       </c>
       <c r="I5" s="176" t="s">
+        <v>237</v>
+      </c>
+      <c r="J5" s="176" t="s">
         <v>9</v>
       </c>
-      <c r="J5" s="12"/>
       <c r="K5" s="12"/>
       <c r="L5" s="12"/>
       <c r="M5" s="12"/>
-      <c r="N5" s="11"/>
+      <c r="N5" s="12"/>
       <c r="O5" s="11"/>
-      <c r="P5" s="12"/>
+      <c r="P5" s="11"/>
       <c r="Q5" s="12"/>
-      <c r="R5" s="11"/>
+      <c r="R5" s="12"/>
       <c r="S5" s="11"/>
       <c r="T5" s="11"/>
       <c r="U5" s="11"/>
@@ -8008,6 +8446,7 @@
       <c r="Z5" s="11"/>
       <c r="AA5" s="11"/>
       <c r="AB5" s="11"/>
+      <c r="AC5" s="11"/>
     </row>
     <row r="6" s="188" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="185" t="s">
@@ -8023,13 +8462,13 @@
       <c r="I6" s="178"/>
       <c r="J6" s="178"/>
       <c r="K6" s="178"/>
-      <c r="L6" s="186"/>
+      <c r="L6" s="178"/>
       <c r="M6" s="186"/>
-      <c r="N6" s="187"/>
+      <c r="N6" s="186"/>
       <c r="O6" s="187"/>
-      <c r="P6" s="186"/>
+      <c r="P6" s="187"/>
       <c r="Q6" s="186"/>
-      <c r="R6" s="187"/>
+      <c r="R6" s="186"/>
       <c r="S6" s="187"/>
       <c r="T6" s="187"/>
       <c r="U6" s="187"/>
@@ -8040,10 +8479,11 @@
       <c r="Z6" s="187"/>
       <c r="AA6" s="187"/>
       <c r="AB6" s="187"/>
+      <c r="AC6" s="187"/>
     </row>
     <row r="7" s="179" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="34" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B7" s="34" t="s">
         <v>226</v>
@@ -8051,29 +8491,31 @@
       <c r="C7" s="34"/>
       <c r="D7" s="34"/>
       <c r="E7" s="34" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F7" s="34" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="G7" s="34" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="H7" s="34" t="s">
-        <v>241</v>
-      </c>
-      <c r="I7" s="31" t="s">
+        <v>242</v>
+      </c>
+      <c r="I7" s="34" t="s">
+        <v>243</v>
+      </c>
+      <c r="J7" s="31" t="s">
         <v>123</v>
       </c>
-      <c r="J7" s="12"/>
       <c r="K7" s="12"/>
       <c r="L7" s="12"/>
       <c r="M7" s="12"/>
-      <c r="N7" s="11"/>
+      <c r="N7" s="12"/>
       <c r="O7" s="11"/>
-      <c r="P7" s="12"/>
+      <c r="P7" s="11"/>
       <c r="Q7" s="12"/>
-      <c r="R7" s="11"/>
+      <c r="R7" s="12"/>
       <c r="S7" s="11"/>
       <c r="T7" s="11"/>
       <c r="U7" s="11"/>
@@ -8084,8 +8526,9 @@
       <c r="Z7" s="11"/>
       <c r="AA7" s="11"/>
       <c r="AB7" s="11"/>
-    </row>
-    <row r="8" s="180" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="AC7" s="11"/>
+    </row>
+    <row r="8" s="180" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="23" t="s">
         <v>23</v>
       </c>
@@ -8101,11 +8544,11 @@
       <c r="K8" s="23"/>
       <c r="L8" s="23"/>
       <c r="M8" s="23"/>
-      <c r="N8" s="24"/>
+      <c r="N8" s="23"/>
       <c r="O8" s="24"/>
-      <c r="P8" s="23"/>
+      <c r="P8" s="24"/>
       <c r="Q8" s="23"/>
-      <c r="R8" s="24"/>
+      <c r="R8" s="23"/>
       <c r="S8" s="24"/>
       <c r="T8" s="24"/>
       <c r="U8" s="24"/>
@@ -8116,6 +8559,7 @@
       <c r="Z8" s="24"/>
       <c r="AA8" s="24"/>
       <c r="AB8" s="24"/>
+      <c r="AC8" s="24"/>
     </row>
     <row r="9" s="11" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="27" t="s">
@@ -8131,22 +8575,25 @@
         <v>27</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="F9" s="27" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="H9" s="27" t="s">
-        <v>245</v>
-      </c>
-      <c r="I9" s="189" t="s">
+        <v>247</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="J9" s="189" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="190"/>
       <c r="K9" s="190"/>
+      <c r="L9" s="190"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="191" t="s">
@@ -8155,109 +8602,281 @@
       <c r="B10" s="192" t="n">
         <v>44986</v>
       </c>
-      <c r="C10" s="182" t="s">
+      <c r="C10" s="193" t="s">
         <v>232</v>
       </c>
-      <c r="D10" s="193" t="s">
-        <v>246</v>
-      </c>
-      <c r="E10" s="194" t="s">
-        <v>247</v>
-      </c>
-      <c r="F10" s="34" t="n">
-        <v>11</v>
-      </c>
-      <c r="G10" s="195" t="s">
-        <v>248</v>
-      </c>
-      <c r="H10" s="195" t="n">
+      <c r="D10" s="194" t="s">
+        <v>249</v>
+      </c>
+      <c r="E10" s="195"/>
+      <c r="F10" s="196"/>
+      <c r="G10" s="197" t="s">
+        <v>250</v>
+      </c>
+      <c r="H10" s="198" t="n">
         <v>40</v>
       </c>
-      <c r="I10" s="190" t="s">
-        <v>235</v>
-      </c>
-      <c r="J10" s="190"/>
+      <c r="I10" s="198" t="n">
+        <f aca="false">H10/GrowthRun!C10</f>
+        <v>1.33333333333333</v>
+      </c>
+      <c r="J10" s="199" t="s">
+        <v>251</v>
+      </c>
       <c r="K10" s="190"/>
+      <c r="L10" s="190"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="191" t="s">
-        <v>249</v>
+        <v>36</v>
       </c>
       <c r="B11" s="192" t="n">
         <v>44986</v>
       </c>
-      <c r="C11" s="182" t="s">
+      <c r="C11" s="193" t="s">
         <v>232</v>
       </c>
-      <c r="D11" s="193" t="s">
-        <v>246</v>
-      </c>
-      <c r="E11" s="194" t="s">
-        <v>247</v>
-      </c>
-      <c r="F11" s="34" t="n">
-        <v>13</v>
-      </c>
-      <c r="G11" s="195" t="s">
-        <v>248</v>
-      </c>
-      <c r="H11" s="195" t="n">
+      <c r="D11" s="194" t="s">
+        <v>249</v>
+      </c>
+      <c r="E11" s="195"/>
+      <c r="F11" s="196"/>
+      <c r="G11" s="197" t="s">
+        <v>250</v>
+      </c>
+      <c r="H11" s="198" t="n">
         <v>50</v>
       </c>
-      <c r="I11" s="77" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="183"/>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="183"/>
+      <c r="I11" s="198" t="n">
+        <f aca="false">H11/GrowthRun!C10</f>
+        <v>1.66666666666667</v>
+      </c>
+      <c r="J11" s="200" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="191" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="192" t="n">
+        <v>44986</v>
+      </c>
+      <c r="C12" s="193" t="s">
+        <v>232</v>
+      </c>
+      <c r="D12" s="194" t="s">
+        <v>249</v>
+      </c>
+      <c r="E12" s="195"/>
+      <c r="F12" s="196"/>
+      <c r="G12" s="197" t="s">
+        <v>250</v>
+      </c>
+      <c r="H12" s="198" t="n">
+        <v>120</v>
+      </c>
+      <c r="I12" s="198" t="n">
+        <f aca="false">H12/GrowthRun!C10</f>
+        <v>4</v>
+      </c>
+      <c r="J12" s="199" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="191" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="192" t="n">
+        <v>44986</v>
+      </c>
+      <c r="C13" s="193" t="s">
+        <v>232</v>
+      </c>
+      <c r="D13" s="194" t="s">
+        <v>249</v>
+      </c>
+      <c r="E13" s="195"/>
+      <c r="F13" s="196"/>
+      <c r="G13" s="197" t="s">
+        <v>250</v>
+      </c>
+      <c r="H13" s="198" t="n">
+        <v>110</v>
+      </c>
+      <c r="I13" s="198" t="n">
+        <f aca="false">H13/GrowthRun!C10</f>
+        <v>3.66666666666667</v>
+      </c>
+      <c r="J13" s="200" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="183"/>
+      <c r="B14" s="201"/>
+      <c r="C14" s="202"/>
+      <c r="D14" s="203"/>
+      <c r="E14" s="203"/>
+      <c r="F14" s="203"/>
+      <c r="G14" s="202"/>
+      <c r="H14" s="202"/>
+      <c r="I14" s="202"/>
+      <c r="J14" s="202"/>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="183"/>
+      <c r="B15" s="201"/>
+      <c r="C15" s="202"/>
+      <c r="D15" s="203"/>
+      <c r="E15" s="203"/>
+      <c r="F15" s="203"/>
+      <c r="G15" s="202"/>
+      <c r="H15" s="202"/>
+      <c r="I15" s="202"/>
+      <c r="J15" s="202"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="183"/>
+      <c r="B16" s="201"/>
+      <c r="C16" s="202"/>
+      <c r="D16" s="203"/>
+      <c r="E16" s="203"/>
+      <c r="F16" s="203"/>
+      <c r="G16" s="202"/>
+      <c r="H16" s="202"/>
+      <c r="I16" s="202"/>
+      <c r="J16" s="202"/>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="183"/>
+      <c r="B17" s="201"/>
+      <c r="C17" s="202"/>
+      <c r="D17" s="203"/>
+      <c r="E17" s="203"/>
+      <c r="F17" s="203"/>
+      <c r="G17" s="202"/>
+      <c r="H17" s="202"/>
+      <c r="I17" s="202"/>
+      <c r="J17" s="202"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="183"/>
+      <c r="B18" s="201"/>
+      <c r="C18" s="202"/>
+      <c r="D18" s="203"/>
+      <c r="E18" s="203"/>
+      <c r="F18" s="203"/>
+      <c r="G18" s="202"/>
+      <c r="H18" s="202"/>
+      <c r="I18" s="202"/>
+      <c r="J18" s="202"/>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="183"/>
+      <c r="B19" s="201"/>
+      <c r="C19" s="202"/>
+      <c r="D19" s="203"/>
+      <c r="E19" s="203"/>
+      <c r="F19" s="203"/>
+      <c r="G19" s="202"/>
+      <c r="H19" s="202"/>
+      <c r="I19" s="202"/>
+      <c r="J19" s="202"/>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="183"/>
+      <c r="B20" s="201"/>
+      <c r="C20" s="202"/>
+      <c r="D20" s="203"/>
+      <c r="E20" s="203"/>
+      <c r="F20" s="203"/>
+      <c r="G20" s="202"/>
+      <c r="H20" s="202"/>
+      <c r="I20" s="202"/>
+      <c r="J20" s="202"/>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="183"/>
+      <c r="B21" s="201"/>
+      <c r="C21" s="202"/>
+      <c r="D21" s="203"/>
+      <c r="E21" s="203"/>
+      <c r="F21" s="203"/>
+      <c r="G21" s="202"/>
+      <c r="H21" s="202"/>
+      <c r="I21" s="202"/>
+      <c r="J21" s="202"/>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="183"/>
+      <c r="B22" s="201"/>
+      <c r="C22" s="202"/>
+      <c r="D22" s="203"/>
+      <c r="E22" s="203"/>
+      <c r="F22" s="203"/>
+      <c r="G22" s="202"/>
+      <c r="H22" s="202"/>
+      <c r="I22" s="202"/>
+      <c r="J22" s="202"/>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="183"/>
+      <c r="B23" s="201"/>
+      <c r="C23" s="202"/>
+      <c r="D23" s="203"/>
+      <c r="E23" s="203"/>
+      <c r="F23" s="203"/>
+      <c r="G23" s="202"/>
+      <c r="H23" s="202"/>
+      <c r="I23" s="202"/>
+      <c r="J23" s="202"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="183"/>
+      <c r="B24" s="201"/>
+      <c r="C24" s="202"/>
+      <c r="D24" s="203"/>
+      <c r="E24" s="203"/>
+      <c r="F24" s="203"/>
+      <c r="G24" s="202"/>
+      <c r="H24" s="202"/>
+      <c r="I24" s="202"/>
+      <c r="J24" s="202"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="183"/>
+      <c r="B25" s="201"/>
+      <c r="C25" s="202"/>
+      <c r="D25" s="203"/>
+      <c r="E25" s="203"/>
+      <c r="F25" s="203"/>
+      <c r="G25" s="202"/>
+      <c r="H25" s="202"/>
+      <c r="I25" s="202"/>
+      <c r="J25" s="202"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="183"/>
+      <c r="B26" s="201"/>
+      <c r="C26" s="202"/>
+      <c r="D26" s="203"/>
+      <c r="E26" s="203"/>
+      <c r="F26" s="203"/>
+      <c r="G26" s="202"/>
+      <c r="H26" s="202"/>
+      <c r="I26" s="202"/>
+      <c r="J26" s="202"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="183"/>
+      <c r="B27" s="201"/>
+      <c r="C27" s="202"/>
+      <c r="D27" s="203"/>
+      <c r="E27" s="203"/>
+      <c r="F27" s="203"/>
+      <c r="G27" s="202"/>
+      <c r="H27" s="202"/>
+      <c r="I27" s="202"/>
+      <c r="J27" s="202"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="183"/>
+      <c r="B28" s="201"/>
+      <c r="C28" s="202"/>
+      <c r="D28" s="203"/>
+      <c r="E28" s="203"/>
+      <c r="F28" s="203"/>
+      <c r="G28" s="202"/>
+      <c r="H28" s="202"/>
+      <c r="I28" s="202"/>
+      <c r="J28" s="202"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="183"/>

</xml_diff>